<commit_message>
Changes to vasopressin substance definition (in spreadsheet and xml) and vasopressin pharmacodynamics scenarios.  Vasopressin now produces better fit to validation data.  Removed 1 extraneous vasopressin scenario.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="852" windowWidth="15096" windowHeight="7056" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -2249,9 +2249,6 @@
     <t>0.075 ug/mL</t>
   </si>
   <si>
-    <t>0.001 ug/mL</t>
-  </si>
-  <si>
     <t>10.5 mL/min kg</t>
   </si>
   <si>
@@ -2280,6 +2277,9 @@
   </si>
   <si>
     <t>0.008 ug/mL</t>
+  </si>
+  <si>
+    <t>0.0003 ug/mL</t>
   </si>
 </sst>
 </file>
@@ -3709,30 +3709,30 @@
       <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.5546875" style="141" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="145" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="145" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" style="141" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="145" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="145" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="145" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="145" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="145" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="145" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="145" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="145" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="145" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="145" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" style="145" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="145" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" style="145" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="145" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="10.6640625" style="145" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.109375" style="145" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" style="145" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="145"/>
+    <col min="5" max="5" width="14.28515625" style="145" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="145" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="145" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="145" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="145" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="145" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="145" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="145" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="145" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="145" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="145" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="10.7109375" style="145" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" style="145" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" style="145" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="145"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="140"/>
       <c r="B1" s="201" t="s">
         <v>578</v>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="U1" s="203"/>
     </row>
-    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="141" t="s">
         <v>0</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="140" t="s">
         <v>557</v>
       </c>
@@ -3853,7 +3853,7 @@
       <c r="T3" s="158"/>
       <c r="U3" s="159"/>
     </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="148" t="s">
         <v>405</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="140" t="s">
         <v>585</v>
       </c>
@@ -3943,7 +3943,7 @@
       <c r="T5" s="152"/>
       <c r="U5" s="153"/>
     </row>
-    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="149" t="s">
         <v>5</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="149" t="s">
         <v>6</v>
       </c>
@@ -4061,7 +4061,7 @@
       <c r="T7" s="156"/>
       <c r="U7" s="157"/>
     </row>
-    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="149" t="s">
         <v>7</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="149" t="s">
         <v>163</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="140" t="s">
         <v>586</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="T10" s="152"/>
       <c r="U10" s="153"/>
     </row>
-    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="149" t="s">
         <v>584</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="T11" s="156"/>
       <c r="U11" s="157"/>
     </row>
-    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="149" t="s">
         <v>550</v>
       </c>
@@ -4258,7 +4258,7 @@
       <c r="T12" s="156"/>
       <c r="U12" s="157"/>
     </row>
-    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="149" t="s">
         <v>61</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="149" t="s">
         <v>546</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="149" t="s">
         <v>547</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="149" t="s">
         <v>63</v>
       </c>
@@ -4527,7 +4527,7 @@
       <c r="T17" s="152"/>
       <c r="U17" s="153"/>
     </row>
-    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="149" t="s">
         <v>579</v>
       </c>
@@ -4552,7 +4552,7 @@
       <c r="T18" s="156"/>
       <c r="U18" s="157"/>
     </row>
-    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="149" t="s">
         <v>8</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="149" t="s">
         <v>555</v>
       </c>
@@ -4606,7 +4606,7 @@
       <c r="T20" s="156"/>
       <c r="U20" s="157"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="140" t="s">
         <v>587</v>
       </c>
@@ -4631,7 +4631,7 @@
       <c r="T21" s="152"/>
       <c r="U21" s="153"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="149" t="s">
         <v>552</v>
       </c>
@@ -4656,7 +4656,7 @@
       <c r="T22" s="156"/>
       <c r="U22" s="157"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="149" t="s">
         <v>553</v>
       </c>
@@ -4681,7 +4681,7 @@
       <c r="T23" s="156"/>
       <c r="U23" s="157"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="149" t="s">
         <v>551</v>
       </c>
@@ -4706,7 +4706,7 @@
       <c r="T24" s="156"/>
       <c r="U24" s="157"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="149" t="s">
         <v>556</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="T25" s="156"/>
       <c r="U25" s="157"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="149" t="s">
         <v>554</v>
       </c>
@@ -4773,167 +4773,167 @@
   <dimension ref="A1:FN78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CL3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="DR24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DH40" sqref="DH40"/>
+      <selection pane="bottomRight" activeCell="EH41" sqref="EH41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="71" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="105" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="17.6640625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="16.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.44140625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="17.6640625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="16.44140625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="16.6640625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="11.33203125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="16.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="11.5546875" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="16.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="11.5546875" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="15.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="16.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="11.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="16.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="11.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="33" width="22.5546875" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="13.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="37" width="26.109375" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="15.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="16.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="14.33203125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="13.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="45" width="21.5546875" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="14.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="49" width="21.5546875" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="11.5546875" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="15.88671875" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="16.6640625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="11.44140625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="12.33203125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="11.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="14.44140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="60" max="60" width="18.5546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="38.28515625" style="71" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="105" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="17.7109375" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="16.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="17.7109375" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="16.42578125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="16.7109375" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.28515625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="16.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="11.5703125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="16.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="11.5703125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="15.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="16.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="11.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="16.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="11.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="33" width="22.5703125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="13.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="37" width="26.140625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="15.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="16.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="41" width="14.28515625" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="13.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="45" width="21.5703125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="14.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="49" width="21.5703125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="11.5703125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="15.85546875" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="16.7109375" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="11.42578125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="12.28515625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="11.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="14.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="60" max="60" width="18.5703125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="61" max="61" width="24" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="14.44140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="64" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="65" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="11.33203125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="18.5546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="69" max="69" width="18.33203125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="70" max="70" width="13.88671875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="73" width="14.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="74" max="74" width="11.44140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="77" width="14.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="78" max="78" width="21.44140625" style="105" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="79" max="81" width="21.5546875" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="82" max="82" width="14.109375" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="83" max="85" width="18.109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="86" max="86" width="12.6640625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="87" max="87" width="20.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="88" max="88" width="16.109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="14.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="64" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="65" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="11.28515625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="18.5703125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="69" width="18.28515625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="70" max="70" width="13.85546875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="73" width="14.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="74" max="74" width="11.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="77" width="14.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="78" max="78" width="21.42578125" style="105" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="79" max="81" width="21.5703125" style="105" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="82" max="82" width="14.140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="85" width="18.140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="86" max="86" width="12.7109375" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="87" max="87" width="20.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="88" max="88" width="16.140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="89" max="89" width="24" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="90" max="90" width="14.44140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="91" max="91" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="92" max="92" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="93" max="93" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="12.5546875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="95" max="95" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="96" max="96" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="97" max="97" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="98" max="98" width="15.44140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="99" max="99" width="58.33203125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="100" max="100" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="102" max="102" width="15.44140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="103" max="103" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="104" max="104" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="105" max="105" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="106" max="106" width="13.44140625" style="58" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="107" max="107" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="108" max="108" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="109" max="109" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="110" max="110" width="13.77734375" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="111" max="111" width="14.44140625" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="112" max="112" width="27.109375" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="113" max="113" width="20.109375" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="114" max="114" width="13.44140625" style="106" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="116" max="116" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="117" max="117" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="118" max="118" width="14.33203125" style="106" customWidth="1" collapsed="1"/>
-    <col min="119" max="119" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="120" max="121" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="122" max="122" width="14.44140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="123" max="123" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="124" max="124" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="125" max="125" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="126" max="126" width="21.5546875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="127" max="127" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="128" max="128" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="129" max="129" width="11.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="130" max="130" width="23.6640625" style="106" customWidth="1" collapsed="1"/>
-    <col min="131" max="131" width="15.109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="132" max="132" width="15.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="133" max="133" width="30.5546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="134" max="134" width="15.5546875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="135" max="135" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="136" max="136" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="137" max="137" width="15.5546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="138" max="138" width="15.5546875" style="106" customWidth="1" collapsed="1"/>
-    <col min="139" max="141" width="15.5546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="142" max="142" width="17.5546875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="143" max="143" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="144" max="144" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="145" max="145" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="146" max="146" width="8.5546875" style="58" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="147" max="147" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="148" max="148" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="149" max="149" width="11.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="150" max="150" width="11.88671875" style="58" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="151" max="151" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="152" max="152" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="153" max="153" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="154" max="154" width="15.6640625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="155" max="155" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="156" max="156" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="157" max="157" width="11.44140625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="158" max="158" width="19.5546875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="159" max="159" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="160" max="160" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="161" max="161" width="19.5546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="162" max="162" width="22.5546875" style="106" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="163" max="163" width="15.88671875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="164" max="164" width="16.6640625" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="165" max="165" width="22.5546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="166" max="166" width="26.109375" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="90" max="90" width="14.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="91" max="91" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="92" max="92" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="93" max="93" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="12.5703125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="96" max="96" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="97" max="97" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="98" max="98" width="15.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="58.28515625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="100" max="100" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="101" max="101" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="102" max="102" width="15.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="104" max="104" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="105" max="105" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="106" max="106" width="13.42578125" style="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="107" max="107" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="108" max="108" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="109" max="109" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="110" max="110" width="13.7109375" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="111" max="111" width="14.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="112" max="112" width="27.140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="113" max="113" width="20.140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="114" max="114" width="13.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="115" max="115" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="116" max="116" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="117" max="117" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="118" max="118" width="14.28515625" style="106" customWidth="1" collapsed="1"/>
+    <col min="119" max="119" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="120" max="121" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="122" max="122" width="14.42578125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="123" max="123" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="124" max="124" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="125" max="125" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="126" max="126" width="21.5703125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="127" max="127" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="128" max="128" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="129" max="129" width="11.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="130" max="130" width="23.7109375" style="106" customWidth="1" collapsed="1"/>
+    <col min="131" max="131" width="15.140625" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="132" max="132" width="15.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="133" max="133" width="30.5703125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="134" max="134" width="15.5703125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="135" max="135" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="136" max="136" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="137" max="137" width="15.5703125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="138" max="138" width="15.5703125" style="106" customWidth="1" collapsed="1"/>
+    <col min="139" max="141" width="15.5703125" style="106" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="142" max="142" width="17.5703125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="143" max="143" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="144" max="144" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="145" max="145" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="146" max="146" width="8.5703125" style="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="147" max="147" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="148" max="148" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="149" max="149" width="11.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="150" max="150" width="11.85546875" style="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="151" max="151" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="152" max="152" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="153" max="153" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="154" max="154" width="15.7109375" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="155" max="155" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="156" max="156" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="157" max="157" width="11.42578125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="158" max="158" width="19.5703125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="159" max="159" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="160" max="160" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="161" max="161" width="19.5703125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="162" max="162" width="22.5703125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="163" max="163" width="15.85546875" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="164" max="164" width="16.7109375" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="165" max="165" width="22.5703125" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="166" max="166" width="26.140625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="167" max="169" width="23" style="106" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="170" max="170" width="20.5546875" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="171" max="16384" width="9.109375" style="29"/>
+    <col min="170" max="170" width="20.5703125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="171" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:170" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="64"/>
       <c r="B1" s="59"/>
       <c r="C1" s="103" t="s">
@@ -5357,7 +5357,7 @@
       </c>
       <c r="FN1" s="177"/>
     </row>
-    <row r="2" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
         <v>0</v>
       </c>
@@ -5686,16 +5686,16 @@
         <v>48</v>
       </c>
       <c r="DF2" s="104" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="DG2" s="104" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="DH2" s="104" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="DI2" s="104" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="DJ2" s="104" t="s">
         <v>193</v>
@@ -5869,7 +5869,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="3" spans="1:170" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:170" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>335</v>
       </c>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="FN3" s="183"/>
     </row>
-    <row r="4" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="5" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="67" t="s">
         <v>718</v>
       </c>
@@ -6745,7 +6745,7 @@
       <c r="FM5" s="186"/>
       <c r="FN5" s="185"/>
     </row>
-    <row r="6" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="67" t="s">
         <v>10</v>
       </c>
@@ -6937,7 +6937,7 @@
       <c r="FM6" s="186"/>
       <c r="FN6" s="185"/>
     </row>
-    <row r="7" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="67" t="s">
         <v>540</v>
       </c>
@@ -7117,7 +7117,7 @@
       <c r="FM7" s="186"/>
       <c r="FN7" s="185"/>
     </row>
-    <row r="8" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="67" t="s">
         <v>541</v>
       </c>
@@ -7297,7 +7297,7 @@
       <c r="FM8" s="186"/>
       <c r="FN8" s="185"/>
     </row>
-    <row r="9" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="67" t="s">
         <v>715</v>
       </c>
@@ -7479,7 +7479,7 @@
       <c r="FM9" s="186"/>
       <c r="FN9" s="185"/>
     </row>
-    <row r="10" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="67" t="s">
         <v>43</v>
       </c>
@@ -7646,7 +7646,7 @@
       <c r="DD10" s="115"/>
       <c r="DE10" s="115"/>
       <c r="DF10" s="115" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="DG10" s="115"/>
       <c r="DH10" s="115"/>
@@ -7735,7 +7735,7 @@
       <c r="FM10" s="186"/>
       <c r="FN10" s="185"/>
     </row>
-    <row r="11" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="67" t="s">
         <v>74</v>
       </c>
@@ -7921,7 +7921,7 @@
       <c r="FM11" s="186"/>
       <c r="FN11" s="185"/>
     </row>
-    <row r="12" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="67" t="s">
         <v>73</v>
       </c>
@@ -8113,7 +8113,7 @@
       <c r="FM12" s="186"/>
       <c r="FN12" s="185"/>
     </row>
-    <row r="13" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:170" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="86" t="s">
         <v>331</v>
       </c>
@@ -8523,7 +8523,7 @@
       </c>
       <c r="FN13" s="177"/>
     </row>
-    <row r="14" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="69" t="s">
         <v>655</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="69" t="s">
         <v>642</v>
       </c>
@@ -9063,7 +9063,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="17" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:170" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="86" t="s">
         <v>332</v>
       </c>
@@ -9473,7 +9473,7 @@
       </c>
       <c r="FN17" s="177"/>
     </row>
-    <row r="18" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="67" t="s">
         <v>94</v>
       </c>
@@ -9691,7 +9691,7 @@
       <c r="FM18" s="186"/>
       <c r="FN18" s="185"/>
     </row>
-    <row r="19" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="67" t="s">
         <v>90</v>
       </c>
@@ -9915,7 +9915,7 @@
       <c r="FM19" s="186"/>
       <c r="FN19" s="185"/>
     </row>
-    <row r="20" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="67" t="s">
         <v>92</v>
       </c>
@@ -10042,7 +10042,7 @@
       <c r="CV20" s="115"/>
       <c r="CW20" s="115"/>
       <c r="CX20" s="115" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="CY20" s="115"/>
       <c r="CZ20" s="115"/>
@@ -10133,7 +10133,7 @@
       <c r="FM20" s="186"/>
       <c r="FN20" s="185"/>
     </row>
-    <row r="21" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
         <v>370</v>
       </c>
@@ -10351,7 +10351,7 @@
       <c r="FM21" s="186"/>
       <c r="FN21" s="185"/>
     </row>
-    <row r="22" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="67" t="s">
         <v>93</v>
       </c>
@@ -10502,11 +10502,11 @@
       <c r="DD22" s="115"/>
       <c r="DE22" s="115"/>
       <c r="DF22" s="115" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="DG22" s="115"/>
       <c r="DH22" s="115" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="DI22" s="115"/>
       <c r="DJ22" s="115" t="s">
@@ -10583,7 +10583,7 @@
       <c r="FM22" s="186"/>
       <c r="FN22" s="185"/>
     </row>
-    <row r="23" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:170" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="87" t="s">
         <v>330</v>
       </c>
@@ -10993,7 +10993,7 @@
       </c>
       <c r="FN23" s="177"/>
     </row>
-    <row r="24" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="88" t="s">
         <v>326</v>
       </c>
@@ -11313,7 +11313,7 @@
       <c r="FM24" s="185"/>
       <c r="FN24" s="185"/>
     </row>
-    <row r="25" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:170" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="87" t="s">
         <v>325</v>
       </c>
@@ -11927,7 +11927,7 @@
       <c r="FM26" s="185"/>
       <c r="FN26" s="185"/>
     </row>
-    <row r="27" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="88" t="s">
         <v>371</v>
       </c>
@@ -12577,7 +12577,7 @@
       <c r="FM29" s="185"/>
       <c r="FN29" s="185"/>
     </row>
-    <row r="30" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:170" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="86" t="s">
         <v>333</v>
       </c>
@@ -12987,7 +12987,7 @@
       </c>
       <c r="FN30" s="177"/>
     </row>
-    <row r="31" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="67" t="s">
         <v>88</v>
       </c>
@@ -13116,7 +13116,7 @@
       </c>
       <c r="DG31" s="115"/>
       <c r="DH31" s="115" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="DI31" s="115"/>
       <c r="DJ31" s="115">
@@ -13189,7 +13189,7 @@
       <c r="FM31" s="186"/>
       <c r="FN31" s="185"/>
     </row>
-    <row r="32" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="67" t="s">
         <v>111</v>
       </c>
@@ -13318,7 +13318,7 @@
       </c>
       <c r="DG32" s="115"/>
       <c r="DH32" s="115" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="DI32" s="115"/>
       <c r="DJ32" s="115" t="s">
@@ -13391,7 +13391,7 @@
       <c r="FM32" s="186"/>
       <c r="FN32" s="185"/>
     </row>
-    <row r="33" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="67" t="s">
         <v>91</v>
       </c>
@@ -13520,7 +13520,7 @@
       </c>
       <c r="DG33" s="115"/>
       <c r="DH33" s="115" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="DI33" s="115"/>
       <c r="DJ33" s="115">
@@ -13593,7 +13593,7 @@
       <c r="FM33" s="186"/>
       <c r="FN33" s="185"/>
     </row>
-    <row r="34" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="67" t="s">
         <v>90</v>
       </c>
@@ -13790,7 +13790,7 @@
       </c>
       <c r="DG34" s="115"/>
       <c r="DH34" s="115" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="DI34" s="115"/>
       <c r="DJ34" s="115">
@@ -13903,7 +13903,7 @@
       <c r="FM34" s="186"/>
       <c r="FN34" s="185"/>
     </row>
-    <row r="35" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="67" t="s">
         <v>87</v>
       </c>
@@ -14103,7 +14103,7 @@
       <c r="FM35" s="186"/>
       <c r="FN35" s="185"/>
     </row>
-    <row r="36" spans="1:170" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:170" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="67" t="s">
         <v>89</v>
       </c>
@@ -14232,7 +14232,7 @@
       </c>
       <c r="DG36" s="115"/>
       <c r="DH36" s="115" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="DI36" s="115"/>
       <c r="DJ36" s="115">
@@ -14305,7 +14305,7 @@
       <c r="FM36" s="186"/>
       <c r="FN36" s="185"/>
     </row>
-    <row r="37" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:170" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="86" t="s">
         <v>334</v>
       </c>
@@ -14715,7 +14715,7 @@
       </c>
       <c r="FN37" s="177"/>
     </row>
-    <row r="38" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="69" t="s">
         <v>317</v>
       </c>
@@ -14927,7 +14927,7 @@
       <c r="FM38" s="185"/>
       <c r="FN38" s="185"/>
     </row>
-    <row r="39" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="69" t="s">
         <v>318</v>
       </c>
@@ -15100,7 +15100,7 @@
       <c r="EF39" s="119"/>
       <c r="EG39" s="119"/>
       <c r="EH39" s="119">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="EI39" s="119"/>
       <c r="EJ39" s="119"/>
@@ -15135,7 +15135,7 @@
       <c r="FM39" s="185"/>
       <c r="FN39" s="185"/>
     </row>
-    <row r="40" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="69" t="s">
         <v>319</v>
       </c>
@@ -15266,12 +15266,12 @@
       <c r="DD40" s="119"/>
       <c r="DE40" s="119"/>
       <c r="DF40" s="119" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="DG40" s="119"/>
       <c r="DH40" s="119"/>
       <c r="DI40" s="119" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="DJ40" s="119" t="s">
         <v>377</v>
@@ -15310,7 +15310,7 @@
       <c r="EF40" s="119"/>
       <c r="EG40" s="119"/>
       <c r="EH40" s="119" t="s">
-        <v>739</v>
+        <v>749</v>
       </c>
       <c r="EI40" s="119"/>
       <c r="EJ40" s="119"/>
@@ -15345,7 +15345,7 @@
       <c r="FM40" s="185"/>
       <c r="FN40" s="185"/>
     </row>
-    <row r="41" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="69" t="s">
         <v>626</v>
       </c>
@@ -15553,7 +15553,7 @@
       <c r="FM41" s="185"/>
       <c r="FN41" s="185"/>
     </row>
-    <row r="42" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="69" t="s">
         <v>3</v>
       </c>
@@ -15761,7 +15761,7 @@
       <c r="FM42" s="185"/>
       <c r="FN42" s="185"/>
     </row>
-    <row r="43" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="69" t="s">
         <v>320</v>
       </c>
@@ -15969,7 +15969,7 @@
       <c r="FM43" s="185"/>
       <c r="FN43" s="185"/>
     </row>
-    <row r="44" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:170" s="5" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="69" t="s">
         <v>625</v>
       </c>
@@ -16207,7 +16207,7 @@
       <c r="FM44" s="185"/>
       <c r="FN44" s="185"/>
     </row>
-    <row r="45" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="69" t="s">
         <v>624</v>
       </c>
@@ -16437,7 +16437,7 @@
       <c r="FM45" s="185"/>
       <c r="FN45" s="185"/>
     </row>
-    <row r="46" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="69" t="s">
         <v>4</v>
       </c>
@@ -16645,7 +16645,7 @@
       <c r="FM46" s="185"/>
       <c r="FN46" s="185"/>
     </row>
-    <row r="47" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="69" t="s">
         <v>321</v>
       </c>
@@ -16853,7 +16853,7 @@
       <c r="FM47" s="185"/>
       <c r="FN47" s="185"/>
     </row>
-    <row r="48" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="69" t="s">
         <v>322</v>
       </c>
@@ -17026,7 +17026,7 @@
       <c r="EF48" s="119"/>
       <c r="EG48" s="119"/>
       <c r="EH48" s="119">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="EI48" s="119"/>
       <c r="EJ48" s="119"/>
@@ -17061,7 +17061,7 @@
       <c r="FM48" s="185"/>
       <c r="FN48" s="185"/>
     </row>
-    <row r="49" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="69" t="s">
         <v>323</v>
       </c>
@@ -17269,7 +17269,7 @@
       <c r="FM49" s="185"/>
       <c r="FN49" s="185"/>
     </row>
-    <row r="50" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="69" t="s">
         <v>622</v>
       </c>
@@ -17477,7 +17477,7 @@
       <c r="FM50" s="185"/>
       <c r="FN50" s="185"/>
     </row>
-    <row r="51" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="69" t="s">
         <v>660</v>
       </c>
@@ -17745,7 +17745,7 @@
       <c r="FM51" s="185"/>
       <c r="FN51" s="185"/>
     </row>
-    <row r="52" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:170" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="165" t="s">
         <v>661</v>
       </c>
@@ -17953,7 +17953,7 @@
       <c r="FM52" s="185"/>
       <c r="FN52" s="185"/>
     </row>
-    <row r="53" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="164" t="s">
         <v>594</v>
       </c>
@@ -18361,7 +18361,7 @@
       </c>
       <c r="FN53" s="177"/>
     </row>
-    <row r="54" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="70" t="s">
         <v>113</v>
       </c>
@@ -18543,7 +18543,7 @@
       <c r="FM54" s="185"/>
       <c r="FN54" s="185"/>
     </row>
-    <row r="55" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="68" t="s">
         <v>591</v>
       </c>
@@ -18951,7 +18951,7 @@
       </c>
       <c r="FN55" s="177"/>
     </row>
-    <row r="56" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="70" t="s">
         <v>113</v>
       </c>
@@ -19133,7 +19133,7 @@
       <c r="FM56" s="185"/>
       <c r="FN56" s="185"/>
     </row>
-    <row r="57" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="68" t="s">
         <v>590</v>
       </c>
@@ -19541,7 +19541,7 @@
       </c>
       <c r="FN57" s="177"/>
     </row>
-    <row r="58" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="70" t="s">
         <v>113</v>
       </c>
@@ -19723,7 +19723,7 @@
       <c r="FM58" s="185"/>
       <c r="FN58" s="185"/>
     </row>
-    <row r="59" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="68" t="s">
         <v>595</v>
       </c>
@@ -20131,7 +20131,7 @@
       </c>
       <c r="FN59" s="177"/>
     </row>
-    <row r="60" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="70" t="s">
         <v>113</v>
       </c>
@@ -20313,7 +20313,7 @@
       <c r="FM60" s="185"/>
       <c r="FN60" s="185"/>
     </row>
-    <row r="61" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="68" t="s">
         <v>600</v>
       </c>
@@ -20721,7 +20721,7 @@
       </c>
       <c r="FN61" s="177"/>
     </row>
-    <row r="62" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="70" t="s">
         <v>113</v>
       </c>
@@ -20903,7 +20903,7 @@
       <c r="FM62" s="185"/>
       <c r="FN62" s="185"/>
     </row>
-    <row r="63" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="68" t="s">
         <v>601</v>
       </c>
@@ -21311,7 +21311,7 @@
       </c>
       <c r="FN63" s="177"/>
     </row>
-    <row r="64" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="70" t="s">
         <v>113</v>
       </c>
@@ -21493,7 +21493,7 @@
       <c r="FM64" s="185"/>
       <c r="FN64" s="185"/>
     </row>
-    <row r="65" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="68" t="s">
         <v>597</v>
       </c>
@@ -21901,7 +21901,7 @@
       </c>
       <c r="FN65" s="177"/>
     </row>
-    <row r="66" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="70" t="s">
         <v>113</v>
       </c>
@@ -22083,7 +22083,7 @@
       <c r="FM66" s="185"/>
       <c r="FN66" s="185"/>
     </row>
-    <row r="67" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="68" t="s">
         <v>592</v>
       </c>
@@ -22491,7 +22491,7 @@
       </c>
       <c r="FN67" s="177"/>
     </row>
-    <row r="68" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="70" t="s">
         <v>113</v>
       </c>
@@ -22673,7 +22673,7 @@
       <c r="FM68" s="185"/>
       <c r="FN68" s="185"/>
     </row>
-    <row r="69" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="68" t="s">
         <v>589</v>
       </c>
@@ -23081,7 +23081,7 @@
       </c>
       <c r="FN69" s="177"/>
     </row>
-    <row r="70" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="70" t="s">
         <v>113</v>
       </c>
@@ -23263,7 +23263,7 @@
       <c r="FM70" s="185"/>
       <c r="FN70" s="185"/>
     </row>
-    <row r="71" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="68" t="s">
         <v>598</v>
       </c>
@@ -23671,7 +23671,7 @@
       </c>
       <c r="FN71" s="177"/>
     </row>
-    <row r="72" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="70" t="s">
         <v>113</v>
       </c>
@@ -23853,7 +23853,7 @@
       <c r="FM72" s="185"/>
       <c r="FN72" s="185"/>
     </row>
-    <row r="73" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="68" t="s">
         <v>599</v>
       </c>
@@ -24261,7 +24261,7 @@
       </c>
       <c r="FN73" s="177"/>
     </row>
-    <row r="74" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="70" t="s">
         <v>113</v>
       </c>
@@ -24443,7 +24443,7 @@
       <c r="FM74" s="185"/>
       <c r="FN74" s="185"/>
     </row>
-    <row r="75" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="68" t="s">
         <v>593</v>
       </c>
@@ -24851,7 +24851,7 @@
       </c>
       <c r="FN75" s="177"/>
     </row>
-    <row r="76" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="70" t="s">
         <v>113</v>
       </c>
@@ -25033,7 +25033,7 @@
       <c r="FM76" s="185"/>
       <c r="FN76" s="185"/>
     </row>
-    <row r="77" spans="1:170" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:170" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="68" t="s">
         <v>596</v>
       </c>
@@ -25441,7 +25441,7 @@
       </c>
       <c r="FN77" s="177"/>
     </row>
-    <row r="78" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:170" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="70" t="s">
         <v>113</v>
       </c>
@@ -25637,23 +25637,23 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
     <col min="2" max="3" width="37" style="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="29" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="31.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16"/>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
       <c r="D1" s="195"/>
       <c r="E1" s="83"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
@@ -25670,7 +25670,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>52</v>
       </c>
@@ -25684,10 +25684,10 @@
         <v>697</v>
       </c>
       <c r="E3" s="78" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="84" t="s">
         <v>2</v>
@@ -25700,7 +25700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>60</v>
       </c>
@@ -25717,7 +25717,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
@@ -25734,7 +25734,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="84" t="s">
         <v>2</v>
@@ -25747,7 +25747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>60</v>
       </c>
@@ -25764,7 +25764,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>53</v>
       </c>
@@ -25781,7 +25781,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="84" t="s">
         <v>2</v>
@@ -25794,7 +25794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
@@ -25807,7 +25807,7 @@
       </c>
       <c r="E11" s="80"/>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>53</v>
       </c>
@@ -25820,7 +25820,7 @@
       </c>
       <c r="E12" s="80"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="84" t="s">
         <v>2</v>
@@ -25833,7 +25833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>60</v>
       </c>
@@ -25846,7 +25846,7 @@
       </c>
       <c r="E14" s="80"/>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>53</v>
       </c>
@@ -25859,7 +25859,7 @@
       </c>
       <c r="E15" s="80"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="84" t="s">
         <v>2</v>
@@ -25872,7 +25872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>60</v>
       </c>
@@ -25885,7 +25885,7 @@
       </c>
       <c r="E17" s="80"/>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -25898,7 +25898,7 @@
       </c>
       <c r="E18" s="80"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="82"/>
       <c r="B19" s="84" t="s">
         <v>2</v>
@@ -25911,7 +25911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="79" t="s">
         <v>60</v>
       </c>
@@ -25922,7 +25922,7 @@
       <c r="D20" s="80"/>
       <c r="E20" s="80"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="79" t="s">
         <v>53</v>
       </c>
@@ -25933,7 +25933,7 @@
       <c r="D21" s="80"/>
       <c r="E21" s="80"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="82"/>
       <c r="B22" s="84" t="s">
         <v>2</v>
@@ -25946,7 +25946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="79" t="s">
         <v>60</v>
       </c>
@@ -25957,7 +25957,7 @@
       <c r="D23" s="80"/>
       <c r="E23" s="80"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="79" t="s">
         <v>53</v>
       </c>
@@ -25968,7 +25968,7 @@
       <c r="D24" s="80"/>
       <c r="E24" s="80"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="82"/>
       <c r="B25" s="84" t="s">
         <v>2</v>
@@ -25981,7 +25981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="79" t="s">
         <v>60</v>
       </c>
@@ -25992,7 +25992,7 @@
       <c r="D26" s="80"/>
       <c r="E26" s="80"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="79" t="s">
         <v>53</v>
       </c>
@@ -26003,7 +26003,7 @@
       <c r="D27" s="80"/>
       <c r="E27" s="80"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="82"/>
       <c r="B28" s="84" t="s">
         <v>2</v>
@@ -26016,7 +26016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="79" t="s">
         <v>60</v>
       </c>
@@ -26027,7 +26027,7 @@
       <c r="D29" s="80"/>
       <c r="E29" s="80"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="79" t="s">
         <v>53</v>
       </c>
@@ -26052,22 +26052,22 @@
       <selection pane="topRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.44140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="29" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" style="29" customWidth="1"/>
-    <col min="14" max="14" width="28.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.42578125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="29" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" style="29" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -27141,11 +27141,11 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="17.44140625" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="29"/>
+    <col min="1" max="1" width="35.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="17.42578125" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -27347,15 +27347,15 @@
       <selection activeCell="G196" sqref="G196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" style="29" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="29" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="29"/>
+    <col min="1" max="1" width="37.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="29" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27378,7 +27378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
         <v>141</v>
       </c>
@@ -27392,7 +27392,7 @@
       <c r="E2" s="46"/>
       <c r="F2" s="46"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>141</v>
       </c>
@@ -27406,7 +27406,7 @@
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>141</v>
       </c>
@@ -27420,7 +27420,7 @@
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>141</v>
       </c>
@@ -27434,7 +27434,7 @@
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>141</v>
       </c>
@@ -27448,7 +27448,7 @@
       <c r="E6" s="48"/>
       <c r="F6" s="48"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>141</v>
       </c>
@@ -27462,7 +27462,7 @@
       <c r="E7" s="48"/>
       <c r="F7" s="48"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>141</v>
       </c>
@@ -27476,7 +27476,7 @@
       <c r="E8" s="48"/>
       <c r="F8" s="48"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>141</v>
       </c>
@@ -27490,7 +27490,7 @@
       <c r="E9" s="48"/>
       <c r="F9" s="48"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>141</v>
       </c>
@@ -27504,7 +27504,7 @@
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>153</v>
       </c>
@@ -27516,7 +27516,7 @@
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
         <v>154</v>
       </c>
@@ -27572,7 +27572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>141</v>
       </c>
@@ -27586,7 +27586,7 @@
       <c r="E16" s="46"/>
       <c r="F16" s="46"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
         <v>141</v>
       </c>
@@ -27600,7 +27600,7 @@
       <c r="E17" s="48"/>
       <c r="F17" s="48"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
         <v>141</v>
       </c>
@@ -27614,7 +27614,7 @@
       <c r="E18" s="48"/>
       <c r="F18" s="48"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
         <v>141</v>
       </c>
@@ -27628,7 +27628,7 @@
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
         <v>141</v>
       </c>
@@ -27642,7 +27642,7 @@
       <c r="E20" s="48"/>
       <c r="F20" s="48"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
         <v>141</v>
       </c>
@@ -27656,7 +27656,7 @@
       <c r="E21" s="48"/>
       <c r="F21" s="48"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
         <v>141</v>
       </c>
@@ -27670,7 +27670,7 @@
       <c r="E22" s="48"/>
       <c r="F22" s="48"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>141</v>
       </c>
@@ -27684,7 +27684,7 @@
       <c r="E23" s="48"/>
       <c r="F23" s="48"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
         <v>141</v>
       </c>
@@ -27698,7 +27698,7 @@
       <c r="E24" s="48"/>
       <c r="F24" s="48"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
         <v>141</v>
       </c>
@@ -27712,7 +27712,7 @@
       <c r="E25" s="48"/>
       <c r="F25" s="48"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
         <v>141</v>
       </c>
@@ -27726,7 +27726,7 @@
       <c r="E26" s="48"/>
       <c r="F26" s="48"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>153</v>
       </c>
@@ -27738,7 +27738,7 @@
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>154</v>
       </c>
@@ -27794,7 +27794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="45" t="s">
         <v>141</v>
       </c>
@@ -27808,7 +27808,7 @@
       <c r="E32" s="46"/>
       <c r="F32" s="46"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="47" t="s">
         <v>141</v>
       </c>
@@ -27822,7 +27822,7 @@
       <c r="E33" s="48"/>
       <c r="F33" s="48"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
         <v>141</v>
       </c>
@@ -27836,7 +27836,7 @@
       <c r="E34" s="48"/>
       <c r="F34" s="48"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
         <v>141</v>
       </c>
@@ -27850,7 +27850,7 @@
       <c r="E35" s="48"/>
       <c r="F35" s="48"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
         <v>141</v>
       </c>
@@ -27864,7 +27864,7 @@
       <c r="E36" s="48"/>
       <c r="F36" s="48"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
         <v>141</v>
       </c>
@@ -27878,7 +27878,7 @@
       <c r="E37" s="48"/>
       <c r="F37" s="48"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
         <v>141</v>
       </c>
@@ -27892,7 +27892,7 @@
       <c r="E38" s="48"/>
       <c r="F38" s="48"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="47" t="s">
         <v>141</v>
       </c>
@@ -27906,7 +27906,7 @@
       <c r="E39" s="48"/>
       <c r="F39" s="48"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="47" t="s">
         <v>141</v>
       </c>
@@ -27920,7 +27920,7 @@
       <c r="E40" s="48"/>
       <c r="F40" s="48"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="47" t="s">
         <v>141</v>
       </c>
@@ -27934,7 +27934,7 @@
       <c r="E41" s="48"/>
       <c r="F41" s="48"/>
     </row>
-    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
         <v>141</v>
       </c>
@@ -27948,7 +27948,7 @@
       <c r="E42" s="48"/>
       <c r="F42" s="48"/>
     </row>
-    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="s">
         <v>153</v>
       </c>
@@ -27960,7 +27960,7 @@
       <c r="E43" s="39"/>
       <c r="F43" s="39"/>
     </row>
-    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="s">
         <v>154</v>
       </c>
@@ -28016,7 +28016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="45" t="s">
         <v>141</v>
       </c>
@@ -28030,7 +28030,7 @@
       <c r="E48" s="46"/>
       <c r="F48" s="46"/>
     </row>
-    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
         <v>141</v>
       </c>
@@ -28044,7 +28044,7 @@
       <c r="E49" s="48"/>
       <c r="F49" s="48"/>
     </row>
-    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
         <v>141</v>
       </c>
@@ -28058,7 +28058,7 @@
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
     </row>
-    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="47" t="s">
         <v>141</v>
       </c>
@@ -28072,7 +28072,7 @@
       <c r="E51" s="48"/>
       <c r="F51" s="48"/>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="47" t="s">
         <v>141</v>
       </c>
@@ -28086,7 +28086,7 @@
       <c r="E52" s="48"/>
       <c r="F52" s="48"/>
     </row>
-    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
         <v>141</v>
       </c>
@@ -28100,7 +28100,7 @@
       <c r="E53" s="48"/>
       <c r="F53" s="48"/>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="47" t="s">
         <v>141</v>
       </c>
@@ -28114,7 +28114,7 @@
       <c r="E54" s="48"/>
       <c r="F54" s="48"/>
     </row>
-    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="47" t="s">
         <v>141</v>
       </c>
@@ -28128,7 +28128,7 @@
       <c r="E55" s="48"/>
       <c r="F55" s="48"/>
     </row>
-    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
         <v>141</v>
       </c>
@@ -28142,7 +28142,7 @@
       <c r="E56" s="48"/>
       <c r="F56" s="48"/>
     </row>
-    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="47" t="s">
         <v>141</v>
       </c>
@@ -28156,7 +28156,7 @@
       <c r="E57" s="48"/>
       <c r="F57" s="48"/>
     </row>
-    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="47" t="s">
         <v>141</v>
       </c>
@@ -28170,7 +28170,7 @@
       <c r="E58" s="48"/>
       <c r="F58" s="48"/>
     </row>
-    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="37" t="s">
         <v>153</v>
       </c>
@@ -28182,7 +28182,7 @@
       <c r="E59" s="39"/>
       <c r="F59" s="39"/>
     </row>
-    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="37" t="s">
         <v>154</v>
       </c>
@@ -28238,7 +28238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="45" t="s">
         <v>141</v>
       </c>
@@ -28252,7 +28252,7 @@
       <c r="E64" s="46"/>
       <c r="F64" s="46"/>
     </row>
-    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
         <v>141</v>
       </c>
@@ -28266,7 +28266,7 @@
       <c r="E65" s="48"/>
       <c r="F65" s="48"/>
     </row>
-    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="47" t="s">
         <v>141</v>
       </c>
@@ -28280,7 +28280,7 @@
       <c r="E66" s="48"/>
       <c r="F66" s="48"/>
     </row>
-    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="47" t="s">
         <v>141</v>
       </c>
@@ -28294,7 +28294,7 @@
       <c r="E67" s="48"/>
       <c r="F67" s="48"/>
     </row>
-    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="47" t="s">
         <v>141</v>
       </c>
@@ -28308,7 +28308,7 @@
       <c r="E68" s="48"/>
       <c r="F68" s="48"/>
     </row>
-    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="47" t="s">
         <v>141</v>
       </c>
@@ -28322,7 +28322,7 @@
       <c r="E69" s="48"/>
       <c r="F69" s="48"/>
     </row>
-    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="47" t="s">
         <v>141</v>
       </c>
@@ -28336,7 +28336,7 @@
       <c r="E70" s="48"/>
       <c r="F70" s="48"/>
     </row>
-    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="47" t="s">
         <v>141</v>
       </c>
@@ -28350,7 +28350,7 @@
       <c r="E71" s="48"/>
       <c r="F71" s="48"/>
     </row>
-    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="47" t="s">
         <v>141</v>
       </c>
@@ -28364,7 +28364,7 @@
       <c r="E72" s="48"/>
       <c r="F72" s="48"/>
     </row>
-    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="47" t="s">
         <v>141</v>
       </c>
@@ -28378,7 +28378,7 @@
       <c r="E73" s="48"/>
       <c r="F73" s="48"/>
     </row>
-    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="47" t="s">
         <v>141</v>
       </c>
@@ -28392,7 +28392,7 @@
       <c r="E74" s="48"/>
       <c r="F74" s="48"/>
     </row>
-    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="37" t="s">
         <v>153</v>
       </c>
@@ -28404,7 +28404,7 @@
       <c r="E75" s="39"/>
       <c r="F75" s="39"/>
     </row>
-    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="37" t="s">
         <v>154</v>
       </c>
@@ -28460,7 +28460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
         <v>141</v>
       </c>
@@ -28474,7 +28474,7 @@
       <c r="E80" s="46"/>
       <c r="F80" s="46"/>
     </row>
-    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="45" t="s">
         <v>141</v>
       </c>
@@ -28488,7 +28488,7 @@
       <c r="E81" s="46"/>
       <c r="F81" s="46"/>
     </row>
-    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="45" t="s">
         <v>141</v>
       </c>
@@ -28502,7 +28502,7 @@
       <c r="E82" s="46"/>
       <c r="F82" s="46"/>
     </row>
-    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="47" t="s">
         <v>141</v>
       </c>
@@ -28516,7 +28516,7 @@
       <c r="E83" s="48"/>
       <c r="F83" s="48"/>
     </row>
-    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="47" t="s">
         <v>141</v>
       </c>
@@ -28530,7 +28530,7 @@
       <c r="E84" s="48"/>
       <c r="F84" s="48"/>
     </row>
-    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="47" t="s">
         <v>141</v>
       </c>
@@ -28544,7 +28544,7 @@
       <c r="E85" s="48"/>
       <c r="F85" s="48"/>
     </row>
-    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="47" t="s">
         <v>141</v>
       </c>
@@ -28558,7 +28558,7 @@
       <c r="E86" s="48"/>
       <c r="F86" s="48"/>
     </row>
-    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="47" t="s">
         <v>141</v>
       </c>
@@ -28572,7 +28572,7 @@
       <c r="E87" s="48"/>
       <c r="F87" s="48"/>
     </row>
-    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="47" t="s">
         <v>141</v>
       </c>
@@ -28586,7 +28586,7 @@
       <c r="E88" s="48"/>
       <c r="F88" s="48"/>
     </row>
-    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="47" t="s">
         <v>141</v>
       </c>
@@ -28600,7 +28600,7 @@
       <c r="E89" s="48"/>
       <c r="F89" s="48"/>
     </row>
-    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="47" t="s">
         <v>141</v>
       </c>
@@ -28614,7 +28614,7 @@
       <c r="E90" s="48"/>
       <c r="F90" s="48"/>
     </row>
-    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="37" t="s">
         <v>153</v>
       </c>
@@ -28626,7 +28626,7 @@
       <c r="E91" s="39"/>
       <c r="F91" s="39"/>
     </row>
-    <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="37" t="s">
         <v>154</v>
       </c>
@@ -28682,7 +28682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="45" t="s">
         <v>141</v>
       </c>
@@ -28696,7 +28696,7 @@
       <c r="E96" s="46"/>
       <c r="F96" s="46"/>
     </row>
-    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="45" t="s">
         <v>141</v>
       </c>
@@ -28710,7 +28710,7 @@
       <c r="E97" s="46"/>
       <c r="F97" s="46"/>
     </row>
-    <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="45" t="s">
         <v>141</v>
       </c>
@@ -28724,7 +28724,7 @@
       <c r="E98" s="46"/>
       <c r="F98" s="46"/>
     </row>
-    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="45" t="s">
         <v>141</v>
       </c>
@@ -28738,7 +28738,7 @@
       <c r="E99" s="46"/>
       <c r="F99" s="46"/>
     </row>
-    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="47" t="s">
         <v>141</v>
       </c>
@@ -28752,7 +28752,7 @@
       <c r="E100" s="48"/>
       <c r="F100" s="48"/>
     </row>
-    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="47" t="s">
         <v>141</v>
       </c>
@@ -28766,7 +28766,7 @@
       <c r="E101" s="48"/>
       <c r="F101" s="48"/>
     </row>
-    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="47" t="s">
         <v>141</v>
       </c>
@@ -28780,7 +28780,7 @@
       <c r="E102" s="48"/>
       <c r="F102" s="48"/>
     </row>
-    <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="47" t="s">
         <v>141</v>
       </c>
@@ -28794,7 +28794,7 @@
       <c r="E103" s="48"/>
       <c r="F103" s="48"/>
     </row>
-    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="47" t="s">
         <v>141</v>
       </c>
@@ -28808,7 +28808,7 @@
       <c r="E104" s="48"/>
       <c r="F104" s="48"/>
     </row>
-    <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="47" t="s">
         <v>141</v>
       </c>
@@ -28822,7 +28822,7 @@
       <c r="E105" s="48"/>
       <c r="F105" s="48"/>
     </row>
-    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="47" t="s">
         <v>141</v>
       </c>
@@ -28836,7 +28836,7 @@
       <c r="E106" s="48"/>
       <c r="F106" s="48"/>
     </row>
-    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="37" t="s">
         <v>153</v>
       </c>
@@ -28848,7 +28848,7 @@
       <c r="E107" s="39"/>
       <c r="F107" s="39"/>
     </row>
-    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="37" t="s">
         <v>154</v>
       </c>
@@ -28904,7 +28904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="45" t="s">
         <v>141</v>
       </c>
@@ -28918,7 +28918,7 @@
       <c r="E112" s="46"/>
       <c r="F112" s="46"/>
     </row>
-    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="47" t="s">
         <v>141</v>
       </c>
@@ -28932,7 +28932,7 @@
       <c r="E113" s="48"/>
       <c r="F113" s="48"/>
     </row>
-    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="47" t="s">
         <v>141</v>
       </c>
@@ -28946,7 +28946,7 @@
       <c r="E114" s="48"/>
       <c r="F114" s="48"/>
     </row>
-    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="47" t="s">
         <v>141</v>
       </c>
@@ -28960,7 +28960,7 @@
       <c r="E115" s="48"/>
       <c r="F115" s="48"/>
     </row>
-    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="47" t="s">
         <v>141</v>
       </c>
@@ -28974,7 +28974,7 @@
       <c r="E116" s="48"/>
       <c r="F116" s="48"/>
     </row>
-    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="47" t="s">
         <v>141</v>
       </c>
@@ -28988,7 +28988,7 @@
       <c r="E117" s="48"/>
       <c r="F117" s="48"/>
     </row>
-    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="47" t="s">
         <v>141</v>
       </c>
@@ -29002,7 +29002,7 @@
       <c r="E118" s="48"/>
       <c r="F118" s="48"/>
     </row>
-    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="47" t="s">
         <v>141</v>
       </c>
@@ -29016,7 +29016,7 @@
       <c r="E119" s="48"/>
       <c r="F119" s="48"/>
     </row>
-    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="47" t="s">
         <v>141</v>
       </c>
@@ -29030,7 +29030,7 @@
       <c r="E120" s="48"/>
       <c r="F120" s="48"/>
     </row>
-    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="47" t="s">
         <v>141</v>
       </c>
@@ -29044,7 +29044,7 @@
       <c r="E121" s="48"/>
       <c r="F121" s="48"/>
     </row>
-    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="47" t="s">
         <v>141</v>
       </c>
@@ -29058,7 +29058,7 @@
       <c r="E122" s="48"/>
       <c r="F122" s="48"/>
     </row>
-    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="37" t="s">
         <v>153</v>
       </c>
@@ -29070,7 +29070,7 @@
       <c r="E123" s="39"/>
       <c r="F123" s="39"/>
     </row>
-    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="37" t="s">
         <v>154</v>
       </c>
@@ -29126,7 +29126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="45" t="s">
         <v>141</v>
       </c>
@@ -29140,7 +29140,7 @@
       <c r="E128" s="46"/>
       <c r="F128" s="46"/>
     </row>
-    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="47" t="s">
         <v>141</v>
       </c>
@@ -29154,7 +29154,7 @@
       <c r="E129" s="48"/>
       <c r="F129" s="48"/>
     </row>
-    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="47" t="s">
         <v>141</v>
       </c>
@@ -29168,7 +29168,7 @@
       <c r="E130" s="48"/>
       <c r="F130" s="48"/>
     </row>
-    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="47" t="s">
         <v>141</v>
       </c>
@@ -29182,7 +29182,7 @@
       <c r="E131" s="48"/>
       <c r="F131" s="48"/>
     </row>
-    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="47" t="s">
         <v>141</v>
       </c>
@@ -29196,7 +29196,7 @@
       <c r="E132" s="48"/>
       <c r="F132" s="48"/>
     </row>
-    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="47" t="s">
         <v>141</v>
       </c>
@@ -29210,7 +29210,7 @@
       <c r="E133" s="48"/>
       <c r="F133" s="48"/>
     </row>
-    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="47" t="s">
         <v>141</v>
       </c>
@@ -29224,7 +29224,7 @@
       <c r="E134" s="48"/>
       <c r="F134" s="48"/>
     </row>
-    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="47" t="s">
         <v>141</v>
       </c>
@@ -29238,7 +29238,7 @@
       <c r="E135" s="48"/>
       <c r="F135" s="48"/>
     </row>
-    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="47" t="s">
         <v>141</v>
       </c>
@@ -29252,7 +29252,7 @@
       <c r="E136" s="48"/>
       <c r="F136" s="48"/>
     </row>
-    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="47" t="s">
         <v>141</v>
       </c>
@@ -29266,7 +29266,7 @@
       <c r="E137" s="48"/>
       <c r="F137" s="48"/>
     </row>
-    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="47" t="s">
         <v>141</v>
       </c>
@@ -29280,7 +29280,7 @@
       <c r="E138" s="48"/>
       <c r="F138" s="48"/>
     </row>
-    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="37" t="s">
         <v>153</v>
       </c>
@@ -29292,7 +29292,7 @@
       <c r="E139" s="39"/>
       <c r="F139" s="39"/>
     </row>
-    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="37" t="s">
         <v>154</v>
       </c>
@@ -29348,7 +29348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="45" t="s">
         <v>141</v>
       </c>
@@ -29362,7 +29362,7 @@
       <c r="E144" s="46"/>
       <c r="F144" s="46"/>
     </row>
-    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="45" t="s">
         <v>141</v>
       </c>
@@ -29376,7 +29376,7 @@
       <c r="E145" s="46"/>
       <c r="F145" s="46"/>
     </row>
-    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="45" t="s">
         <v>141</v>
       </c>
@@ -29390,7 +29390,7 @@
       <c r="E146" s="46"/>
       <c r="F146" s="46"/>
     </row>
-    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="45" t="s">
         <v>141</v>
       </c>
@@ -29404,7 +29404,7 @@
       <c r="E147" s="46"/>
       <c r="F147" s="46"/>
     </row>
-    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="47" t="s">
         <v>141</v>
       </c>
@@ -29418,7 +29418,7 @@
       <c r="E148" s="48"/>
       <c r="F148" s="48"/>
     </row>
-    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="47" t="s">
         <v>141</v>
       </c>
@@ -29432,7 +29432,7 @@
       <c r="E149" s="48"/>
       <c r="F149" s="48"/>
     </row>
-    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="47" t="s">
         <v>141</v>
       </c>
@@ -29446,7 +29446,7 @@
       <c r="E150" s="48"/>
       <c r="F150" s="48"/>
     </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="47" t="s">
         <v>141</v>
       </c>
@@ -29460,7 +29460,7 @@
       <c r="E151" s="48"/>
       <c r="F151" s="48"/>
     </row>
-    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="47" t="s">
         <v>141</v>
       </c>
@@ -29474,7 +29474,7 @@
       <c r="E152" s="48"/>
       <c r="F152" s="48"/>
     </row>
-    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="47" t="s">
         <v>141</v>
       </c>
@@ -29488,7 +29488,7 @@
       <c r="E153" s="48"/>
       <c r="F153" s="48"/>
     </row>
-    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="47" t="s">
         <v>141</v>
       </c>
@@ -29502,7 +29502,7 @@
       <c r="E154" s="48"/>
       <c r="F154" s="48"/>
     </row>
-    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="37" t="s">
         <v>153</v>
       </c>
@@ -29514,7 +29514,7 @@
       <c r="E155" s="39"/>
       <c r="F155" s="39"/>
     </row>
-    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="37" t="s">
         <v>154</v>
       </c>
@@ -29570,7 +29570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="45" t="s">
         <v>141</v>
       </c>
@@ -29584,7 +29584,7 @@
       <c r="E160" s="46"/>
       <c r="F160" s="46"/>
     </row>
-    <row r="161" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="45" t="s">
         <v>141</v>
       </c>
@@ -29598,7 +29598,7 @@
       <c r="E161" s="46"/>
       <c r="F161" s="46"/>
     </row>
-    <row r="162" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="45" t="s">
         <v>141</v>
       </c>
@@ -29612,7 +29612,7 @@
       <c r="E162" s="46"/>
       <c r="F162" s="46"/>
     </row>
-    <row r="163" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="45" t="s">
         <v>141</v>
       </c>
@@ -29626,7 +29626,7 @@
       <c r="E163" s="46"/>
       <c r="F163" s="46"/>
     </row>
-    <row r="164" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="47" t="s">
         <v>141</v>
       </c>
@@ -29640,7 +29640,7 @@
       <c r="E164" s="48"/>
       <c r="F164" s="48"/>
     </row>
-    <row r="165" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="47" t="s">
         <v>141</v>
       </c>
@@ -29654,7 +29654,7 @@
       <c r="E165" s="48"/>
       <c r="F165" s="48"/>
     </row>
-    <row r="166" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="47" t="s">
         <v>141</v>
       </c>
@@ -29668,7 +29668,7 @@
       <c r="E166" s="48"/>
       <c r="F166" s="48"/>
     </row>
-    <row r="167" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="47" t="s">
         <v>141</v>
       </c>
@@ -29682,7 +29682,7 @@
       <c r="E167" s="48"/>
       <c r="F167" s="48"/>
     </row>
-    <row r="168" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="47" t="s">
         <v>141</v>
       </c>
@@ -29696,7 +29696,7 @@
       <c r="E168" s="48"/>
       <c r="F168" s="48"/>
     </row>
-    <row r="169" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="47" t="s">
         <v>141</v>
       </c>
@@ -29710,7 +29710,7 @@
       <c r="E169" s="48"/>
       <c r="F169" s="48"/>
     </row>
-    <row r="170" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="47" t="s">
         <v>141</v>
       </c>
@@ -29724,7 +29724,7 @@
       <c r="E170" s="48"/>
       <c r="F170" s="48"/>
     </row>
-    <row r="171" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="37" t="s">
         <v>153</v>
       </c>
@@ -29736,7 +29736,7 @@
       <c r="E171" s="39"/>
       <c r="F171" s="39"/>
     </row>
-    <row r="172" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="37" t="s">
         <v>154</v>
       </c>
@@ -29792,7 +29792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="45" t="s">
         <v>141</v>
       </c>
@@ -29806,7 +29806,7 @@
       <c r="E176" s="46"/>
       <c r="F176" s="46"/>
     </row>
-    <row r="177" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="45" t="s">
         <v>141</v>
       </c>
@@ -29820,7 +29820,7 @@
       <c r="E177" s="46"/>
       <c r="F177" s="46"/>
     </row>
-    <row r="178" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="45" t="s">
         <v>141</v>
       </c>
@@ -29834,7 +29834,7 @@
       <c r="E178" s="46"/>
       <c r="F178" s="46"/>
     </row>
-    <row r="179" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="45" t="s">
         <v>141</v>
       </c>
@@ -29848,7 +29848,7 @@
       <c r="E179" s="46"/>
       <c r="F179" s="46"/>
     </row>
-    <row r="180" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="47" t="s">
         <v>141</v>
       </c>
@@ -29862,7 +29862,7 @@
       <c r="E180" s="48"/>
       <c r="F180" s="48"/>
     </row>
-    <row r="181" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="47" t="s">
         <v>141</v>
       </c>
@@ -29876,7 +29876,7 @@
       <c r="E181" s="48"/>
       <c r="F181" s="48"/>
     </row>
-    <row r="182" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="47" t="s">
         <v>141</v>
       </c>
@@ -29890,7 +29890,7 @@
       <c r="E182" s="48"/>
       <c r="F182" s="48"/>
     </row>
-    <row r="183" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="47" t="s">
         <v>141</v>
       </c>
@@ -29904,7 +29904,7 @@
       <c r="E183" s="48"/>
       <c r="F183" s="48"/>
     </row>
-    <row r="184" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="47" t="s">
         <v>141</v>
       </c>
@@ -29918,7 +29918,7 @@
       <c r="E184" s="48"/>
       <c r="F184" s="48"/>
     </row>
-    <row r="185" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="47" t="s">
         <v>141</v>
       </c>
@@ -29932,7 +29932,7 @@
       <c r="E185" s="48"/>
       <c r="F185" s="48"/>
     </row>
-    <row r="186" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="47" t="s">
         <v>141</v>
       </c>
@@ -29946,7 +29946,7 @@
       <c r="E186" s="48"/>
       <c r="F186" s="48"/>
     </row>
-    <row r="187" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="37" t="s">
         <v>153</v>
       </c>
@@ -29958,7 +29958,7 @@
       <c r="E187" s="39"/>
       <c r="F187" s="39"/>
     </row>
-    <row r="188" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="37" t="s">
         <v>154</v>
       </c>
@@ -30014,7 +30014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="45" t="s">
         <v>141</v>
       </c>
@@ -30028,7 +30028,7 @@
       <c r="E192" s="46"/>
       <c r="F192" s="46"/>
     </row>
-    <row r="193" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="47" t="s">
         <v>141</v>
       </c>
@@ -30042,7 +30042,7 @@
       <c r="E193" s="48"/>
       <c r="F193" s="48"/>
     </row>
-    <row r="194" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="47" t="s">
         <v>141</v>
       </c>
@@ -30056,7 +30056,7 @@
       <c r="E194" s="48"/>
       <c r="F194" s="48"/>
     </row>
-    <row r="195" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="47" t="s">
         <v>141</v>
       </c>
@@ -30070,7 +30070,7 @@
       <c r="E195" s="48"/>
       <c r="F195" s="48"/>
     </row>
-    <row r="196" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="47" t="s">
         <v>141</v>
       </c>
@@ -30084,7 +30084,7 @@
       <c r="E196" s="48"/>
       <c r="F196" s="48"/>
     </row>
-    <row r="197" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="47" t="s">
         <v>141</v>
       </c>
@@ -30098,7 +30098,7 @@
       <c r="E197" s="48"/>
       <c r="F197" s="48"/>
     </row>
-    <row r="198" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="47" t="s">
         <v>141</v>
       </c>
@@ -30112,7 +30112,7 @@
       <c r="E198" s="48"/>
       <c r="F198" s="48"/>
     </row>
-    <row r="199" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="47" t="s">
         <v>141</v>
       </c>
@@ -30126,7 +30126,7 @@
       <c r="E199" s="48"/>
       <c r="F199" s="48"/>
     </row>
-    <row r="200" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="47" t="s">
         <v>141</v>
       </c>
@@ -30140,7 +30140,7 @@
       <c r="E200" s="48"/>
       <c r="F200" s="48"/>
     </row>
-    <row r="201" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="47" t="s">
         <v>141</v>
       </c>
@@ -30154,7 +30154,7 @@
       <c r="E201" s="48"/>
       <c r="F201" s="48"/>
     </row>
-    <row r="202" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="47" t="s">
         <v>141</v>
       </c>
@@ -30168,7 +30168,7 @@
       <c r="E202" s="48"/>
       <c r="F202" s="48"/>
     </row>
-    <row r="203" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="37" t="s">
         <v>153</v>
       </c>
@@ -30180,7 +30180,7 @@
       <c r="E203" s="39"/>
       <c r="F203" s="39"/>
     </row>
-    <row r="204" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="37" t="s">
         <v>154</v>
       </c>
@@ -30192,7 +30192,7 @@
       <c r="E204" s="39"/>
       <c r="F204" s="39"/>
     </row>
-    <row r="205" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A205" s="37" t="s">
         <v>155</v>
       </c>
@@ -30204,7 +30204,7 @@
       <c r="E205" s="39"/>
       <c r="F205" s="39"/>
     </row>
-    <row r="206" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A206" s="49" t="s">
         <v>162</v>
       </c>
@@ -30216,7 +30216,7 @@
       <c r="E206" s="44"/>
       <c r="F206" s="44"/>
     </row>
-    <row r="207" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A207" s="35" t="s">
         <v>717</v>
       </c>
@@ -30236,7 +30236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A208" s="45" t="s">
         <v>141</v>
       </c>
@@ -30250,7 +30250,7 @@
       <c r="E208" s="46"/>
       <c r="F208" s="46"/>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A209" s="47" t="s">
         <v>141</v>
       </c>
@@ -30264,7 +30264,7 @@
       <c r="E209" s="48"/>
       <c r="F209" s="48"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A210" s="47" t="s">
         <v>141</v>
       </c>
@@ -30278,7 +30278,7 @@
       <c r="E210" s="48"/>
       <c r="F210" s="48"/>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A211" s="47" t="s">
         <v>141</v>
       </c>
@@ -30292,7 +30292,7 @@
       <c r="E211" s="48"/>
       <c r="F211" s="48"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A212" s="47" t="s">
         <v>141</v>
       </c>
@@ -30306,7 +30306,7 @@
       <c r="E212" s="48"/>
       <c r="F212" s="48"/>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A213" s="47" t="s">
         <v>141</v>
       </c>
@@ -30320,7 +30320,7 @@
       <c r="E213" s="48"/>
       <c r="F213" s="48"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A214" s="47" t="s">
         <v>141</v>
       </c>
@@ -30334,7 +30334,7 @@
       <c r="E214" s="48"/>
       <c r="F214" s="48"/>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A215" s="47" t="s">
         <v>141</v>
       </c>
@@ -30348,7 +30348,7 @@
       <c r="E215" s="48"/>
       <c r="F215" s="48"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A216" s="47" t="s">
         <v>141</v>
       </c>
@@ -30362,7 +30362,7 @@
       <c r="E216" s="48"/>
       <c r="F216" s="48"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A217" s="47" t="s">
         <v>141</v>
       </c>
@@ -30376,7 +30376,7 @@
       <c r="E217" s="48"/>
       <c r="F217" s="48"/>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A218" s="47" t="s">
         <v>141</v>
       </c>
@@ -30390,7 +30390,7 @@
       <c r="E218" s="48"/>
       <c r="F218" s="48"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A219" s="37" t="s">
         <v>153</v>
       </c>
@@ -30402,7 +30402,7 @@
       <c r="E219" s="39"/>
       <c r="F219" s="39"/>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A220" s="37" t="s">
         <v>154</v>
       </c>
@@ -30414,7 +30414,7 @@
       <c r="E220" s="39"/>
       <c r="F220" s="39"/>
     </row>
-    <row r="221" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A221" s="37" t="s">
         <v>155</v>
       </c>
@@ -30426,7 +30426,7 @@
       <c r="E221" s="39"/>
       <c r="F221" s="39"/>
     </row>
-    <row r="222" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A222" s="49" t="s">
         <v>162</v>
       </c>
@@ -30452,12 +30452,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" style="12" customWidth="1"/>
-    <col min="3" max="3" width="50.88671875" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="29"/>
+    <col min="3" max="3" width="50.85546875" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30471,21 +30471,21 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>196</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>238</v>
       </c>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>198</v>
       </c>
@@ -30494,7 +30494,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>197</v>
       </c>
@@ -30519,21 +30519,21 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>236</v>
       </c>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
         <v>237</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>242</v>
       </c>
@@ -30558,7 +30558,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>239</v>
       </c>
@@ -30583,63 +30583,63 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
         <v>203</v>
       </c>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>204</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="55" t="s">
         <v>205</v>
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="55" t="s">
         <v>206</v>
       </c>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="55" t="s">
         <v>207</v>
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="47"/>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="55" t="s">
         <v>208</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="55" t="s">
         <v>209</v>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="47"/>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>210</v>
       </c>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
     </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="55" t="s">
         <v>211</v>
       </c>
@@ -30664,28 +30664,28 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
         <v>214</v>
       </c>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="55" t="s">
         <v>215</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="55" t="s">
         <v>216</v>
       </c>
       <c r="B29" s="47"/>
       <c r="C29" s="47"/>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="55" t="s">
         <v>217</v>
       </c>
@@ -30710,56 +30710,56 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
         <v>220</v>
       </c>
       <c r="B33" s="45"/>
       <c r="C33" s="45"/>
     </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="55" t="s">
         <v>221</v>
       </c>
       <c r="B34" s="47"/>
       <c r="C34" s="47"/>
     </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>222</v>
       </c>
       <c r="B35" s="47"/>
       <c r="C35" s="47"/>
     </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
         <v>223</v>
       </c>
       <c r="B36" s="47"/>
       <c r="C36" s="47"/>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="55" t="s">
         <v>224</v>
       </c>
       <c r="B37" s="47"/>
       <c r="C37" s="47"/>
     </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
         <v>225</v>
       </c>
       <c r="B38" s="47"/>
       <c r="C38" s="47"/>
     </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="55" t="s">
         <v>226</v>
       </c>
       <c r="B39" s="47"/>
       <c r="C39" s="47"/>
     </row>
-    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="55" t="s">
         <v>227</v>
       </c>
@@ -30784,35 +30784,35 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
         <v>230</v>
       </c>
       <c r="B43" s="45"/>
       <c r="C43" s="45"/>
     </row>
-    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="55" t="s">
         <v>231</v>
       </c>
       <c r="B44" s="47"/>
       <c r="C44" s="47"/>
     </row>
-    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="55" t="s">
         <v>232</v>
       </c>
       <c r="B45" s="47"/>
       <c r="C45" s="47"/>
     </row>
-    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="55" t="s">
         <v>233</v>
       </c>
       <c r="B46" s="47"/>
       <c r="C46" s="47"/>
     </row>
-    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="55" t="s">
         <v>234</v>
       </c>
@@ -30837,63 +30837,63 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="54" t="s">
         <v>246</v>
       </c>
       <c r="B50" s="45"/>
       <c r="C50" s="45"/>
     </row>
-    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>247</v>
       </c>
       <c r="B51" s="47"/>
       <c r="C51" s="47"/>
     </row>
-    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>248</v>
       </c>
       <c r="B52" s="47"/>
       <c r="C52" s="47"/>
     </row>
-    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="55" t="s">
         <v>249</v>
       </c>
       <c r="B53" s="47"/>
       <c r="C53" s="47"/>
     </row>
-    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="55" t="s">
         <v>250</v>
       </c>
       <c r="B54" s="47"/>
       <c r="C54" s="47"/>
     </row>
-    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>241</v>
       </c>
       <c r="B55" s="47"/>
       <c r="C55" s="47"/>
     </row>
-    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="56" t="s">
         <v>240</v>
       </c>
       <c r="B56" s="57"/>
       <c r="C56" s="57"/>
     </row>
-    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="55" t="s">
         <v>251</v>
       </c>
       <c r="B57" s="47"/>
       <c r="C57" s="47"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="55" t="s">
         <v>252</v>
       </c>
@@ -30914,24 +30914,24 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="124"/>
-    <col min="3" max="3" width="19.5546875" style="138" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.5546875" style="139" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" style="139" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" style="139" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" style="139" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.44140625" style="139" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="139" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" style="139" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" style="139" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" style="139" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="73.5546875" style="124" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="124"/>
+    <col min="1" max="2" width="9.140625" style="124"/>
+    <col min="3" max="3" width="19.5703125" style="138" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.5703125" style="139" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="139" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="139" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="139" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" style="139" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="139" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="139" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="139" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="139" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="73.5703125" style="124" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="124"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="120" t="s">
         <v>405</v>
       </c>
@@ -30975,7 +30975,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="125" t="s">
         <v>417</v>
       </c>
@@ -31019,7 +31019,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="125" t="s">
         <v>417</v>
       </c>
@@ -31063,7 +31063,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="125" t="s">
         <v>417</v>
       </c>
@@ -31105,7 +31105,7 @@
       </c>
       <c r="N4" s="125"/>
     </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="125" t="s">
         <v>417</v>
       </c>
@@ -31149,7 +31149,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="125" t="s">
         <v>417</v>
       </c>
@@ -31193,7 +31193,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="125" t="s">
         <v>417</v>
       </c>
@@ -31237,7 +31237,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="125" t="s">
         <v>417</v>
       </c>
@@ -31279,7 +31279,7 @@
       </c>
       <c r="N8" s="125"/>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="125" t="s">
         <v>417</v>
       </c>
@@ -31323,7 +31323,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="125" t="s">
         <v>417</v>
       </c>
@@ -31367,7 +31367,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="125" t="s">
         <v>417</v>
       </c>
@@ -31409,7 +31409,7 @@
       </c>
       <c r="N11" s="125"/>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="125" t="s">
         <v>417</v>
       </c>
@@ -31451,7 +31451,7 @@
       </c>
       <c r="N12" s="125"/>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="125" t="s">
         <v>417</v>
       </c>
@@ -31493,7 +31493,7 @@
       </c>
       <c r="N13" s="125"/>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="125" t="s">
         <v>417</v>
       </c>
@@ -31535,7 +31535,7 @@
       </c>
       <c r="N14" s="125"/>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="130" t="s">
         <v>523</v>
       </c>
@@ -31579,7 +31579,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="130" t="s">
         <v>523</v>
       </c>
@@ -31621,7 +31621,7 @@
       </c>
       <c r="N16" s="130"/>
     </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="130" t="s">
         <v>523</v>
       </c>
@@ -31663,7 +31663,7 @@
       </c>
       <c r="N17" s="130"/>
     </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="130" t="s">
         <v>523</v>
       </c>
@@ -31705,7 +31705,7 @@
       </c>
       <c r="N18" s="130"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="130" t="s">
         <v>523</v>
       </c>
@@ -31747,7 +31747,7 @@
       </c>
       <c r="N19" s="130"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="130" t="s">
         <v>523</v>
       </c>
@@ -31789,7 +31789,7 @@
       </c>
       <c r="N20" s="130"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="130" t="s">
         <v>523</v>
       </c>
@@ -31831,7 +31831,7 @@
       </c>
       <c r="N21" s="130"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="130" t="s">
         <v>523</v>
       </c>
@@ -31873,7 +31873,7 @@
       </c>
       <c r="N22" s="130"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="130" t="s">
         <v>523</v>
       </c>
@@ -31915,7 +31915,7 @@
       </c>
       <c r="N23" s="130"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="130" t="s">
         <v>523</v>
       </c>
@@ -31957,7 +31957,7 @@
       </c>
       <c r="N24" s="130"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="130" t="s">
         <v>523</v>
       </c>
@@ -31999,7 +31999,7 @@
       </c>
       <c r="N25" s="130"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="130" t="s">
         <v>523</v>
       </c>
@@ -32041,7 +32041,7 @@
       </c>
       <c r="N26" s="130"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="130" t="s">
         <v>523</v>
       </c>
@@ -32083,7 +32083,7 @@
       </c>
       <c r="N27" s="130"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="125" t="s">
         <v>417</v>
       </c>
@@ -32107,7 +32107,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="125" t="s">
         <v>417</v>
       </c>
@@ -32129,7 +32129,7 @@
       <c r="M29" s="128"/>
       <c r="N29" s="125"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="125" t="s">
         <v>417</v>
       </c>
@@ -32151,7 +32151,7 @@
       <c r="M30" s="128"/>
       <c r="N30" s="125"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="125" t="s">
         <v>417</v>
       </c>
@@ -32173,7 +32173,7 @@
       <c r="M31" s="128"/>
       <c r="N31" s="125"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="125" t="s">
         <v>417</v>
       </c>
@@ -32195,7 +32195,7 @@
       <c r="M32" s="128"/>
       <c r="N32" s="125"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="125" t="s">
         <v>417</v>
       </c>
@@ -32217,7 +32217,7 @@
       <c r="M33" s="128"/>
       <c r="N33" s="125"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="125" t="s">
         <v>417</v>
       </c>
@@ -32239,7 +32239,7 @@
       <c r="M34" s="128"/>
       <c r="N34" s="125"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="125" t="s">
         <v>417</v>
       </c>
@@ -32261,7 +32261,7 @@
       <c r="M35" s="128"/>
       <c r="N35" s="125"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="125" t="s">
         <v>417</v>
       </c>
@@ -32283,7 +32283,7 @@
       <c r="M36" s="128"/>
       <c r="N36" s="125"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="125" t="s">
         <v>417</v>
       </c>
@@ -32305,7 +32305,7 @@
       <c r="M37" s="128"/>
       <c r="N37" s="125"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="125" t="s">
         <v>417</v>
       </c>
@@ -32327,7 +32327,7 @@
       <c r="M38" s="128"/>
       <c r="N38" s="125"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="125" t="s">
         <v>417</v>
       </c>
@@ -32349,7 +32349,7 @@
       <c r="M39" s="128"/>
       <c r="N39" s="125"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="125" t="s">
         <v>417</v>
       </c>
@@ -32371,7 +32371,7 @@
       <c r="M40" s="128"/>
       <c r="N40" s="125"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="130" t="s">
         <v>523</v>
       </c>
@@ -32393,7 +32393,7 @@
       <c r="M41" s="132"/>
       <c r="N41" s="130"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="130" t="s">
         <v>523</v>
       </c>
@@ -32415,7 +32415,7 @@
       <c r="M42" s="132"/>
       <c r="N42" s="130"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="130" t="s">
         <v>523</v>
       </c>
@@ -32437,7 +32437,7 @@
       <c r="M43" s="132"/>
       <c r="N43" s="130"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="130" t="s">
         <v>523</v>
       </c>
@@ -32459,7 +32459,7 @@
       <c r="M44" s="132"/>
       <c r="N44" s="130"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="130" t="s">
         <v>523</v>
       </c>
@@ -32481,7 +32481,7 @@
       <c r="M45" s="132"/>
       <c r="N45" s="130"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="130" t="s">
         <v>523</v>
       </c>
@@ -32503,7 +32503,7 @@
       <c r="M46" s="132"/>
       <c r="N46" s="130"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="130" t="s">
         <v>523</v>
       </c>
@@ -32525,7 +32525,7 @@
       <c r="M47" s="132"/>
       <c r="N47" s="130"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="130" t="s">
         <v>523</v>
       </c>
@@ -32547,7 +32547,7 @@
       <c r="M48" s="132"/>
       <c r="N48" s="130"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="130" t="s">
         <v>523</v>
       </c>
@@ -32569,7 +32569,7 @@
       <c r="M49" s="132"/>
       <c r="N49" s="130"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="130" t="s">
         <v>523</v>
       </c>
@@ -32591,7 +32591,7 @@
       <c r="M50" s="132"/>
       <c r="N50" s="130"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="130" t="s">
         <v>523</v>
       </c>
@@ -32613,7 +32613,7 @@
       <c r="M51" s="132"/>
       <c r="N51" s="130"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="130" t="s">
         <v>523</v>
       </c>
@@ -32635,7 +32635,7 @@
       <c r="M52" s="132"/>
       <c r="N52" s="130"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="130" t="s">
         <v>523</v>
       </c>
@@ -32657,7 +32657,7 @@
       <c r="M53" s="132"/>
       <c r="N53" s="130"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="125" t="s">
         <v>417</v>
       </c>
@@ -32681,7 +32681,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="125" t="s">
         <v>417</v>
       </c>
@@ -32703,7 +32703,7 @@
       <c r="M55" s="128"/>
       <c r="N55" s="125"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="125" t="s">
         <v>417</v>
       </c>
@@ -32725,7 +32725,7 @@
       <c r="M56" s="128"/>
       <c r="N56" s="125"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="125" t="s">
         <v>417</v>
       </c>
@@ -32747,7 +32747,7 @@
       <c r="M57" s="128"/>
       <c r="N57" s="125"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="125" t="s">
         <v>417</v>
       </c>
@@ -32769,7 +32769,7 @@
       <c r="M58" s="128"/>
       <c r="N58" s="125"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="125" t="s">
         <v>417</v>
       </c>
@@ -32791,7 +32791,7 @@
       <c r="M59" s="128"/>
       <c r="N59" s="125"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="125" t="s">
         <v>417</v>
       </c>
@@ -32813,7 +32813,7 @@
       <c r="M60" s="128"/>
       <c r="N60" s="125"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="125" t="s">
         <v>417</v>
       </c>
@@ -32835,7 +32835,7 @@
       <c r="M61" s="128"/>
       <c r="N61" s="125"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="125" t="s">
         <v>417</v>
       </c>
@@ -32857,7 +32857,7 @@
       <c r="M62" s="128"/>
       <c r="N62" s="125"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="125" t="s">
         <v>417</v>
       </c>
@@ -32879,7 +32879,7 @@
       <c r="M63" s="128"/>
       <c r="N63" s="125"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="125" t="s">
         <v>417</v>
       </c>
@@ -32901,7 +32901,7 @@
       <c r="M64" s="128"/>
       <c r="N64" s="125"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="125" t="s">
         <v>417</v>
       </c>
@@ -32923,7 +32923,7 @@
       <c r="M65" s="128"/>
       <c r="N65" s="125"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="125" t="s">
         <v>417</v>
       </c>
@@ -32945,7 +32945,7 @@
       <c r="M66" s="128"/>
       <c r="N66" s="125"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="130" t="s">
         <v>523</v>
       </c>
@@ -32967,7 +32967,7 @@
       <c r="M67" s="132"/>
       <c r="N67" s="130"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="130" t="s">
         <v>523</v>
       </c>
@@ -32989,7 +32989,7 @@
       <c r="M68" s="132"/>
       <c r="N68" s="130"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="130" t="s">
         <v>523</v>
       </c>
@@ -33011,7 +33011,7 @@
       <c r="M69" s="132"/>
       <c r="N69" s="130"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="130" t="s">
         <v>523</v>
       </c>
@@ -33033,7 +33033,7 @@
       <c r="M70" s="132"/>
       <c r="N70" s="130"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="130" t="s">
         <v>523</v>
       </c>
@@ -33055,7 +33055,7 @@
       <c r="M71" s="132"/>
       <c r="N71" s="130"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="130" t="s">
         <v>523</v>
       </c>
@@ -33077,7 +33077,7 @@
       <c r="M72" s="132"/>
       <c r="N72" s="130"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="130" t="s">
         <v>523</v>
       </c>
@@ -33099,7 +33099,7 @@
       <c r="M73" s="132"/>
       <c r="N73" s="130"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="130" t="s">
         <v>523</v>
       </c>
@@ -33121,7 +33121,7 @@
       <c r="M74" s="132"/>
       <c r="N74" s="130"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="130" t="s">
         <v>523</v>
       </c>
@@ -33143,7 +33143,7 @@
       <c r="M75" s="132"/>
       <c r="N75" s="130"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="130" t="s">
         <v>523</v>
       </c>
@@ -33165,7 +33165,7 @@
       <c r="M76" s="132"/>
       <c r="N76" s="130"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="130" t="s">
         <v>523</v>
       </c>
@@ -33187,7 +33187,7 @@
       <c r="M77" s="132"/>
       <c r="N77" s="130"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="130" t="s">
         <v>523</v>
       </c>
@@ -33209,7 +33209,7 @@
       <c r="M78" s="132"/>
       <c r="N78" s="130"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="130" t="s">
         <v>523</v>
       </c>
@@ -33231,7 +33231,7 @@
       <c r="M79" s="132"/>
       <c r="N79" s="130"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="125" t="s">
         <v>417</v>
       </c>
@@ -33255,7 +33255,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="125" t="s">
         <v>417</v>
       </c>
@@ -33277,7 +33277,7 @@
       <c r="M81" s="128"/>
       <c r="N81" s="125"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="125" t="s">
         <v>417</v>
       </c>
@@ -33299,7 +33299,7 @@
       <c r="M82" s="128"/>
       <c r="N82" s="125"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="125" t="s">
         <v>417</v>
       </c>
@@ -33321,7 +33321,7 @@
       <c r="M83" s="128"/>
       <c r="N83" s="125"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="125" t="s">
         <v>417</v>
       </c>
@@ -33343,7 +33343,7 @@
       <c r="M84" s="128"/>
       <c r="N84" s="125"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="125" t="s">
         <v>417</v>
       </c>
@@ -33365,7 +33365,7 @@
       <c r="M85" s="128"/>
       <c r="N85" s="125"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="125" t="s">
         <v>417</v>
       </c>
@@ -33387,7 +33387,7 @@
       <c r="M86" s="128"/>
       <c r="N86" s="125"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="125" t="s">
         <v>417</v>
       </c>
@@ -33409,7 +33409,7 @@
       <c r="M87" s="128"/>
       <c r="N87" s="125"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="125" t="s">
         <v>417</v>
       </c>
@@ -33431,7 +33431,7 @@
       <c r="M88" s="128"/>
       <c r="N88" s="125"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="125" t="s">
         <v>417</v>
       </c>
@@ -33453,7 +33453,7 @@
       <c r="M89" s="128"/>
       <c r="N89" s="125"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="125" t="s">
         <v>417</v>
       </c>
@@ -33475,7 +33475,7 @@
       <c r="M90" s="128"/>
       <c r="N90" s="125"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="125" t="s">
         <v>417</v>
       </c>
@@ -33497,7 +33497,7 @@
       <c r="M91" s="128"/>
       <c r="N91" s="125"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="125" t="s">
         <v>417</v>
       </c>
@@ -33519,7 +33519,7 @@
       <c r="M92" s="128"/>
       <c r="N92" s="125"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="130" t="s">
         <v>523</v>
       </c>
@@ -33541,7 +33541,7 @@
       <c r="M93" s="132"/>
       <c r="N93" s="130"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="130" t="s">
         <v>523</v>
       </c>
@@ -33563,7 +33563,7 @@
       <c r="M94" s="132"/>
       <c r="N94" s="130"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="130" t="s">
         <v>523</v>
       </c>
@@ -33585,7 +33585,7 @@
       <c r="M95" s="132"/>
       <c r="N95" s="130"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="130" t="s">
         <v>523</v>
       </c>
@@ -33607,7 +33607,7 @@
       <c r="M96" s="132"/>
       <c r="N96" s="130"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="130" t="s">
         <v>523</v>
       </c>
@@ -33629,7 +33629,7 @@
       <c r="M97" s="132"/>
       <c r="N97" s="130"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="130" t="s">
         <v>523</v>
       </c>
@@ -33651,7 +33651,7 @@
       <c r="M98" s="132"/>
       <c r="N98" s="130"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="130" t="s">
         <v>523</v>
       </c>
@@ -33673,7 +33673,7 @@
       <c r="M99" s="132"/>
       <c r="N99" s="130"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="130" t="s">
         <v>523</v>
       </c>
@@ -33695,7 +33695,7 @@
       <c r="M100" s="132"/>
       <c r="N100" s="130"/>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="130" t="s">
         <v>523</v>
       </c>
@@ -33717,7 +33717,7 @@
       <c r="M101" s="132"/>
       <c r="N101" s="130"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="130" t="s">
         <v>523</v>
       </c>
@@ -33739,7 +33739,7 @@
       <c r="M102" s="132"/>
       <c r="N102" s="130"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="130" t="s">
         <v>523</v>
       </c>
@@ -33761,7 +33761,7 @@
       <c r="M103" s="132"/>
       <c r="N103" s="130"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="130" t="s">
         <v>523</v>
       </c>
@@ -33783,7 +33783,7 @@
       <c r="M104" s="132"/>
       <c r="N104" s="130"/>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="130" t="s">
         <v>523</v>
       </c>

</xml_diff>

<commit_message>
Final changes to PK data for Piperacillin and Tazobactam (EC50 for Piperacillin still to be investigated).  PK Validation scenario as well as validation data for each compound have been uploaded.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4938" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4938" uniqueCount="780">
   <si>
     <t>Name</t>
   </si>
@@ -2302,9 +2302,6 @@
     <t>Hayashi2010Pharmacokinetic</t>
   </si>
   <si>
-    <t>1.98 mL/min kg</t>
-  </si>
-  <si>
     <t>Wise1991Pharmacokinetics</t>
   </si>
   <si>
@@ -2317,18 +2314,9 @@
     <t>Between 70% and 80% unbound</t>
   </si>
   <si>
-    <t>1.04 mL/min kg</t>
-  </si>
-  <si>
-    <t>1.83 mL/min kg</t>
-  </si>
-  <si>
     <t>When given with PIP (significant difference if alone)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1.0 mL/min kg</t>
-  </si>
-  <si>
     <t>Hyatt1995InVitro</t>
   </si>
   <si>
@@ -2363,6 +2351,30 @@
   </si>
   <si>
     <t>0.0268 g/mL</t>
+  </si>
+  <si>
+    <t>0.022 mL/min kg</t>
+  </si>
+  <si>
+    <t>1.27 mL/min kg</t>
+  </si>
+  <si>
+    <t>3.64 mL/min kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.27 mL/min kg</t>
+  </si>
+  <si>
+    <t>0.006 mL/min kg</t>
+  </si>
+  <si>
+    <t>1.69 mL/min kg</t>
+  </si>
+  <si>
+    <t>2.57 mL/min kg</t>
+  </si>
+  <si>
+    <t>2.0 ug/mL</t>
   </si>
 </sst>
 </file>
@@ -4856,10 +4868,10 @@
   <dimension ref="A1:FV78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="DN51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="DF26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="EN74" sqref="EN74"/>
+      <selection pane="bottomRight" activeCell="DJ47" sqref="DJ47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -10132,7 +10144,7 @@
         <v>754</v>
       </c>
       <c r="DM19" s="115" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="DN19" s="115">
         <v>1</v>
@@ -10178,7 +10190,7 @@
         <v>754</v>
       </c>
       <c r="EO19" s="115" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="EP19" s="115">
         <v>0.99</v>
@@ -10363,7 +10375,7 @@
       <c r="DH20" s="115"/>
       <c r="DI20" s="115"/>
       <c r="DJ20" s="115" t="s">
-        <v>340</v>
+        <v>772</v>
       </c>
       <c r="DK20" s="115"/>
       <c r="DL20" s="115"/>
@@ -10405,7 +10417,7 @@
       <c r="EJ20" s="115"/>
       <c r="EK20" s="115"/>
       <c r="EL20" s="115" t="s">
-        <v>340</v>
+        <v>776</v>
       </c>
       <c r="EM20" s="115"/>
       <c r="EN20" s="115"/>
@@ -10593,14 +10605,14 @@
       <c r="DH21" s="115"/>
       <c r="DI21" s="115"/>
       <c r="DJ21" s="115" t="s">
-        <v>611</v>
+        <v>773</v>
       </c>
       <c r="DK21" s="115"/>
       <c r="DL21" s="115" t="s">
+        <v>755</v>
+      </c>
+      <c r="DM21" s="115" t="s">
         <v>756</v>
-      </c>
-      <c r="DM21" s="115" t="s">
-        <v>757</v>
       </c>
       <c r="DN21" s="115" t="s">
         <v>127</v>
@@ -10639,14 +10651,14 @@
       <c r="EJ21" s="115"/>
       <c r="EK21" s="115"/>
       <c r="EL21" s="115" t="s">
-        <v>760</v>
+        <v>777</v>
       </c>
       <c r="EM21" s="115"/>
       <c r="EN21" s="115" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="EO21" s="115" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="EP21" s="115" t="s">
         <v>736</v>
@@ -10845,14 +10857,14 @@
       </c>
       <c r="DI22" s="115"/>
       <c r="DJ22" s="115" t="s">
-        <v>755</v>
+        <v>774</v>
       </c>
       <c r="DK22" s="115"/>
       <c r="DL22" s="115" t="s">
+        <v>755</v>
+      </c>
+      <c r="DM22" s="115" t="s">
         <v>756</v>
-      </c>
-      <c r="DM22" s="115" t="s">
-        <v>757</v>
       </c>
       <c r="DN22" s="115" t="s">
         <v>262</v>
@@ -10891,14 +10903,14 @@
       <c r="EJ22" s="115"/>
       <c r="EK22" s="115"/>
       <c r="EL22" s="115" t="s">
-        <v>761</v>
+        <v>778</v>
       </c>
       <c r="EM22" s="115"/>
       <c r="EN22" s="115" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="EO22" s="115" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="EP22" s="115" t="s">
         <v>737</v>
@@ -11564,14 +11576,14 @@
       <c r="DH24" s="115"/>
       <c r="DI24" s="115"/>
       <c r="DJ24" s="115" t="s">
-        <v>763</v>
+        <v>775</v>
       </c>
       <c r="DK24" s="115"/>
       <c r="DL24" s="115" t="s">
+        <v>755</v>
+      </c>
+      <c r="DM24" s="115" t="s">
         <v>756</v>
-      </c>
-      <c r="DM24" s="115" t="s">
-        <v>757</v>
       </c>
       <c r="DN24" s="115" t="str">
         <f t="shared" si="0"/>
@@ -11651,14 +11663,14 @@
       <c r="EJ24" s="115"/>
       <c r="EK24" s="115"/>
       <c r="EL24" s="115" t="s">
-        <v>760</v>
+        <v>777</v>
       </c>
       <c r="EM24" s="115"/>
       <c r="EN24" s="115" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="EO24" s="115" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="EP24" s="115" t="s">
         <v>736</v>
@@ -15781,14 +15793,14 @@
         <v>747</v>
       </c>
       <c r="DJ40" s="119" t="s">
-        <v>691</v>
+        <v>779</v>
       </c>
       <c r="DK40" s="119"/>
       <c r="DL40" s="119" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="DM40" s="119" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="DN40" s="119" t="s">
         <v>377</v>
@@ -16003,7 +16015,7 @@
       <c r="DH41" s="119"/>
       <c r="DI41" s="119"/>
       <c r="DJ41" s="119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DK41" s="119"/>
       <c r="DL41" s="119"/>
@@ -19754,7 +19766,7 @@
         <v>754</v>
       </c>
       <c r="DM56" s="117" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="DN56" s="76"/>
       <c r="DO56" s="117"/>
@@ -19790,7 +19802,7 @@
         <v>754</v>
       </c>
       <c r="EO56" s="117" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="EP56" s="117"/>
       <c r="EQ56" s="117"/>
@@ -20986,7 +20998,7 @@
         <v>754</v>
       </c>
       <c r="DM60" s="117" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="DN60" s="76"/>
       <c r="DO60" s="117"/>
@@ -21022,7 +21034,7 @@
         <v>754</v>
       </c>
       <c r="EO60" s="117" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="EP60" s="117"/>
       <c r="EQ60" s="117"/>
@@ -21604,7 +21616,7 @@
         <v>754</v>
       </c>
       <c r="DM62" s="117" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="DN62" s="76"/>
       <c r="DO62" s="117"/>
@@ -21640,7 +21652,7 @@
         <v>754</v>
       </c>
       <c r="EO62" s="117" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="EP62" s="117"/>
       <c r="EQ62" s="117"/>
@@ -22256,7 +22268,7 @@
         <v>754</v>
       </c>
       <c r="EO64" s="117" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="EP64" s="117"/>
       <c r="EQ64" s="117"/>
@@ -22838,7 +22850,7 @@
         <v>754</v>
       </c>
       <c r="DM66" s="117" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="DN66" s="76"/>
       <c r="DO66" s="117"/>
@@ -22874,7 +22886,7 @@
         <v>754</v>
       </c>
       <c r="EO66" s="117" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="EP66" s="117"/>
       <c r="EQ66" s="117"/>
@@ -24070,7 +24082,7 @@
         <v>754</v>
       </c>
       <c r="DM70" s="117" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="DN70" s="76"/>
       <c r="DO70" s="117"/>
@@ -24106,7 +24118,7 @@
         <v>754</v>
       </c>
       <c r="EO70" s="117" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="EP70" s="117"/>
       <c r="EQ70" s="117"/>
@@ -24688,7 +24700,7 @@
         <v>754</v>
       </c>
       <c r="DM72" s="117" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="DN72" s="76"/>
       <c r="DO72" s="117"/>
@@ -24724,7 +24736,7 @@
         <v>754</v>
       </c>
       <c r="EO72" s="117" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="EP72" s="117"/>
       <c r="EQ72" s="117"/>
@@ -25340,7 +25352,7 @@
         <v>754</v>
       </c>
       <c r="EO74" s="117" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="EP74" s="117"/>
       <c r="EQ74" s="117"/>
@@ -26570,7 +26582,7 @@
         <v>754</v>
       </c>
       <c r="EO78" s="117" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="EP78" s="117"/>
       <c r="EQ78" s="117"/>
@@ -26667,7 +26679,7 @@
         <v>697</v>
       </c>
       <c r="E3" s="78" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -26714,7 +26726,7 @@
         <v>698</v>
       </c>
       <c r="E6" s="80" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -26761,7 +26773,7 @@
         <v>699</v>
       </c>
       <c r="E9" s="80" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -26804,7 +26816,7 @@
         <v>700</v>
       </c>
       <c r="E12" s="80" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update to xlsx to include hyperhidrosis and max work rate
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\remotes\sed-stash\biogears\core\share\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntatum\BioGearsCMake\core\share\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4863" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4865" uniqueCount="722">
   <si>
     <t>Name</t>
   </si>
@@ -2194,6 +2194,12 @@
   </si>
   <si>
     <t>2.0 ug/mL</t>
+  </si>
+  <si>
+    <t>MaxWorkRate</t>
+  </si>
+  <si>
+    <t>Hyperhidrosis</t>
   </si>
 </sst>
 </file>
@@ -2742,7 +2748,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3235,6 +3241,12 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent2" xfId="7" builtinId="34"/>
@@ -3553,13 +3565,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4460,83 +4472,83 @@
       <c r="U20" s="151"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="134" t="s">
-        <v>527</v>
-      </c>
-      <c r="B21" s="146"/>
-      <c r="C21" s="140"/>
-      <c r="D21" s="140"/>
-      <c r="E21" s="147"/>
-      <c r="F21" s="146"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="140"/>
-      <c r="I21" s="147"/>
-      <c r="J21" s="146"/>
-      <c r="K21" s="140"/>
-      <c r="L21" s="140"/>
-      <c r="M21" s="140"/>
-      <c r="N21" s="140"/>
-      <c r="O21" s="140"/>
-      <c r="P21" s="140"/>
-      <c r="Q21" s="140"/>
-      <c r="R21" s="140"/>
-      <c r="S21" s="147"/>
-      <c r="T21" s="146"/>
-      <c r="U21" s="147"/>
+      <c r="A21" s="143" t="s">
+        <v>720</v>
+      </c>
+      <c r="B21" s="150"/>
+      <c r="C21" s="198"/>
+      <c r="D21" s="198"/>
+      <c r="E21" s="199"/>
+      <c r="F21" s="150"/>
+      <c r="G21" s="198"/>
+      <c r="H21" s="198"/>
+      <c r="I21" s="199"/>
+      <c r="J21" s="150"/>
+      <c r="K21" s="198"/>
+      <c r="L21" s="198"/>
+      <c r="M21" s="198"/>
+      <c r="N21" s="198"/>
+      <c r="O21" s="198"/>
+      <c r="P21" s="198"/>
+      <c r="Q21" s="198"/>
+      <c r="R21" s="198"/>
+      <c r="S21" s="199"/>
+      <c r="T21" s="150"/>
+      <c r="U21" s="199"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="143" t="s">
-        <v>492</v>
+        <v>721</v>
       </c>
       <c r="B22" s="150"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="151"/>
+      <c r="C22" s="198"/>
+      <c r="D22" s="198"/>
+      <c r="E22" s="199"/>
       <c r="F22" s="150"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="138"/>
-      <c r="I22" s="151"/>
+      <c r="G22" s="198"/>
+      <c r="H22" s="198"/>
+      <c r="I22" s="199"/>
       <c r="J22" s="150"/>
-      <c r="K22" s="138"/>
-      <c r="L22" s="138"/>
-      <c r="M22" s="138"/>
-      <c r="N22" s="138"/>
-      <c r="O22" s="138"/>
-      <c r="P22" s="138"/>
-      <c r="Q22" s="138"/>
-      <c r="R22" s="138"/>
-      <c r="S22" s="151"/>
+      <c r="K22" s="198"/>
+      <c r="L22" s="198"/>
+      <c r="M22" s="198"/>
+      <c r="N22" s="198"/>
+      <c r="O22" s="198"/>
+      <c r="P22" s="198"/>
+      <c r="Q22" s="198"/>
+      <c r="R22" s="198"/>
+      <c r="S22" s="199"/>
       <c r="T22" s="150"/>
-      <c r="U22" s="151"/>
+      <c r="U22" s="199"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="143" t="s">
-        <v>493</v>
-      </c>
-      <c r="B23" s="150"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="138"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="150"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="138"/>
-      <c r="I23" s="151"/>
-      <c r="J23" s="150"/>
-      <c r="K23" s="138"/>
-      <c r="L23" s="138"/>
-      <c r="M23" s="138"/>
-      <c r="N23" s="138"/>
-      <c r="O23" s="138"/>
-      <c r="P23" s="138"/>
-      <c r="Q23" s="138"/>
-      <c r="R23" s="138"/>
-      <c r="S23" s="151"/>
-      <c r="T23" s="150"/>
-      <c r="U23" s="151"/>
+      <c r="A23" s="134" t="s">
+        <v>527</v>
+      </c>
+      <c r="B23" s="146"/>
+      <c r="C23" s="140"/>
+      <c r="D23" s="140"/>
+      <c r="E23" s="147"/>
+      <c r="F23" s="146"/>
+      <c r="G23" s="140"/>
+      <c r="H23" s="140"/>
+      <c r="I23" s="147"/>
+      <c r="J23" s="146"/>
+      <c r="K23" s="140"/>
+      <c r="L23" s="140"/>
+      <c r="M23" s="140"/>
+      <c r="N23" s="140"/>
+      <c r="O23" s="140"/>
+      <c r="P23" s="140"/>
+      <c r="Q23" s="140"/>
+      <c r="R23" s="140"/>
+      <c r="S23" s="147"/>
+      <c r="T23" s="146"/>
+      <c r="U23" s="147"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="143" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B24" s="150"/>
       <c r="C24" s="138"/>
@@ -4561,7 +4573,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="143" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B25" s="150"/>
       <c r="C25" s="138"/>
@@ -4586,7 +4598,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="143" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B26" s="150"/>
       <c r="C26" s="138"/>
@@ -4608,6 +4620,56 @@
       <c r="S26" s="151"/>
       <c r="T26" s="150"/>
       <c r="U26" s="151"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="143" t="s">
+        <v>496</v>
+      </c>
+      <c r="B27" s="150"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="150"/>
+      <c r="G27" s="138"/>
+      <c r="H27" s="138"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="150"/>
+      <c r="K27" s="138"/>
+      <c r="L27" s="138"/>
+      <c r="M27" s="138"/>
+      <c r="N27" s="138"/>
+      <c r="O27" s="138"/>
+      <c r="P27" s="138"/>
+      <c r="Q27" s="138"/>
+      <c r="R27" s="138"/>
+      <c r="S27" s="151"/>
+      <c r="T27" s="150"/>
+      <c r="U27" s="151"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="143" t="s">
+        <v>494</v>
+      </c>
+      <c r="B28" s="150"/>
+      <c r="C28" s="138"/>
+      <c r="D28" s="138"/>
+      <c r="E28" s="151"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="138"/>
+      <c r="H28" s="138"/>
+      <c r="I28" s="151"/>
+      <c r="J28" s="150"/>
+      <c r="K28" s="138"/>
+      <c r="L28" s="138"/>
+      <c r="M28" s="138"/>
+      <c r="N28" s="138"/>
+      <c r="O28" s="138"/>
+      <c r="P28" s="138"/>
+      <c r="Q28" s="138"/>
+      <c r="R28" s="138"/>
+      <c r="S28" s="151"/>
+      <c r="T28" s="150"/>
+      <c r="U28" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -31205,7 +31267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates to xlsx to include pain susceptibility and include missing patient files
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4865" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4894" uniqueCount="733">
   <si>
     <t>Name</t>
   </si>
@@ -1677,9 +1677,6 @@
     <t>ChronicPericardialEffusion</t>
   </si>
   <si>
-    <t>110 bpm</t>
-  </si>
-  <si>
     <t>0.46 1/atm</t>
   </si>
   <si>
@@ -2200,6 +2197,42 @@
   </si>
   <si>
     <t>Hyperhidrosis</t>
+  </si>
+  <si>
+    <t>PainSusceptibility</t>
+  </si>
+  <si>
+    <t>Toughs</t>
+  </si>
+  <si>
+    <t>13 bpm</t>
+  </si>
+  <si>
+    <t>109 bpm</t>
+  </si>
+  <si>
+    <t>Tristan</t>
+  </si>
+  <si>
+    <t>24 yr</t>
+  </si>
+  <si>
+    <t>67 kg</t>
+  </si>
+  <si>
+    <t>172 cm</t>
+  </si>
+  <si>
+    <t>315 W</t>
+  </si>
+  <si>
+    <t>ToughGirl</t>
+  </si>
+  <si>
+    <t>ToughGuy</t>
+  </si>
+  <si>
+    <t>65 in</t>
   </si>
 </sst>
 </file>
@@ -2748,7 +2781,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3232,6 +3265,12 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3241,10 +3280,22 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3565,13 +3616,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,44 +3642,52 @@
     <col min="13" max="13" width="10.7109375" style="139" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" style="139" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="139" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="10.7109375" style="139" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" style="139" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" style="139" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="139"/>
+    <col min="16" max="18" width="10.7109375" style="139" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" style="139" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="139" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" style="139" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" style="139" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="15.140625" style="139" customWidth="1"/>
+    <col min="25" max="16384" width="8.85546875" style="139"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="134"/>
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="197" t="s">
         <v>518</v>
       </c>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="197"/>
-      <c r="F1" s="195" t="s">
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="197" t="s">
         <v>515</v>
       </c>
-      <c r="G1" s="196"/>
-      <c r="H1" s="196"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="195" t="s">
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="197" t="s">
         <v>516</v>
       </c>
-      <c r="K1" s="196"/>
-      <c r="L1" s="196"/>
-      <c r="M1" s="196"/>
-      <c r="N1" s="196"/>
-      <c r="O1" s="196"/>
-      <c r="P1" s="196"/>
-      <c r="Q1" s="196"/>
-      <c r="R1" s="196"/>
-      <c r="S1" s="197"/>
-      <c r="T1" s="195" t="s">
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
+      <c r="M1" s="198"/>
+      <c r="N1" s="198"/>
+      <c r="O1" s="198"/>
+      <c r="P1" s="198"/>
+      <c r="Q1" s="198"/>
+      <c r="R1" s="198"/>
+      <c r="S1" s="198"/>
+      <c r="T1" s="199"/>
+      <c r="U1" s="197" t="s">
         <v>517</v>
       </c>
-      <c r="U1" s="197"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="199"/>
+      <c r="W1" s="197" t="s">
+        <v>722</v>
+      </c>
+      <c r="X1" s="199"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="135" t="s">
         <v>0</v>
       </c>
@@ -3683,17 +3742,26 @@
       <c r="R2" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="S2" s="145" t="s">
+      <c r="S2" s="200" t="s">
+        <v>725</v>
+      </c>
+      <c r="T2" s="145" t="s">
         <v>247</v>
       </c>
-      <c r="T2" s="144" t="s">
+      <c r="U2" s="144" t="s">
         <v>509</v>
       </c>
-      <c r="U2" s="145" t="s">
+      <c r="V2" s="145" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W2" s="144" t="s">
+        <v>730</v>
+      </c>
+      <c r="X2" s="145" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="134" t="s">
         <v>497</v>
       </c>
@@ -3714,11 +3782,14 @@
       <c r="P3" s="141"/>
       <c r="Q3" s="141"/>
       <c r="R3" s="141"/>
-      <c r="S3" s="153"/>
-      <c r="T3" s="152"/>
-      <c r="U3" s="153"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S3" s="201"/>
+      <c r="T3" s="153"/>
+      <c r="U3" s="152"/>
+      <c r="V3" s="153"/>
+      <c r="W3" s="152"/>
+      <c r="X3" s="153"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="142" t="s">
         <v>345</v>
       </c>
@@ -3773,17 +3844,26 @@
       <c r="R4" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="149" t="s">
+      <c r="S4" s="202" t="s">
+        <v>9</v>
+      </c>
+      <c r="T4" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="T4" s="148" t="s">
+      <c r="U4" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="U4" s="149" t="s">
+      <c r="V4" s="149" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W4" s="148" t="s">
+        <v>30</v>
+      </c>
+      <c r="X4" s="149" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="134" t="s">
         <v>525</v>
       </c>
@@ -3804,11 +3884,14 @@
       <c r="P5" s="140"/>
       <c r="Q5" s="140"/>
       <c r="R5" s="140"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="146"/>
-      <c r="U5" s="147"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S5" s="203"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="146"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="146"/>
+      <c r="X5" s="147"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="143" t="s">
         <v>5</v>
       </c>
@@ -3859,17 +3942,26 @@
       <c r="R6" s="138" t="s">
         <v>244</v>
       </c>
-      <c r="S6" s="151" t="s">
+      <c r="S6" s="204" t="s">
+        <v>726</v>
+      </c>
+      <c r="T6" s="151" t="s">
         <v>501</v>
       </c>
-      <c r="T6" s="150" t="s">
+      <c r="U6" s="150" t="s">
         <v>501</v>
       </c>
-      <c r="U6" s="151" t="s">
+      <c r="V6" s="151" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W6" s="150">
+        <v>44</v>
+      </c>
+      <c r="X6" s="151" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="143" t="s">
         <v>6</v>
       </c>
@@ -3920,13 +4012,22 @@
       <c r="R7" s="138" t="s">
         <v>245</v>
       </c>
-      <c r="S7" s="151" t="s">
+      <c r="S7" s="204" t="s">
+        <v>727</v>
+      </c>
+      <c r="T7" s="151" t="s">
         <v>248</v>
       </c>
-      <c r="T7" s="150"/>
-      <c r="U7" s="151"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U7" s="150"/>
+      <c r="V7" s="151"/>
+      <c r="W7" s="150" t="s">
+        <v>21</v>
+      </c>
+      <c r="X7" s="151" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="143" t="s">
         <v>7</v>
       </c>
@@ -3977,17 +4078,26 @@
       <c r="R8" s="138" t="s">
         <v>246</v>
       </c>
-      <c r="S8" s="151" t="s">
+      <c r="S8" s="204" t="s">
+        <v>728</v>
+      </c>
+      <c r="T8" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="T8" s="150" t="s">
+      <c r="U8" s="150" t="s">
         <v>513</v>
       </c>
-      <c r="U8" s="151" t="s">
+      <c r="V8" s="151" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W8" s="150" t="s">
+        <v>732</v>
+      </c>
+      <c r="X8" s="151" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="143" t="s">
         <v>163</v>
       </c>
@@ -4038,17 +4148,26 @@
       <c r="R9" s="138">
         <v>0.25</v>
       </c>
-      <c r="S9" s="151">
+      <c r="S9" s="204">
+        <v>0.21</v>
+      </c>
+      <c r="T9" s="151">
         <v>0.18</v>
       </c>
-      <c r="T9" s="150">
+      <c r="U9" s="150">
         <v>0.32</v>
       </c>
-      <c r="U9" s="151">
+      <c r="V9" s="151">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W9" s="150">
+        <v>0.21</v>
+      </c>
+      <c r="X9" s="151">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="134" t="s">
         <v>526</v>
       </c>
@@ -4069,11 +4188,14 @@
       <c r="P10" s="140"/>
       <c r="Q10" s="140"/>
       <c r="R10" s="140"/>
-      <c r="S10" s="147"/>
-      <c r="T10" s="146"/>
-      <c r="U10" s="147"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S10" s="203"/>
+      <c r="T10" s="147"/>
+      <c r="U10" s="146"/>
+      <c r="V10" s="147"/>
+      <c r="W10" s="146"/>
+      <c r="X10" s="147"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="143" t="s">
         <v>524</v>
       </c>
@@ -4094,11 +4216,14 @@
       <c r="P11" s="138"/>
       <c r="Q11" s="138"/>
       <c r="R11" s="138"/>
-      <c r="S11" s="151"/>
-      <c r="T11" s="150"/>
-      <c r="U11" s="151"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S11" s="204"/>
+      <c r="T11" s="151"/>
+      <c r="U11" s="150"/>
+      <c r="V11" s="151"/>
+      <c r="W11" s="150"/>
+      <c r="X11" s="151"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="143" t="s">
         <v>490</v>
       </c>
@@ -4119,11 +4244,14 @@
       <c r="P12" s="138"/>
       <c r="Q12" s="138"/>
       <c r="R12" s="138"/>
-      <c r="S12" s="151"/>
-      <c r="T12" s="150"/>
-      <c r="U12" s="151"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S12" s="204"/>
+      <c r="T12" s="151"/>
+      <c r="U12" s="150"/>
+      <c r="V12" s="151"/>
+      <c r="W12" s="150"/>
+      <c r="X12" s="151"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="143" t="s">
         <v>61</v>
       </c>
@@ -4142,7 +4270,7 @@
         <v>22</v>
       </c>
       <c r="H13" s="138" t="s">
-        <v>548</v>
+        <v>724</v>
       </c>
       <c r="I13" s="151" t="s">
         <v>546</v>
@@ -4154,7 +4282,7 @@
         <v>41</v>
       </c>
       <c r="L13" s="138" t="s">
-        <v>548</v>
+        <v>724</v>
       </c>
       <c r="M13" s="138" t="s">
         <v>22</v>
@@ -4163,7 +4291,7 @@
         <v>506</v>
       </c>
       <c r="O13" s="138" t="s">
-        <v>548</v>
+        <v>724</v>
       </c>
       <c r="P13" s="138" t="s">
         <v>67</v>
@@ -4174,17 +4302,26 @@
       <c r="R13" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="S13" s="151" t="s">
+      <c r="S13" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="150" t="s">
+      <c r="T13" s="151" t="s">
+        <v>22</v>
+      </c>
+      <c r="U13" s="150" t="s">
         <v>511</v>
       </c>
-      <c r="U13" s="151" t="s">
+      <c r="V13" s="151" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W13" s="150" t="s">
+        <v>22</v>
+      </c>
+      <c r="X13" s="151" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="143" t="s">
         <v>486</v>
       </c>
@@ -4235,17 +4372,26 @@
       <c r="R14" s="138" t="s">
         <v>488</v>
       </c>
-      <c r="S14" s="151" t="s">
+      <c r="S14" s="204" t="s">
         <v>488</v>
       </c>
-      <c r="T14" s="150" t="s">
+      <c r="T14" s="151" t="s">
+        <v>488</v>
+      </c>
+      <c r="U14" s="150" t="s">
         <v>502</v>
       </c>
-      <c r="U14" s="151" t="s">
+      <c r="V14" s="151" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W14" s="150" t="s">
+        <v>488</v>
+      </c>
+      <c r="X14" s="151" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="143" t="s">
         <v>487</v>
       </c>
@@ -4296,17 +4442,26 @@
       <c r="R15" s="138" t="s">
         <v>489</v>
       </c>
-      <c r="S15" s="151" t="s">
+      <c r="S15" s="204" t="s">
         <v>489</v>
       </c>
-      <c r="T15" s="150" t="s">
+      <c r="T15" s="151" t="s">
+        <v>489</v>
+      </c>
+      <c r="U15" s="150" t="s">
         <v>503</v>
       </c>
-      <c r="U15" s="151" t="s">
+      <c r="V15" s="151" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W15" s="150" t="s">
+        <v>489</v>
+      </c>
+      <c r="X15" s="151" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="143" t="s">
         <v>63</v>
       </c>
@@ -4357,17 +4512,26 @@
       <c r="R16" s="138" t="s">
         <v>69</v>
       </c>
-      <c r="S16" s="151" t="s">
+      <c r="S16" s="204" t="s">
+        <v>218</v>
+      </c>
+      <c r="T16" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="T16" s="150" t="s">
-        <v>222</v>
-      </c>
-      <c r="U16" s="151" t="s">
+      <c r="U16" s="150" t="s">
+        <v>723</v>
+      </c>
+      <c r="V16" s="151" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="W16" s="150" t="s">
+        <v>218</v>
+      </c>
+      <c r="X16" s="151" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="154" t="s">
         <v>528</v>
       </c>
@@ -4388,11 +4552,14 @@
       <c r="P17" s="140"/>
       <c r="Q17" s="140"/>
       <c r="R17" s="140"/>
-      <c r="S17" s="147"/>
-      <c r="T17" s="146"/>
-      <c r="U17" s="147"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S17" s="203"/>
+      <c r="T17" s="147"/>
+      <c r="U17" s="146"/>
+      <c r="V17" s="147"/>
+      <c r="W17" s="146"/>
+      <c r="X17" s="147"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="143" t="s">
         <v>519</v>
       </c>
@@ -4413,11 +4580,14 @@
       <c r="P18" s="138"/>
       <c r="Q18" s="138"/>
       <c r="R18" s="138"/>
-      <c r="S18" s="151"/>
-      <c r="T18" s="150"/>
-      <c r="U18" s="151"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S18" s="204"/>
+      <c r="T18" s="151"/>
+      <c r="U18" s="150"/>
+      <c r="V18" s="151"/>
+      <c r="W18" s="150"/>
+      <c r="X18" s="151"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="143" t="s">
         <v>8</v>
       </c>
@@ -4438,15 +4608,18 @@
       <c r="P19" s="138"/>
       <c r="Q19" s="138"/>
       <c r="R19" s="138"/>
-      <c r="S19" s="151"/>
-      <c r="T19" s="150">
+      <c r="S19" s="204"/>
+      <c r="T19" s="151"/>
+      <c r="U19" s="150">
         <v>0.5</v>
       </c>
-      <c r="U19" s="151">
+      <c r="V19" s="151">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W19" s="150"/>
+      <c r="X19" s="151"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="143" t="s">
         <v>495</v>
       </c>
@@ -4467,113 +4640,136 @@
       <c r="P20" s="138"/>
       <c r="Q20" s="138"/>
       <c r="R20" s="138"/>
-      <c r="S20" s="151"/>
-      <c r="T20" s="150"/>
-      <c r="U20" s="151"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S20" s="204"/>
+      <c r="T20" s="151"/>
+      <c r="U20" s="150"/>
+      <c r="V20" s="151"/>
+      <c r="W20" s="150"/>
+      <c r="X20" s="151"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="143" t="s">
+        <v>719</v>
+      </c>
+      <c r="B21" s="150"/>
+      <c r="C21" s="195"/>
+      <c r="D21" s="195"/>
+      <c r="E21" s="196"/>
+      <c r="F21" s="150"/>
+      <c r="G21" s="195"/>
+      <c r="H21" s="195"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="150"/>
+      <c r="K21" s="195"/>
+      <c r="L21" s="195"/>
+      <c r="M21" s="195"/>
+      <c r="N21" s="195"/>
+      <c r="O21" s="195"/>
+      <c r="P21" s="195"/>
+      <c r="Q21" s="195"/>
+      <c r="R21" s="195"/>
+      <c r="S21" s="205" t="s">
+        <v>729</v>
+      </c>
+      <c r="T21" s="196"/>
+      <c r="U21" s="150"/>
+      <c r="V21" s="196"/>
+      <c r="W21" s="150"/>
+      <c r="X21" s="196"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="143" t="s">
         <v>720</v>
       </c>
-      <c r="B21" s="150"/>
-      <c r="C21" s="198"/>
-      <c r="D21" s="198"/>
-      <c r="E21" s="199"/>
-      <c r="F21" s="150"/>
-      <c r="G21" s="198"/>
-      <c r="H21" s="198"/>
-      <c r="I21" s="199"/>
-      <c r="J21" s="150"/>
-      <c r="K21" s="198"/>
-      <c r="L21" s="198"/>
-      <c r="M21" s="198"/>
-      <c r="N21" s="198"/>
-      <c r="O21" s="198"/>
-      <c r="P21" s="198"/>
-      <c r="Q21" s="198"/>
-      <c r="R21" s="198"/>
-      <c r="S21" s="199"/>
-      <c r="T21" s="150"/>
-      <c r="U21" s="199"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="143" t="s">
+      <c r="B22" s="150"/>
+      <c r="C22" s="195"/>
+      <c r="D22" s="195"/>
+      <c r="E22" s="196"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="195"/>
+      <c r="H22" s="195"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="150"/>
+      <c r="K22" s="195"/>
+      <c r="L22" s="195"/>
+      <c r="M22" s="195"/>
+      <c r="N22" s="195"/>
+      <c r="O22" s="195"/>
+      <c r="P22" s="195"/>
+      <c r="Q22" s="195"/>
+      <c r="R22" s="195"/>
+      <c r="S22" s="205">
+        <v>0.2</v>
+      </c>
+      <c r="T22" s="196"/>
+      <c r="U22" s="150"/>
+      <c r="V22" s="196"/>
+      <c r="W22" s="150"/>
+      <c r="X22" s="196"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="143" t="s">
         <v>721</v>
       </c>
-      <c r="B22" s="150"/>
-      <c r="C22" s="198"/>
-      <c r="D22" s="198"/>
-      <c r="E22" s="199"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="198"/>
-      <c r="H22" s="198"/>
-      <c r="I22" s="199"/>
-      <c r="J22" s="150"/>
-      <c r="K22" s="198"/>
-      <c r="L22" s="198"/>
-      <c r="M22" s="198"/>
-      <c r="N22" s="198"/>
-      <c r="O22" s="198"/>
-      <c r="P22" s="198"/>
-      <c r="Q22" s="198"/>
-      <c r="R22" s="198"/>
-      <c r="S22" s="199"/>
-      <c r="T22" s="150"/>
-      <c r="U22" s="199"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="134" t="s">
+      <c r="B23" s="150"/>
+      <c r="C23" s="195"/>
+      <c r="D23" s="195"/>
+      <c r="E23" s="196"/>
+      <c r="F23" s="150"/>
+      <c r="G23" s="195"/>
+      <c r="H23" s="195"/>
+      <c r="I23" s="196"/>
+      <c r="J23" s="150"/>
+      <c r="K23" s="195"/>
+      <c r="L23" s="195"/>
+      <c r="M23" s="195"/>
+      <c r="N23" s="195"/>
+      <c r="O23" s="195"/>
+      <c r="P23" s="195"/>
+      <c r="Q23" s="195"/>
+      <c r="R23" s="195"/>
+      <c r="S23" s="205"/>
+      <c r="T23" s="196"/>
+      <c r="U23" s="150"/>
+      <c r="V23" s="196"/>
+      <c r="W23" s="150">
+        <v>-0.5</v>
+      </c>
+      <c r="X23" s="196">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="134" t="s">
         <v>527</v>
       </c>
-      <c r="B23" s="146"/>
-      <c r="C23" s="140"/>
-      <c r="D23" s="140"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="146"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="147"/>
-      <c r="J23" s="146"/>
-      <c r="K23" s="140"/>
-      <c r="L23" s="140"/>
-      <c r="M23" s="140"/>
-      <c r="N23" s="140"/>
-      <c r="O23" s="140"/>
-      <c r="P23" s="140"/>
-      <c r="Q23" s="140"/>
-      <c r="R23" s="140"/>
-      <c r="S23" s="147"/>
-      <c r="T23" s="146"/>
-      <c r="U23" s="147"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="143" t="s">
+      <c r="B24" s="146"/>
+      <c r="C24" s="140"/>
+      <c r="D24" s="140"/>
+      <c r="E24" s="147"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="140"/>
+      <c r="H24" s="140"/>
+      <c r="I24" s="147"/>
+      <c r="J24" s="146"/>
+      <c r="K24" s="140"/>
+      <c r="L24" s="140"/>
+      <c r="M24" s="140"/>
+      <c r="N24" s="140"/>
+      <c r="O24" s="140"/>
+      <c r="P24" s="140"/>
+      <c r="Q24" s="140"/>
+      <c r="R24" s="140"/>
+      <c r="S24" s="203"/>
+      <c r="T24" s="147"/>
+      <c r="U24" s="146"/>
+      <c r="V24" s="147"/>
+      <c r="W24" s="146"/>
+      <c r="X24" s="147"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="143" t="s">
         <v>492</v>
-      </c>
-      <c r="B24" s="150"/>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="151"/>
-      <c r="F24" s="150"/>
-      <c r="G24" s="138"/>
-      <c r="H24" s="138"/>
-      <c r="I24" s="151"/>
-      <c r="J24" s="150"/>
-      <c r="K24" s="138"/>
-      <c r="L24" s="138"/>
-      <c r="M24" s="138"/>
-      <c r="N24" s="138"/>
-      <c r="O24" s="138"/>
-      <c r="P24" s="138"/>
-      <c r="Q24" s="138"/>
-      <c r="R24" s="138"/>
-      <c r="S24" s="151"/>
-      <c r="T24" s="150"/>
-      <c r="U24" s="151"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="143" t="s">
-        <v>493</v>
       </c>
       <c r="B25" s="150"/>
       <c r="C25" s="138"/>
@@ -4592,13 +4788,16 @@
       <c r="P25" s="138"/>
       <c r="Q25" s="138"/>
       <c r="R25" s="138"/>
-      <c r="S25" s="151"/>
-      <c r="T25" s="150"/>
-      <c r="U25" s="151"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S25" s="204"/>
+      <c r="T25" s="151"/>
+      <c r="U25" s="150"/>
+      <c r="V25" s="151"/>
+      <c r="W25" s="150"/>
+      <c r="X25" s="151"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="143" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B26" s="150"/>
       <c r="C26" s="138"/>
@@ -4617,13 +4816,16 @@
       <c r="P26" s="138"/>
       <c r="Q26" s="138"/>
       <c r="R26" s="138"/>
-      <c r="S26" s="151"/>
-      <c r="T26" s="150"/>
-      <c r="U26" s="151"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S26" s="204"/>
+      <c r="T26" s="151"/>
+      <c r="U26" s="150"/>
+      <c r="V26" s="151"/>
+      <c r="W26" s="150"/>
+      <c r="X26" s="151"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="143" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="B27" s="150"/>
       <c r="C27" s="138"/>
@@ -4642,13 +4844,16 @@
       <c r="P27" s="138"/>
       <c r="Q27" s="138"/>
       <c r="R27" s="138"/>
-      <c r="S27" s="151"/>
-      <c r="T27" s="150"/>
-      <c r="U27" s="151"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S27" s="204"/>
+      <c r="T27" s="151"/>
+      <c r="U27" s="150"/>
+      <c r="V27" s="151"/>
+      <c r="W27" s="150"/>
+      <c r="X27" s="151"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="143" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B28" s="150"/>
       <c r="C28" s="138"/>
@@ -4667,16 +4872,48 @@
       <c r="P28" s="138"/>
       <c r="Q28" s="138"/>
       <c r="R28" s="138"/>
-      <c r="S28" s="151"/>
-      <c r="T28" s="150"/>
-      <c r="U28" s="151"/>
+      <c r="S28" s="204"/>
+      <c r="T28" s="151"/>
+      <c r="U28" s="150"/>
+      <c r="V28" s="151"/>
+      <c r="W28" s="150"/>
+      <c r="X28" s="151"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="143" t="s">
+        <v>494</v>
+      </c>
+      <c r="B29" s="150"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="138"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="138"/>
+      <c r="N29" s="138"/>
+      <c r="O29" s="138"/>
+      <c r="P29" s="138"/>
+      <c r="Q29" s="138"/>
+      <c r="R29" s="138"/>
+      <c r="S29" s="204"/>
+      <c r="T29" s="151"/>
+      <c r="U29" s="150"/>
+      <c r="V29" s="151"/>
+      <c r="W29" s="150"/>
+      <c r="X29" s="151"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="J1:S1"/>
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="J1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5317,16 +5554,16 @@
         <v>13</v>
       </c>
       <c r="F2" s="98" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G2" s="98" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H2" s="98" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I2" s="98" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J2" s="98" t="s">
         <v>44</v>
@@ -5425,16 +5662,16 @@
         <v>15</v>
       </c>
       <c r="AP2" s="98" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AQ2" s="98" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AR2" s="98" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AS2" s="98" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AT2" s="98" t="s">
         <v>171</v>
@@ -5449,16 +5686,16 @@
         <v>171</v>
       </c>
       <c r="AX2" s="98" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AY2" s="98" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AZ2" s="98" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="BA2" s="98" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="BB2" s="98" t="s">
         <v>168</v>
@@ -5485,16 +5722,16 @@
         <v>169</v>
       </c>
       <c r="BJ2" s="98" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="BK2" s="98" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="BL2" s="98" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="BM2" s="98" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="BN2" s="98" t="s">
         <v>175</v>
@@ -5509,16 +5746,16 @@
         <v>175</v>
       </c>
       <c r="BR2" s="98" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="BS2" s="98" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="BT2" s="98" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="BU2" s="98" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="BV2" s="98" t="s">
         <v>166</v>
@@ -5629,28 +5866,28 @@
         <v>48</v>
       </c>
       <c r="DF2" s="98" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="DG2" s="98" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="DH2" s="98" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="DI2" s="98" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="DJ2" s="98" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="DK2" s="98" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="DL2" s="98" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="DM2" s="98" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="DN2" s="98" t="s">
         <v>193</v>
@@ -5677,16 +5914,16 @@
         <v>194</v>
       </c>
       <c r="DV2" s="98" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="DW2" s="98" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="DX2" s="98" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="DY2" s="98" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="DZ2" s="98" t="s">
         <v>62</v>
@@ -5701,16 +5938,16 @@
         <v>62</v>
       </c>
       <c r="ED2" s="98" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="EE2" s="98" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="EF2" s="98" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="EG2" s="98" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="EH2" s="98" t="s">
         <v>49</v>
@@ -5725,28 +5962,28 @@
         <v>49</v>
       </c>
       <c r="EL2" s="98" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="EM2" s="98" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="EN2" s="98" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="EO2" s="98" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="EP2" s="98" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="EQ2" s="98" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="ER2" s="98" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="ES2" s="98" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="ET2" s="98" t="s">
         <v>112</v>
@@ -5761,16 +5998,16 @@
         <v>112</v>
       </c>
       <c r="EX2" s="98" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="EY2" s="98" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="EZ2" s="98" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="FA2" s="98" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="FB2" s="98" t="s">
         <v>14</v>
@@ -5797,16 +6034,16 @@
         <v>209</v>
       </c>
       <c r="FJ2" s="103" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="FK2" s="103" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="FL2" s="103" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="FM2" s="103" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="FN2" s="103" t="s">
         <v>210</v>
@@ -5833,7 +6070,7 @@
         <v>211</v>
       </c>
       <c r="FV2" s="98" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="3" spans="1:178" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6334,7 +6571,7 @@
       <c r="AY4" s="169"/>
       <c r="AZ4" s="169"/>
       <c r="BA4" s="169" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="BB4" s="169" t="s">
         <v>17</v>
@@ -6354,7 +6591,7 @@
       <c r="BK4" s="169"/>
       <c r="BL4" s="169"/>
       <c r="BM4" s="169" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="BN4" s="169" t="s">
         <v>17</v>
@@ -6368,7 +6605,7 @@
       <c r="BS4" s="169"/>
       <c r="BT4" s="169"/>
       <c r="BU4" s="169" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="BV4" s="169" t="s">
         <v>17</v>
@@ -6527,12 +6764,12 @@
       <c r="FT4" s="180"/>
       <c r="FU4" s="180"/>
       <c r="FV4" s="179" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" spans="1:178" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B5" s="104"/>
       <c r="C5" s="104"/>
@@ -6555,25 +6792,25 @@
       <c r="T5" s="90"/>
       <c r="U5" s="90"/>
       <c r="V5" s="90" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="W5" s="90"/>
       <c r="X5" s="90"/>
       <c r="Y5" s="90"/>
       <c r="Z5" s="90" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="AA5" s="90"/>
       <c r="AB5" s="90"/>
       <c r="AC5" s="90"/>
       <c r="AD5" s="90" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="AE5" s="90"/>
       <c r="AF5" s="90"/>
       <c r="AG5" s="90"/>
       <c r="AH5" s="90" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="AI5" s="90"/>
       <c r="AJ5" s="90"/>
@@ -6623,13 +6860,13 @@
       <c r="CB5" s="109"/>
       <c r="CC5" s="109"/>
       <c r="CD5" s="109" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="CE5" s="109"/>
       <c r="CF5" s="109"/>
       <c r="CG5" s="109"/>
       <c r="CH5" s="109" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="CI5" s="109"/>
       <c r="CJ5" s="109"/>
@@ -6639,25 +6876,25 @@
       <c r="CN5" s="109"/>
       <c r="CO5" s="109"/>
       <c r="CP5" s="109" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="CQ5" s="109"/>
       <c r="CR5" s="109"/>
       <c r="CS5" s="109"/>
       <c r="CT5" s="109" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="CU5" s="109"/>
       <c r="CV5" s="109"/>
       <c r="CW5" s="109"/>
       <c r="CX5" s="109" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="CY5" s="109"/>
       <c r="CZ5" s="109"/>
       <c r="DA5" s="109"/>
       <c r="DB5" s="109" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="DC5" s="109"/>
       <c r="DD5" s="109"/>
@@ -6667,13 +6904,13 @@
       <c r="DH5" s="109"/>
       <c r="DI5" s="109"/>
       <c r="DJ5" s="109" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="DK5" s="109"/>
       <c r="DL5" s="109"/>
       <c r="DM5" s="109"/>
       <c r="DN5" s="109" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="DO5" s="109"/>
       <c r="DP5" s="109"/>
@@ -6683,13 +6920,13 @@
       <c r="DT5" s="109"/>
       <c r="DU5" s="109"/>
       <c r="DV5" s="109" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="DW5" s="109"/>
       <c r="DX5" s="109"/>
       <c r="DY5" s="109"/>
       <c r="DZ5" s="109" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="EA5" s="109"/>
       <c r="EB5" s="109"/>
@@ -6699,13 +6936,13 @@
       <c r="EF5" s="109"/>
       <c r="EG5" s="109"/>
       <c r="EH5" s="109" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="EI5" s="109"/>
       <c r="EJ5" s="109"/>
       <c r="EK5" s="109"/>
       <c r="EL5" s="109" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="EM5" s="109"/>
       <c r="EN5" s="109"/>
@@ -6755,12 +6992,12 @@
       <c r="D6" s="104"/>
       <c r="E6" s="104"/>
       <c r="F6" s="104" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G6" s="104"/>
       <c r="H6" s="104"/>
       <c r="I6" s="104" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J6" s="101" t="s">
         <v>220</v>
@@ -6827,7 +7064,7 @@
       <c r="BP6" s="169"/>
       <c r="BQ6" s="169"/>
       <c r="BR6" s="169" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="BS6" s="169"/>
       <c r="BT6" s="169"/>
@@ -6843,7 +7080,7 @@
       <c r="CB6" s="109"/>
       <c r="CC6" s="109"/>
       <c r="CD6" s="109" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="CE6" s="109"/>
       <c r="CF6" s="109"/>
@@ -6897,7 +7134,7 @@
       <c r="EB6" s="109"/>
       <c r="EC6" s="109"/>
       <c r="ED6" s="109" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="EE6" s="109"/>
       <c r="EF6" s="109"/>
@@ -7011,7 +7248,7 @@
       <c r="BH7" s="169"/>
       <c r="BI7" s="169"/>
       <c r="BJ7" s="169" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BK7" s="169"/>
       <c r="BL7" s="169"/>
@@ -7021,7 +7258,7 @@
       <c r="BP7" s="169"/>
       <c r="BQ7" s="169"/>
       <c r="BR7" s="169" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="BS7" s="169"/>
       <c r="BT7" s="169"/>
@@ -7322,7 +7559,7 @@
     </row>
     <row r="9" spans="1:178" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B9" s="104"/>
       <c r="C9" s="104"/>
@@ -7345,25 +7582,25 @@
       <c r="T9" s="90"/>
       <c r="U9" s="90"/>
       <c r="V9" s="90" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="W9" s="90"/>
       <c r="X9" s="90"/>
       <c r="Y9" s="90"/>
       <c r="Z9" s="87" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AA9" s="90"/>
       <c r="AB9" s="90"/>
       <c r="AC9" s="90"/>
       <c r="AD9" s="87" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AE9" s="90"/>
       <c r="AF9" s="90"/>
       <c r="AG9" s="90"/>
       <c r="AH9" s="90" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="AI9" s="90"/>
       <c r="AJ9" s="90"/>
@@ -7521,7 +7758,7 @@
       <c r="D10" s="104"/>
       <c r="E10" s="104"/>
       <c r="F10" s="104" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G10" s="104"/>
       <c r="H10" s="104"/>
@@ -7557,7 +7794,7 @@
       <c r="AB10" s="90"/>
       <c r="AC10" s="90"/>
       <c r="AD10" s="90" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AE10" s="90"/>
       <c r="AF10" s="90"/>
@@ -7575,7 +7812,7 @@
       <c r="AN10" s="178"/>
       <c r="AO10" s="178"/>
       <c r="AP10" s="164" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AQ10" s="164"/>
       <c r="AR10" s="164"/>
@@ -7587,7 +7824,7 @@
       <c r="AV10" s="164"/>
       <c r="AW10" s="164"/>
       <c r="AX10" s="169" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AY10" s="169"/>
       <c r="AZ10" s="169"/>
@@ -7617,7 +7854,7 @@
       <c r="BP10" s="169"/>
       <c r="BQ10" s="169"/>
       <c r="BR10" s="169" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="BS10" s="169"/>
       <c r="BT10" s="169"/>
@@ -7635,7 +7872,7 @@
       <c r="CB10" s="109"/>
       <c r="CC10" s="109"/>
       <c r="CD10" s="109" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="CE10" s="109"/>
       <c r="CF10" s="109"/>
@@ -7677,17 +7914,17 @@
       <c r="DD10" s="109"/>
       <c r="DE10" s="109"/>
       <c r="DF10" s="109" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="DG10" s="109"/>
       <c r="DH10" s="109"/>
       <c r="DI10" s="109"/>
       <c r="DJ10" s="109" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="DK10" s="109"/>
       <c r="DL10" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM10" s="109"/>
       <c r="DN10" s="109" t="s">
@@ -7703,7 +7940,7 @@
       <c r="DT10" s="109"/>
       <c r="DU10" s="109"/>
       <c r="DV10" s="109" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="DW10" s="109"/>
       <c r="DX10" s="109"/>
@@ -7715,7 +7952,7 @@
       <c r="EB10" s="109"/>
       <c r="EC10" s="109"/>
       <c r="ED10" s="109" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="EE10" s="109"/>
       <c r="EF10" s="109"/>
@@ -7727,15 +7964,15 @@
       <c r="EJ10" s="109"/>
       <c r="EK10" s="109"/>
       <c r="EL10" s="109" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="EM10" s="109"/>
       <c r="EN10" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO10" s="109"/>
       <c r="EP10" s="109" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="EQ10" s="109"/>
       <c r="ER10" s="109"/>
@@ -7763,7 +8000,7 @@
       <c r="FH10" s="180"/>
       <c r="FI10" s="180"/>
       <c r="FJ10" s="179" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="FK10" s="180"/>
       <c r="FL10" s="180"/>
@@ -7987,16 +8224,16 @@
       <c r="D12" s="104"/>
       <c r="E12" s="104"/>
       <c r="F12" s="104" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G12" s="104" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H12" s="104" t="s">
+        <v>585</v>
+      </c>
+      <c r="I12" s="104" t="s">
         <v>586</v>
-      </c>
-      <c r="I12" s="104" t="s">
-        <v>587</v>
       </c>
       <c r="J12" s="101" t="s">
         <v>102</v>
@@ -8071,13 +8308,13 @@
       <c r="BX12" s="169"/>
       <c r="BY12" s="169"/>
       <c r="BZ12" s="109" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="CA12" s="109"/>
       <c r="CB12" s="109"/>
       <c r="CC12" s="109"/>
       <c r="CD12" s="109" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="CE12" s="109"/>
       <c r="CF12" s="109"/>
@@ -8596,7 +8833,7 @@
     </row>
     <row r="14" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B14" s="112"/>
       <c r="C14" s="112"/>
@@ -8784,7 +9021,7 @@
     </row>
     <row r="15" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B15" s="112"/>
       <c r="C15" s="112"/>
@@ -8972,7 +9209,7 @@
     </row>
     <row r="16" spans="1:178" s="5" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B16" s="112"/>
       <c r="C16" s="112"/>
@@ -9051,7 +9288,7 @@
       <c r="BX16" s="169"/>
       <c r="BY16" s="169"/>
       <c r="BZ16" s="157" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="CA16" s="113"/>
       <c r="CB16" s="113"/>
@@ -9109,7 +9346,7 @@
       <c r="EB16" s="113"/>
       <c r="EC16" s="113"/>
       <c r="ED16" s="185" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="EE16" s="113"/>
       <c r="EF16" s="113"/>
@@ -9155,7 +9392,7 @@
       <c r="FT16" s="179"/>
       <c r="FU16" s="179"/>
       <c r="FV16" s="181" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="17" spans="1:178" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9961,10 +10198,10 @@
       </c>
       <c r="DK19" s="109"/>
       <c r="DL19" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM19" s="109" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="DN19" s="109">
         <v>1</v>
@@ -10007,10 +10244,10 @@
       </c>
       <c r="EM19" s="109"/>
       <c r="EN19" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO19" s="109" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="EP19" s="109">
         <v>0.99</v>
@@ -10177,7 +10414,7 @@
       <c r="CV20" s="109"/>
       <c r="CW20" s="109"/>
       <c r="CX20" s="109" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="CY20" s="109"/>
       <c r="CZ20" s="109"/>
@@ -10195,7 +10432,7 @@
       <c r="DH20" s="109"/>
       <c r="DI20" s="109"/>
       <c r="DJ20" s="109" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="DK20" s="109"/>
       <c r="DL20" s="109"/>
@@ -10213,7 +10450,7 @@
       <c r="DT20" s="109"/>
       <c r="DU20" s="109"/>
       <c r="DV20" s="109" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="DW20" s="109"/>
       <c r="DX20" s="109"/>
@@ -10237,7 +10474,7 @@
       <c r="EJ20" s="109"/>
       <c r="EK20" s="109"/>
       <c r="EL20" s="109" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="EM20" s="109"/>
       <c r="EN20" s="109"/>
@@ -10371,7 +10608,7 @@
       <c r="BX21" s="169"/>
       <c r="BY21" s="169"/>
       <c r="BZ21" s="109" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="CA21" s="109"/>
       <c r="CB21" s="109"/>
@@ -10425,14 +10662,14 @@
       <c r="DH21" s="109"/>
       <c r="DI21" s="109"/>
       <c r="DJ21" s="109" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="DK21" s="109"/>
       <c r="DL21" s="109" t="s">
+        <v>694</v>
+      </c>
+      <c r="DM21" s="109" t="s">
         <v>695</v>
-      </c>
-      <c r="DM21" s="109" t="s">
-        <v>696</v>
       </c>
       <c r="DN21" s="109" t="s">
         <v>127</v>
@@ -10471,17 +10708,17 @@
       <c r="EJ21" s="109"/>
       <c r="EK21" s="109"/>
       <c r="EL21" s="109" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EM21" s="109"/>
       <c r="EN21" s="109" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="EO21" s="109" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="EP21" s="109" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="EQ21" s="109"/>
       <c r="ER21" s="109"/>
@@ -10565,29 +10802,29 @@
       <c r="AJ22" s="90"/>
       <c r="AK22" s="90"/>
       <c r="AL22" s="164" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="AM22" s="178"/>
       <c r="AN22" s="178"/>
       <c r="AO22" s="178"/>
       <c r="AP22" s="164" t="s">
+        <v>605</v>
+      </c>
+      <c r="AQ22" s="164" t="s">
+        <v>605</v>
+      </c>
+      <c r="AR22" s="164" t="s">
         <v>606</v>
-      </c>
-      <c r="AQ22" s="164" t="s">
-        <v>606</v>
-      </c>
-      <c r="AR22" s="164" t="s">
-        <v>607</v>
       </c>
       <c r="AS22" s="164"/>
       <c r="AT22" s="167" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AU22" s="164" t="s">
+        <v>619</v>
+      </c>
+      <c r="AV22" s="164" t="s">
         <v>620</v>
-      </c>
-      <c r="AV22" s="164" t="s">
-        <v>621</v>
       </c>
       <c r="AW22" s="164"/>
       <c r="AX22" s="169"/>
@@ -10603,7 +10840,7 @@
       <c r="BH22" s="169"/>
       <c r="BI22" s="169"/>
       <c r="BJ22" s="169" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="BK22" s="169"/>
       <c r="BL22" s="169"/>
@@ -10621,7 +10858,7 @@
       <c r="BX22" s="169"/>
       <c r="BY22" s="169"/>
       <c r="BZ22" s="109" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="CA22" s="109"/>
       <c r="CB22" s="109"/>
@@ -10657,7 +10894,7 @@
       <c r="CV22" s="109"/>
       <c r="CW22" s="109"/>
       <c r="CX22" s="109" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="CY22" s="109"/>
       <c r="CZ22" s="109"/>
@@ -10669,22 +10906,22 @@
       <c r="DD22" s="109"/>
       <c r="DE22" s="109"/>
       <c r="DF22" s="109" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="DG22" s="109"/>
       <c r="DH22" s="109" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="DI22" s="109"/>
       <c r="DJ22" s="109" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="DK22" s="109"/>
       <c r="DL22" s="109" t="s">
+        <v>694</v>
+      </c>
+      <c r="DM22" s="109" t="s">
         <v>695</v>
-      </c>
-      <c r="DM22" s="109" t="s">
-        <v>696</v>
       </c>
       <c r="DN22" s="109" t="s">
         <v>202</v>
@@ -10711,7 +10948,7 @@
       <c r="EB22" s="109"/>
       <c r="EC22" s="109"/>
       <c r="ED22" s="109" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="EE22" s="109"/>
       <c r="EF22" s="109"/>
@@ -10723,17 +10960,17 @@
       <c r="EJ22" s="109"/>
       <c r="EK22" s="109"/>
       <c r="EL22" s="109" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="EM22" s="109"/>
       <c r="EN22" s="109" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="EO22" s="109" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="EP22" s="109" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="EQ22" s="109"/>
       <c r="ER22" s="109"/>
@@ -11396,14 +11633,14 @@
       <c r="DH24" s="109"/>
       <c r="DI24" s="109"/>
       <c r="DJ24" s="109" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="DK24" s="109"/>
       <c r="DL24" s="109" t="s">
+        <v>694</v>
+      </c>
+      <c r="DM24" s="109" t="s">
         <v>695</v>
-      </c>
-      <c r="DM24" s="109" t="s">
-        <v>696</v>
       </c>
       <c r="DN24" s="109" t="str">
         <f t="shared" si="0"/>
@@ -11483,17 +11720,17 @@
       <c r="EJ24" s="109"/>
       <c r="EK24" s="109"/>
       <c r="EL24" s="109" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EM24" s="109"/>
       <c r="EN24" s="109" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="EO24" s="109" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="EP24" s="109" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="EQ24" s="109"/>
       <c r="ER24" s="109"/>
@@ -13379,7 +13616,7 @@
       </c>
       <c r="DG31" s="109"/>
       <c r="DH31" s="109" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="DI31" s="109"/>
       <c r="DJ31" s="109"/>
@@ -13589,7 +13826,7 @@
       </c>
       <c r="DG32" s="109"/>
       <c r="DH32" s="109" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="DI32" s="109"/>
       <c r="DJ32" s="109"/>
@@ -13799,7 +14036,7 @@
       </c>
       <c r="DG33" s="109"/>
       <c r="DH33" s="109" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="DI33" s="109"/>
       <c r="DJ33" s="109"/>
@@ -14077,7 +14314,7 @@
       </c>
       <c r="DG34" s="109"/>
       <c r="DH34" s="109" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="DI34" s="109"/>
       <c r="DJ34" s="109"/>
@@ -14535,7 +14772,7 @@
       </c>
       <c r="DG36" s="109"/>
       <c r="DH36" s="109" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="DI36" s="109"/>
       <c r="DJ36" s="109"/>
@@ -15082,7 +15319,7 @@
         <v>297</v>
       </c>
       <c r="AO38" s="164" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AP38" s="164"/>
       <c r="AQ38" s="164"/>
@@ -15515,7 +15752,7 @@
       <c r="AJ40" s="91"/>
       <c r="AK40" s="91"/>
       <c r="AL40" s="164" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AM40" s="164"/>
       <c r="AN40" s="164"/>
@@ -15563,13 +15800,13 @@
       <c r="CB40" s="113"/>
       <c r="CC40" s="113"/>
       <c r="CD40" s="113" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="CE40" s="113"/>
       <c r="CF40" s="113"/>
       <c r="CG40" s="113"/>
       <c r="CH40" s="113" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="CI40" s="113"/>
       <c r="CJ40" s="113"/>
@@ -15593,34 +15830,34 @@
       <c r="CV40" s="113"/>
       <c r="CW40" s="113"/>
       <c r="CX40" s="113" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="CY40" s="113"/>
       <c r="CZ40" s="113"/>
       <c r="DA40" s="113"/>
       <c r="DB40" s="113" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="DC40" s="113"/>
       <c r="DD40" s="113"/>
       <c r="DE40" s="113"/>
       <c r="DF40" s="113" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="DG40" s="113"/>
       <c r="DH40" s="113"/>
       <c r="DI40" s="113" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="DJ40" s="113" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="DK40" s="113"/>
       <c r="DL40" s="113" t="s">
+        <v>699</v>
+      </c>
+      <c r="DM40" s="113" t="s">
         <v>700</v>
-      </c>
-      <c r="DM40" s="113" t="s">
-        <v>701</v>
       </c>
       <c r="DN40" s="113" t="s">
         <v>317</v>
@@ -15635,7 +15872,7 @@
       <c r="DT40" s="113"/>
       <c r="DU40" s="113"/>
       <c r="DV40" s="113" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="DW40" s="113"/>
       <c r="DX40" s="113"/>
@@ -15647,7 +15884,7 @@
       <c r="EB40" s="113"/>
       <c r="EC40" s="113"/>
       <c r="ED40" s="113" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="EE40" s="113"/>
       <c r="EF40" s="113"/>
@@ -15663,7 +15900,7 @@
       <c r="EN40" s="113"/>
       <c r="EO40" s="113"/>
       <c r="EP40" s="113" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="EQ40" s="113"/>
       <c r="ER40" s="113"/>
@@ -15700,7 +15937,7 @@
     </row>
     <row r="41" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="63" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B41" s="112"/>
       <c r="C41" s="112"/>
@@ -16354,7 +16591,7 @@
     </row>
     <row r="44" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="63" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B44" s="112"/>
       <c r="C44" s="112"/>
@@ -16365,10 +16602,10 @@
       </c>
       <c r="G44" s="112"/>
       <c r="H44" s="112" t="s">
+        <v>567</v>
+      </c>
+      <c r="I44" s="112" t="s">
         <v>568</v>
-      </c>
-      <c r="I44" s="112" t="s">
-        <v>569</v>
       </c>
       <c r="J44" s="112"/>
       <c r="K44" s="112"/>
@@ -16445,10 +16682,10 @@
       </c>
       <c r="CA44" s="113"/>
       <c r="CB44" s="113" t="s">
+        <v>578</v>
+      </c>
+      <c r="CC44" s="113" t="s">
         <v>579</v>
-      </c>
-      <c r="CC44" s="113" t="s">
-        <v>580</v>
       </c>
       <c r="CD44" s="113">
         <v>0</v>
@@ -16461,7 +16698,7 @@
       </c>
       <c r="CI44" s="113"/>
       <c r="CJ44" s="113" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="CK44" s="113"/>
       <c r="CL44" s="113">
@@ -16475,24 +16712,24 @@
       </c>
       <c r="CQ44" s="113"/>
       <c r="CR44" s="113" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="CS44" s="113"/>
       <c r="CT44" s="113">
         <v>-0.5</v>
       </c>
       <c r="CU44" s="113" t="s">
+        <v>570</v>
+      </c>
+      <c r="CV44" s="113" t="s">
         <v>571</v>
-      </c>
-      <c r="CV44" s="113" t="s">
-        <v>572</v>
       </c>
       <c r="CW44" s="113"/>
       <c r="CX44" s="113">
         <v>0</v>
       </c>
       <c r="CY44" s="113" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="CZ44" s="113"/>
       <c r="DA44" s="113"/>
@@ -16501,10 +16738,10 @@
       </c>
       <c r="DC44" s="113"/>
       <c r="DD44" s="113" t="s">
+        <v>572</v>
+      </c>
+      <c r="DE44" s="113" t="s">
         <v>573</v>
-      </c>
-      <c r="DE44" s="113" t="s">
-        <v>574</v>
       </c>
       <c r="DF44" s="113">
         <v>0</v>
@@ -16535,7 +16772,7 @@
       </c>
       <c r="DW44" s="113"/>
       <c r="DX44" s="113" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="DY44" s="113"/>
       <c r="DZ44" s="113">
@@ -16543,7 +16780,7 @@
       </c>
       <c r="EA44" s="113"/>
       <c r="EB44" s="113" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="EC44" s="113"/>
       <c r="ED44" s="113">
@@ -16557,7 +16794,7 @@
       </c>
       <c r="EI44" s="113"/>
       <c r="EJ44" s="113" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="EK44" s="113"/>
       <c r="EL44" s="113"/>
@@ -16602,7 +16839,7 @@
     </row>
     <row r="45" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="63" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B45" s="112"/>
       <c r="C45" s="112"/>
@@ -16613,10 +16850,10 @@
       </c>
       <c r="G45" s="112"/>
       <c r="H45" s="112" t="s">
+        <v>567</v>
+      </c>
+      <c r="I45" s="112" t="s">
         <v>568</v>
-      </c>
-      <c r="I45" s="112" t="s">
-        <v>569</v>
       </c>
       <c r="J45" s="112"/>
       <c r="K45" s="112"/>
@@ -16651,7 +16888,7 @@
       </c>
       <c r="AM45" s="164"/>
       <c r="AN45" s="164" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AO45" s="164"/>
       <c r="AP45" s="164"/>
@@ -16695,10 +16932,10 @@
       </c>
       <c r="CA45" s="113"/>
       <c r="CB45" s="113" t="s">
+        <v>578</v>
+      </c>
+      <c r="CC45" s="113" t="s">
         <v>579</v>
-      </c>
-      <c r="CC45" s="113" t="s">
-        <v>580</v>
       </c>
       <c r="CD45" s="113">
         <v>0</v>
@@ -16711,7 +16948,7 @@
       </c>
       <c r="CI45" s="113"/>
       <c r="CJ45" s="113" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="CK45" s="113"/>
       <c r="CL45" s="113">
@@ -16725,7 +16962,7 @@
       </c>
       <c r="CQ45" s="113"/>
       <c r="CR45" s="113" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="CS45" s="113"/>
       <c r="CT45" s="113">
@@ -16738,7 +16975,7 @@
         <v>-0.25</v>
       </c>
       <c r="CY45" s="113" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="CZ45" s="113"/>
       <c r="DA45" s="113"/>
@@ -16747,10 +16984,10 @@
       </c>
       <c r="DC45" s="113"/>
       <c r="DD45" s="113" t="s">
+        <v>572</v>
+      </c>
+      <c r="DE45" s="113" t="s">
         <v>573</v>
-      </c>
-      <c r="DE45" s="113" t="s">
-        <v>574</v>
       </c>
       <c r="DF45" s="113">
         <v>0</v>
@@ -17714,7 +17951,7 @@
     </row>
     <row r="50" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="63" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B50" s="112"/>
       <c r="C50" s="112"/>
@@ -17932,7 +18169,7 @@
     </row>
     <row r="51" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="63" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B51" s="112"/>
       <c r="C51" s="112"/>
@@ -18210,7 +18447,7 @@
     </row>
     <row r="52" spans="1:178" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="159" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B52" s="102"/>
       <c r="C52" s="102"/>
@@ -18249,7 +18486,7 @@
       <c r="AJ52" s="92"/>
       <c r="AK52" s="90"/>
       <c r="AL52" s="167" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AM52" s="164"/>
       <c r="AN52" s="164"/>
@@ -18291,97 +18528,97 @@
       <c r="BX52" s="169"/>
       <c r="BY52" s="169"/>
       <c r="BZ52" s="113" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="CA52" s="113"/>
       <c r="CB52" s="113"/>
       <c r="CC52" s="113"/>
       <c r="CD52" s="113" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="CE52" s="113"/>
       <c r="CF52" s="113"/>
       <c r="CG52" s="113"/>
       <c r="CH52" s="113" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="CI52" s="113"/>
       <c r="CJ52" s="113"/>
       <c r="CK52" s="113"/>
       <c r="CL52" s="113" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="CM52" s="113"/>
       <c r="CN52" s="113"/>
       <c r="CO52" s="113"/>
       <c r="CP52" s="113" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="CQ52" s="113"/>
       <c r="CR52" s="113"/>
       <c r="CS52" s="113"/>
       <c r="CT52" s="113" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="CU52" s="113"/>
       <c r="CV52" s="113"/>
       <c r="CW52" s="113"/>
       <c r="CX52" s="113" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="CY52" s="113"/>
       <c r="CZ52" s="113"/>
       <c r="DA52" s="113"/>
       <c r="DB52" s="113" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="DC52" s="113"/>
       <c r="DD52" s="113"/>
       <c r="DE52" s="113"/>
       <c r="DF52" s="187" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="DG52" s="113"/>
       <c r="DH52" s="113"/>
       <c r="DI52" s="113"/>
       <c r="DJ52" s="113" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="DK52" s="113"/>
       <c r="DL52" s="113"/>
       <c r="DM52" s="113"/>
       <c r="DN52" s="113" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="DO52" s="113"/>
       <c r="DP52" s="113"/>
       <c r="DQ52" s="113"/>
       <c r="DR52" s="113" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="DS52" s="113"/>
       <c r="DT52" s="113"/>
       <c r="DU52" s="113"/>
       <c r="DV52" s="113" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="DW52" s="113"/>
       <c r="DX52" s="113"/>
       <c r="DY52" s="113"/>
       <c r="DZ52" s="113" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="EA52" s="113"/>
       <c r="EB52" s="113"/>
       <c r="EC52" s="113"/>
       <c r="ED52" s="113" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="EE52" s="113"/>
       <c r="EF52" s="113"/>
       <c r="EG52" s="113"/>
       <c r="EH52" s="113" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="EI52" s="187"/>
       <c r="EJ52" s="187"/>
@@ -18391,7 +18628,7 @@
       <c r="EN52" s="187"/>
       <c r="EO52" s="187"/>
       <c r="EP52" s="187" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="EQ52" s="187"/>
       <c r="ER52" s="187"/>
@@ -18969,7 +19206,7 @@
       </c>
       <c r="DK54" s="111"/>
       <c r="DL54" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM54" s="111"/>
       <c r="DN54" s="70"/>
@@ -19003,7 +19240,7 @@
       </c>
       <c r="EM54" s="111"/>
       <c r="EN54" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO54" s="111"/>
       <c r="EP54" s="111"/>
@@ -19583,10 +19820,10 @@
       </c>
       <c r="DK56" s="111"/>
       <c r="DL56" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM56" s="111" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="DN56" s="70"/>
       <c r="DO56" s="111"/>
@@ -19619,10 +19856,10 @@
       </c>
       <c r="EM56" s="111"/>
       <c r="EN56" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO56" s="111" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="EP56" s="111"/>
       <c r="EQ56" s="111"/>
@@ -20201,7 +20438,7 @@
       </c>
       <c r="DK58" s="111"/>
       <c r="DL58" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM58" s="111"/>
       <c r="DN58" s="70"/>
@@ -20235,7 +20472,7 @@
       </c>
       <c r="EM58" s="111"/>
       <c r="EN58" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO58" s="111"/>
       <c r="EP58" s="111"/>
@@ -20815,10 +21052,10 @@
       </c>
       <c r="DK60" s="111"/>
       <c r="DL60" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM60" s="111" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="DN60" s="70"/>
       <c r="DO60" s="111"/>
@@ -20851,10 +21088,10 @@
       </c>
       <c r="EM60" s="111"/>
       <c r="EN60" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO60" s="111" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="EP60" s="111"/>
       <c r="EQ60" s="111"/>
@@ -21433,10 +21670,10 @@
       </c>
       <c r="DK62" s="111"/>
       <c r="DL62" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM62" s="111" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="DN62" s="70"/>
       <c r="DO62" s="111"/>
@@ -21469,10 +21706,10 @@
       </c>
       <c r="EM62" s="111"/>
       <c r="EN62" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO62" s="111" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="EP62" s="111"/>
       <c r="EQ62" s="111"/>
@@ -22051,7 +22288,7 @@
       </c>
       <c r="DK64" s="111"/>
       <c r="DL64" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM64" s="111"/>
       <c r="DN64" s="70"/>
@@ -22085,10 +22322,10 @@
       </c>
       <c r="EM64" s="111"/>
       <c r="EN64" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO64" s="111" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="EP64" s="111"/>
       <c r="EQ64" s="111"/>
@@ -22667,10 +22904,10 @@
       </c>
       <c r="DK66" s="111"/>
       <c r="DL66" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM66" s="111" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="DN66" s="70"/>
       <c r="DO66" s="111"/>
@@ -22703,10 +22940,10 @@
       </c>
       <c r="EM66" s="111"/>
       <c r="EN66" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO66" s="111" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="EP66" s="111"/>
       <c r="EQ66" s="111"/>
@@ -23285,7 +23522,7 @@
       </c>
       <c r="DK68" s="111"/>
       <c r="DL68" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM68" s="111"/>
       <c r="DN68" s="70"/>
@@ -23319,7 +23556,7 @@
       </c>
       <c r="EM68" s="111"/>
       <c r="EN68" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO68" s="111"/>
       <c r="EP68" s="111"/>
@@ -23899,10 +24136,10 @@
       </c>
       <c r="DK70" s="111"/>
       <c r="DL70" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM70" s="111" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="DN70" s="70"/>
       <c r="DO70" s="111"/>
@@ -23935,10 +24172,10 @@
       </c>
       <c r="EM70" s="111"/>
       <c r="EN70" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO70" s="111" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="EP70" s="111"/>
       <c r="EQ70" s="111"/>
@@ -24517,10 +24754,10 @@
       </c>
       <c r="DK72" s="111"/>
       <c r="DL72" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM72" s="111" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="DN72" s="70"/>
       <c r="DO72" s="111"/>
@@ -24553,10 +24790,10 @@
       </c>
       <c r="EM72" s="111"/>
       <c r="EN72" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO72" s="111" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="EP72" s="111"/>
       <c r="EQ72" s="111"/>
@@ -25135,7 +25372,7 @@
       </c>
       <c r="DK74" s="111"/>
       <c r="DL74" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM74" s="111"/>
       <c r="DN74" s="70"/>
@@ -25169,10 +25406,10 @@
       </c>
       <c r="EM74" s="111"/>
       <c r="EN74" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO74" s="111" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="EP74" s="111"/>
       <c r="EQ74" s="111"/>
@@ -25751,7 +25988,7 @@
       </c>
       <c r="DK76" s="111"/>
       <c r="DL76" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM76" s="111"/>
       <c r="DN76" s="70"/>
@@ -25785,7 +26022,7 @@
       </c>
       <c r="EM76" s="111"/>
       <c r="EN76" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO76" s="111"/>
       <c r="EP76" s="111"/>
@@ -26365,7 +26602,7 @@
       </c>
       <c r="DK78" s="111"/>
       <c r="DL78" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="DM78" s="111"/>
       <c r="DN78" s="70"/>
@@ -26399,10 +26636,10 @@
       </c>
       <c r="EM78" s="111"/>
       <c r="EN78" s="109" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="EO78" s="111" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="EP78" s="111"/>
       <c r="EQ78" s="111"/>
@@ -26496,10 +26733,10 @@
         <v>56</v>
       </c>
       <c r="D3" s="191" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -26529,7 +26766,7 @@
         <v>130</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -26537,16 +26774,16 @@
         <v>53</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C6" s="192" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="74" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E6" s="74" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -26576,7 +26813,7 @@
         <v>483</v>
       </c>
       <c r="E8" s="74" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -26584,16 +26821,16 @@
         <v>53</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C9" s="192" t="s">
         <v>58</v>
       </c>
       <c r="D9" s="74" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E9" s="74" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -26633,10 +26870,10 @@
         <v>230</v>
       </c>
       <c r="D12" s="74" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E12" s="74" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -26674,7 +26911,7 @@
         <v>231</v>
       </c>
       <c r="D15" s="74" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E15" s="74"/>
     </row>
@@ -26713,7 +26950,7 @@
         <v>232</v>
       </c>
       <c r="D18" s="74" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E18" s="74"/>
     </row>
@@ -26771,7 +27008,7 @@
       </c>
       <c r="B23" s="74"/>
       <c r="C23" s="192" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D23" s="74"/>
       <c r="E23" s="74"/>
@@ -26945,10 +27182,10 @@
         <v>264</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="N2" s="30" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -27109,7 +27346,7 @@
         <v>180</v>
       </c>
       <c r="M7" s="71" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N7" s="71" t="s">
         <v>180</v>
@@ -27285,7 +27522,7 @@
         <v>180</v>
       </c>
       <c r="M11" s="71" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N11" s="71" t="s">
         <v>180</v>
@@ -27373,7 +27610,7 @@
         <v>180</v>
       </c>
       <c r="M13" s="71" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N13" s="71" t="s">
         <v>180</v>
@@ -27381,46 +27618,46 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27513,46 +27750,46 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27645,46 +27882,46 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N20" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -27777,46 +28014,46 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N23" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -27835,10 +28072,10 @@
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N24" s="26" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -27865,46 +28102,46 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="B26" s="22" t="s">
-        <v>561</v>
-      </c>
       <c r="C26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="M26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="N26" s="22" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -27923,7 +28160,7 @@
       <c r="K27" s="26"/>
       <c r="L27" s="26"/>
       <c r="M27" s="26" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="N27" s="26"/>
     </row>
@@ -27943,7 +28180,7 @@
       <c r="K28" s="26"/>
       <c r="L28" s="26"/>
       <c r="M28" s="26" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N28" s="26"/>
     </row>
@@ -27990,7 +28227,7 @@
         <v>104</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -28011,10 +28248,10 @@
         <v>214</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E4" s="71" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -28045,10 +28282,10 @@
         <v>213</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E6" s="71" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -28079,10 +28316,10 @@
         <v>215</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -28113,7 +28350,7 @@
         <v>217</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E10" s="71" t="s">
         <v>342</v>
@@ -28130,7 +28367,7 @@
         <v>216</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E11" s="71" t="s">
         <v>343</v>
@@ -30149,7 +30386,7 @@
     </row>
     <row r="143" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="40" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B143" s="41" t="s">
         <v>142</v>
@@ -30371,7 +30608,7 @@
     </row>
     <row r="159" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="40" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B159" s="41" t="s">
         <v>142</v>
@@ -30572,7 +30809,7 @@
         <v>155</v>
       </c>
       <c r="B173" s="42" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C173" s="43"/>
       <c r="D173" s="43"/>
@@ -30593,7 +30830,7 @@
     </row>
     <row r="175" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="40" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B175" s="41" t="s">
         <v>142</v>
@@ -30815,7 +31052,7 @@
     </row>
     <row r="191" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="35" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B191" s="36" t="s">
         <v>142</v>
@@ -31037,7 +31274,7 @@
     </row>
     <row r="207" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="35" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B207" s="36" t="s">
         <v>142</v>

</xml_diff>

<commit_message>
Changes to Ketamine definition.  Adding central nervous response so that it has pain relief effects and changing effect site rate constant to 2.0 /min based on literature.  Removing respiratory modifier because ketamine does not have large respiratory effect.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntatum\BioGearsCMake\core\share\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\biogears\core\share\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4894" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4894" uniqueCount="734">
   <si>
     <t>Name</t>
   </si>
@@ -2233,6 +2233,9 @@
   </si>
   <si>
     <t>65 in</t>
+  </si>
+  <si>
+    <t>0.2 1/min</t>
   </si>
 </sst>
 </file>
@@ -3271,15 +3274,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3296,6 +3290,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3618,7 +3621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3653,39 +3656,39 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="134"/>
-      <c r="B1" s="197" t="s">
+      <c r="B1" s="203" t="s">
         <v>518</v>
       </c>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="197" t="s">
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="203" t="s">
         <v>515</v>
       </c>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="199"/>
-      <c r="J1" s="197" t="s">
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="203" t="s">
         <v>516</v>
       </c>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
-      <c r="M1" s="198"/>
-      <c r="N1" s="198"/>
-      <c r="O1" s="198"/>
-      <c r="P1" s="198"/>
-      <c r="Q1" s="198"/>
-      <c r="R1" s="198"/>
-      <c r="S1" s="198"/>
-      <c r="T1" s="199"/>
-      <c r="U1" s="197" t="s">
+      <c r="K1" s="204"/>
+      <c r="L1" s="204"/>
+      <c r="M1" s="204"/>
+      <c r="N1" s="204"/>
+      <c r="O1" s="204"/>
+      <c r="P1" s="204"/>
+      <c r="Q1" s="204"/>
+      <c r="R1" s="204"/>
+      <c r="S1" s="204"/>
+      <c r="T1" s="205"/>
+      <c r="U1" s="203" t="s">
         <v>517</v>
       </c>
-      <c r="V1" s="199"/>
-      <c r="W1" s="197" t="s">
+      <c r="V1" s="205"/>
+      <c r="W1" s="203" t="s">
         <v>722</v>
       </c>
-      <c r="X1" s="199"/>
+      <c r="X1" s="205"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="135" t="s">
@@ -3742,7 +3745,7 @@
       <c r="R2" s="136" t="s">
         <v>243</v>
       </c>
-      <c r="S2" s="200" t="s">
+      <c r="S2" s="197" t="s">
         <v>725</v>
       </c>
       <c r="T2" s="145" t="s">
@@ -3782,7 +3785,7 @@
       <c r="P3" s="141"/>
       <c r="Q3" s="141"/>
       <c r="R3" s="141"/>
-      <c r="S3" s="201"/>
+      <c r="S3" s="198"/>
       <c r="T3" s="153"/>
       <c r="U3" s="152"/>
       <c r="V3" s="153"/>
@@ -3844,7 +3847,7 @@
       <c r="R4" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="202" t="s">
+      <c r="S4" s="199" t="s">
         <v>9</v>
       </c>
       <c r="T4" s="149" t="s">
@@ -3884,7 +3887,7 @@
       <c r="P5" s="140"/>
       <c r="Q5" s="140"/>
       <c r="R5" s="140"/>
-      <c r="S5" s="203"/>
+      <c r="S5" s="200"/>
       <c r="T5" s="147"/>
       <c r="U5" s="146"/>
       <c r="V5" s="147"/>
@@ -3942,7 +3945,7 @@
       <c r="R6" s="138" t="s">
         <v>244</v>
       </c>
-      <c r="S6" s="204" t="s">
+      <c r="S6" s="201" t="s">
         <v>726</v>
       </c>
       <c r="T6" s="151" t="s">
@@ -4012,7 +4015,7 @@
       <c r="R7" s="138" t="s">
         <v>245</v>
       </c>
-      <c r="S7" s="204" t="s">
+      <c r="S7" s="201" t="s">
         <v>727</v>
       </c>
       <c r="T7" s="151" t="s">
@@ -4078,7 +4081,7 @@
       <c r="R8" s="138" t="s">
         <v>246</v>
       </c>
-      <c r="S8" s="204" t="s">
+      <c r="S8" s="201" t="s">
         <v>728</v>
       </c>
       <c r="T8" s="151" t="s">
@@ -4148,7 +4151,7 @@
       <c r="R9" s="138">
         <v>0.25</v>
       </c>
-      <c r="S9" s="204">
+      <c r="S9" s="201">
         <v>0.21</v>
       </c>
       <c r="T9" s="151">
@@ -4188,7 +4191,7 @@
       <c r="P10" s="140"/>
       <c r="Q10" s="140"/>
       <c r="R10" s="140"/>
-      <c r="S10" s="203"/>
+      <c r="S10" s="200"/>
       <c r="T10" s="147"/>
       <c r="U10" s="146"/>
       <c r="V10" s="147"/>
@@ -4216,7 +4219,7 @@
       <c r="P11" s="138"/>
       <c r="Q11" s="138"/>
       <c r="R11" s="138"/>
-      <c r="S11" s="204"/>
+      <c r="S11" s="201"/>
       <c r="T11" s="151"/>
       <c r="U11" s="150"/>
       <c r="V11" s="151"/>
@@ -4244,7 +4247,7 @@
       <c r="P12" s="138"/>
       <c r="Q12" s="138"/>
       <c r="R12" s="138"/>
-      <c r="S12" s="204"/>
+      <c r="S12" s="201"/>
       <c r="T12" s="151"/>
       <c r="U12" s="150"/>
       <c r="V12" s="151"/>
@@ -4302,7 +4305,7 @@
       <c r="R13" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="S13" s="204" t="s">
+      <c r="S13" s="201" t="s">
         <v>22</v>
       </c>
       <c r="T13" s="151" t="s">
@@ -4372,7 +4375,7 @@
       <c r="R14" s="138" t="s">
         <v>488</v>
       </c>
-      <c r="S14" s="204" t="s">
+      <c r="S14" s="201" t="s">
         <v>488</v>
       </c>
       <c r="T14" s="151" t="s">
@@ -4442,7 +4445,7 @@
       <c r="R15" s="138" t="s">
         <v>489</v>
       </c>
-      <c r="S15" s="204" t="s">
+      <c r="S15" s="201" t="s">
         <v>489</v>
       </c>
       <c r="T15" s="151" t="s">
@@ -4512,7 +4515,7 @@
       <c r="R16" s="138" t="s">
         <v>69</v>
       </c>
-      <c r="S16" s="204" t="s">
+      <c r="S16" s="201" t="s">
         <v>218</v>
       </c>
       <c r="T16" s="151" t="s">
@@ -4552,7 +4555,7 @@
       <c r="P17" s="140"/>
       <c r="Q17" s="140"/>
       <c r="R17" s="140"/>
-      <c r="S17" s="203"/>
+      <c r="S17" s="200"/>
       <c r="T17" s="147"/>
       <c r="U17" s="146"/>
       <c r="V17" s="147"/>
@@ -4580,7 +4583,7 @@
       <c r="P18" s="138"/>
       <c r="Q18" s="138"/>
       <c r="R18" s="138"/>
-      <c r="S18" s="204"/>
+      <c r="S18" s="201"/>
       <c r="T18" s="151"/>
       <c r="U18" s="150"/>
       <c r="V18" s="151"/>
@@ -4608,7 +4611,7 @@
       <c r="P19" s="138"/>
       <c r="Q19" s="138"/>
       <c r="R19" s="138"/>
-      <c r="S19" s="204"/>
+      <c r="S19" s="201"/>
       <c r="T19" s="151"/>
       <c r="U19" s="150">
         <v>0.5</v>
@@ -4640,7 +4643,7 @@
       <c r="P20" s="138"/>
       <c r="Q20" s="138"/>
       <c r="R20" s="138"/>
-      <c r="S20" s="204"/>
+      <c r="S20" s="201"/>
       <c r="T20" s="151"/>
       <c r="U20" s="150"/>
       <c r="V20" s="151"/>
@@ -4668,7 +4671,7 @@
       <c r="P21" s="195"/>
       <c r="Q21" s="195"/>
       <c r="R21" s="195"/>
-      <c r="S21" s="205" t="s">
+      <c r="S21" s="202" t="s">
         <v>729</v>
       </c>
       <c r="T21" s="196"/>
@@ -4698,7 +4701,7 @@
       <c r="P22" s="195"/>
       <c r="Q22" s="195"/>
       <c r="R22" s="195"/>
-      <c r="S22" s="205">
+      <c r="S22" s="202">
         <v>0.2</v>
       </c>
       <c r="T22" s="196"/>
@@ -4728,7 +4731,7 @@
       <c r="P23" s="195"/>
       <c r="Q23" s="195"/>
       <c r="R23" s="195"/>
-      <c r="S23" s="205"/>
+      <c r="S23" s="202"/>
       <c r="T23" s="196"/>
       <c r="U23" s="150"/>
       <c r="V23" s="196"/>
@@ -4760,7 +4763,7 @@
       <c r="P24" s="140"/>
       <c r="Q24" s="140"/>
       <c r="R24" s="140"/>
-      <c r="S24" s="203"/>
+      <c r="S24" s="200"/>
       <c r="T24" s="147"/>
       <c r="U24" s="146"/>
       <c r="V24" s="147"/>
@@ -4788,7 +4791,7 @@
       <c r="P25" s="138"/>
       <c r="Q25" s="138"/>
       <c r="R25" s="138"/>
-      <c r="S25" s="204"/>
+      <c r="S25" s="201"/>
       <c r="T25" s="151"/>
       <c r="U25" s="150"/>
       <c r="V25" s="151"/>
@@ -4816,7 +4819,7 @@
       <c r="P26" s="138"/>
       <c r="Q26" s="138"/>
       <c r="R26" s="138"/>
-      <c r="S26" s="204"/>
+      <c r="S26" s="201"/>
       <c r="T26" s="151"/>
       <c r="U26" s="150"/>
       <c r="V26" s="151"/>
@@ -4844,7 +4847,7 @@
       <c r="P27" s="138"/>
       <c r="Q27" s="138"/>
       <c r="R27" s="138"/>
-      <c r="S27" s="204"/>
+      <c r="S27" s="201"/>
       <c r="T27" s="151"/>
       <c r="U27" s="150"/>
       <c r="V27" s="151"/>
@@ -4872,7 +4875,7 @@
       <c r="P28" s="138"/>
       <c r="Q28" s="138"/>
       <c r="R28" s="138"/>
-      <c r="S28" s="204"/>
+      <c r="S28" s="201"/>
       <c r="T28" s="151"/>
       <c r="U28" s="150"/>
       <c r="V28" s="151"/>
@@ -4900,7 +4903,7 @@
       <c r="P29" s="138"/>
       <c r="Q29" s="138"/>
       <c r="R29" s="138"/>
-      <c r="S29" s="204"/>
+      <c r="S29" s="201"/>
       <c r="T29" s="151"/>
       <c r="U29" s="150"/>
       <c r="V29" s="151"/>
@@ -4924,11 +4927,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FV78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="BN30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="CP46" sqref="CP46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -17184,7 +17187,7 @@
       <c r="CN46" s="113"/>
       <c r="CO46" s="113"/>
       <c r="CP46" s="113">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="CQ46" s="113"/>
       <c r="CR46" s="113"/>
@@ -18334,7 +18337,7 @@
       <c r="CN51" s="113"/>
       <c r="CO51" s="113"/>
       <c r="CP51" s="113">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="CQ51" s="113"/>
       <c r="CR51" s="113"/>
@@ -18552,7 +18555,7 @@
       <c r="CN52" s="113"/>
       <c r="CO52" s="113"/>
       <c r="CP52" s="113" t="s">
-        <v>602</v>
+        <v>733</v>
       </c>
       <c r="CQ52" s="113"/>
       <c r="CR52" s="113"/>

</xml_diff>

<commit_message>
Put a check in Nervous system to only depress ventilation if source of CNS modifier is an opioid.  Made the CNS activity of ketamine stronger.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -4931,7 +4931,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="BN30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CP46" sqref="CP46"/>
+      <selection pane="bottomRight" activeCell="CP51" sqref="CP51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -18337,7 +18337,7 @@
       <c r="CN51" s="113"/>
       <c r="CO51" s="113"/>
       <c r="CP51" s="113">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="CQ51" s="113"/>
       <c r="CR51" s="113"/>

</xml_diff>

<commit_message>
feature:mmcdaniel-antibiotics: Finalize inflammation pre-sepsis tuning
--Adjust inflammation model to use tissue pathogen load that leaks pathogen into the blood stream.
--Update antibiotic values according to inflammation model assumed pathogen growth rate.
--Activate sepsis pathophysiology functionality--not fully tuned
--Generate states for updated inflammation model
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -2316,9 +2316,6 @@
     <t>Zwitterion</t>
   </si>
   <si>
-    <t>0.5 1/hr</t>
-  </si>
-  <si>
     <t>0.029 mg/L</t>
   </si>
   <si>
@@ -2326,6 +2323,9 @@
   </si>
   <si>
     <t>0 1/hr</t>
+  </si>
+  <si>
+    <t>0.75 1/hr</t>
   </si>
 </sst>
 </file>
@@ -5049,10 +5049,10 @@
   <dimension ref="A1:GH82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="DB36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CD36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="EX43" sqref="EX43"/>
+      <selection pane="bottomRight" activeCell="CH54" sqref="CH54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -17006,7 +17006,7 @@
       <c r="CF42" s="113"/>
       <c r="CG42" s="113"/>
       <c r="CH42" s="113" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="CI42" s="113"/>
       <c r="CJ42" s="113"/>
@@ -17042,7 +17042,7 @@
       <c r="DD42" s="113"/>
       <c r="DE42" s="113"/>
       <c r="DF42" s="113" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="DG42" s="113"/>
       <c r="DH42" s="113"/>
@@ -20138,7 +20138,7 @@
       <c r="AJ55" s="94"/>
       <c r="AK55" s="94"/>
       <c r="AL55" s="167" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="AM55" s="164"/>
       <c r="AN55" s="164"/>
@@ -20180,109 +20180,109 @@
       <c r="BX55" s="168"/>
       <c r="BY55" s="168"/>
       <c r="BZ55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="CA55" s="113"/>
       <c r="CB55" s="113"/>
       <c r="CC55" s="113"/>
       <c r="CD55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="CE55" s="113"/>
       <c r="CF55" s="113"/>
       <c r="CG55" s="113"/>
       <c r="CH55" s="113" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="CI55" s="113"/>
       <c r="CJ55" s="113"/>
       <c r="CK55" s="113"/>
       <c r="CL55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="CM55" s="113"/>
       <c r="CN55" s="113"/>
       <c r="CO55" s="113"/>
       <c r="CP55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="CQ55" s="113"/>
       <c r="CR55" s="113"/>
       <c r="CS55" s="113"/>
       <c r="CT55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="CU55" s="113"/>
       <c r="CV55" s="113"/>
       <c r="CW55" s="113"/>
       <c r="CX55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="CY55" s="113"/>
       <c r="CZ55" s="113"/>
       <c r="DA55" s="113"/>
       <c r="DB55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="DC55" s="113"/>
       <c r="DD55" s="113"/>
       <c r="DE55" s="113"/>
       <c r="DF55" s="113" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="DG55" s="113"/>
       <c r="DH55" s="113"/>
       <c r="DI55" s="113"/>
       <c r="DJ55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="DK55" s="113"/>
       <c r="DL55" s="113"/>
       <c r="DM55" s="113"/>
       <c r="DN55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="DO55" s="113"/>
       <c r="DP55" s="113"/>
       <c r="DQ55" s="113"/>
       <c r="DR55" s="113" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="DS55" s="113"/>
       <c r="DT55" s="113"/>
       <c r="DU55" s="113"/>
       <c r="DV55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="DW55" s="113"/>
       <c r="DX55" s="113"/>
       <c r="DY55" s="113"/>
       <c r="DZ55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="EA55" s="113"/>
       <c r="EB55" s="113"/>
       <c r="EC55" s="113"/>
       <c r="ED55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="EE55" s="113"/>
       <c r="EF55" s="113"/>
       <c r="EG55" s="113"/>
       <c r="EH55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="EI55" s="113"/>
       <c r="EJ55" s="113"/>
       <c r="EK55" s="113"/>
       <c r="EL55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="EM55" s="113"/>
       <c r="EN55" s="113"/>
       <c r="EO55" s="113"/>
       <c r="EP55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="EQ55" s="187"/>
       <c r="ER55" s="187"/>
@@ -20292,13 +20292,13 @@
       <c r="EV55" s="187"/>
       <c r="EW55" s="187"/>
       <c r="EX55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="EY55" s="187"/>
       <c r="EZ55" s="187"/>
       <c r="FA55" s="187"/>
       <c r="FB55" s="113" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="FC55" s="187"/>
       <c r="FD55" s="187"/>

</xml_diff>

<commit_message>
f:mmcdaniel-fentanylValidation: Correct fentanyl PKPD parameters
Fentanyl should be classified as "Base", not "WeakBase. Change fraction
unbound to Rogers values.  Adjust PD parameters to reflect new plasma
profile.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core\share\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\worktrees\FentanylValidation\build\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2025,9 +2025,6 @@
     <t>0.55 1/min</t>
   </si>
   <si>
-    <t>0.0422 1/min</t>
-  </si>
-  <si>
     <t>0.11 1/min</t>
   </si>
   <si>
@@ -2043,9 +2040,6 @@
     <t>12 mL/min kg</t>
   </si>
   <si>
-    <t>0.003 ug/mL</t>
-  </si>
-  <si>
     <t>Vasopressin</t>
   </si>
   <si>
@@ -2326,6 +2320,12 @@
   </si>
   <si>
     <t>0.75 1/hr</t>
+  </si>
+  <si>
+    <t>0.007 ug/mL</t>
+  </si>
+  <si>
+    <t>0.145 1/min</t>
   </si>
 </sst>
 </file>
@@ -3807,7 +3807,7 @@
       </c>
       <c r="V1" s="216"/>
       <c r="W1" s="214" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="X1" s="216"/>
     </row>
@@ -3867,7 +3867,7 @@
         <v>240</v>
       </c>
       <c r="S2" s="196" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="T2" s="145" t="s">
         <v>244</v>
@@ -3879,10 +3879,10 @@
         <v>507</v>
       </c>
       <c r="W2" s="144" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="X2" s="145" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -4067,7 +4067,7 @@
         <v>241</v>
       </c>
       <c r="S6" s="200" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="T6" s="151" t="s">
         <v>498</v>
@@ -4137,7 +4137,7 @@
         <v>242</v>
       </c>
       <c r="S7" s="200" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="T7" s="151" t="s">
         <v>245</v>
@@ -4203,7 +4203,7 @@
         <v>243</v>
       </c>
       <c r="S8" s="200" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="T8" s="151" t="s">
         <v>39</v>
@@ -4215,7 +4215,7 @@
         <v>511</v>
       </c>
       <c r="W8" s="150" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="X8" s="151" t="s">
         <v>20</v>
@@ -4394,7 +4394,7 @@
         <v>22</v>
       </c>
       <c r="H13" s="138" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="I13" s="151" t="s">
         <v>543</v>
@@ -4406,7 +4406,7 @@
         <v>41</v>
       </c>
       <c r="L13" s="138" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="M13" s="138" t="s">
         <v>22</v>
@@ -4415,7 +4415,7 @@
         <v>503</v>
       </c>
       <c r="O13" s="138" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="P13" s="138" t="s">
         <v>67</v>
@@ -4643,7 +4643,7 @@
         <v>69</v>
       </c>
       <c r="U16" s="150" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="V16" s="151" t="s">
         <v>221</v>
@@ -4773,7 +4773,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="143" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B21" s="150"/>
       <c r="C21" s="194"/>
@@ -4793,7 +4793,7 @@
       <c r="Q21" s="194"/>
       <c r="R21" s="194"/>
       <c r="S21" s="201" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="T21" s="195"/>
       <c r="U21" s="150"/>
@@ -4803,7 +4803,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="143" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B22" s="150"/>
       <c r="C22" s="194"/>
@@ -4833,7 +4833,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="143" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B23" s="150"/>
       <c r="C23" s="194"/>
@@ -5049,10 +5049,10 @@
   <dimension ref="A1:GH82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CD36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CD23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CH54" sqref="CH54"/>
+      <selection pane="bottomRight" activeCell="CL40" sqref="CL40:CL56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5956,16 +5956,16 @@
         <v>50</v>
       </c>
       <c r="CH2" s="98" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="CI2" s="98" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="CJ2" s="98" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="CK2" s="98" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="CL2" s="98" t="s">
         <v>51</v>
@@ -6028,16 +6028,16 @@
         <v>47</v>
       </c>
       <c r="DF2" s="98" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="DG2" s="98" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="DH2" s="98" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="DI2" s="98" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="DJ2" s="98" t="s">
         <v>48</v>
@@ -6052,28 +6052,28 @@
         <v>48</v>
       </c>
       <c r="DN2" s="98" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="DO2" s="98" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="DP2" s="98" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="DQ2" s="98" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="DR2" s="98" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="DS2" s="98" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="DT2" s="98" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="DU2" s="98" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="DV2" s="98" t="s">
         <v>193</v>
@@ -6148,40 +6148,40 @@
         <v>49</v>
       </c>
       <c r="ET2" s="98" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="EU2" s="98" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="EV2" s="98" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="EW2" s="98" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="EX2" s="98" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="EY2" s="98" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="EZ2" s="98" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="FA2" s="98" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="FB2" s="98" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="FC2" s="98" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="FD2" s="98" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="FE2" s="98" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="FF2" s="98" t="s">
         <v>112</v>
@@ -7094,7 +7094,7 @@
       <c r="CF5" s="109"/>
       <c r="CG5" s="109"/>
       <c r="CH5" s="109" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="CI5" s="109"/>
       <c r="CJ5" s="109"/>
@@ -7128,7 +7128,7 @@
       <c r="DD5" s="109"/>
       <c r="DE5" s="109"/>
       <c r="DF5" s="109" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="DG5" s="109"/>
       <c r="DH5" s="109"/>
@@ -7144,7 +7144,7 @@
       <c r="DP5" s="109"/>
       <c r="DQ5" s="109"/>
       <c r="DR5" s="109" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="DS5" s="109"/>
       <c r="DT5" s="109"/>
@@ -7182,7 +7182,7 @@
       <c r="ER5" s="109"/>
       <c r="ES5" s="109"/>
       <c r="ET5" s="109" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="EU5" s="109"/>
       <c r="EV5" s="109"/>
@@ -8170,13 +8170,13 @@
       <c r="CF10" s="109"/>
       <c r="CG10" s="109"/>
       <c r="CH10" s="109" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="CI10" s="109"/>
       <c r="CJ10" s="109"/>
       <c r="CK10" s="109"/>
       <c r="CL10" s="109" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="CM10" s="109"/>
       <c r="CN10" s="109"/>
@@ -8206,7 +8206,7 @@
       <c r="DD10" s="109"/>
       <c r="DE10" s="109"/>
       <c r="DF10" s="109" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="DG10" s="109"/>
       <c r="DH10" s="109"/>
@@ -8218,17 +8218,17 @@
       <c r="DL10" s="109"/>
       <c r="DM10" s="109"/>
       <c r="DN10" s="109" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="DO10" s="109"/>
       <c r="DP10" s="109"/>
       <c r="DQ10" s="109"/>
       <c r="DR10" s="109" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="DS10" s="109"/>
       <c r="DT10" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU10" s="109"/>
       <c r="DV10" s="109" t="s">
@@ -8268,21 +8268,21 @@
       <c r="ER10" s="109"/>
       <c r="ES10" s="109"/>
       <c r="ET10" s="109" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="EU10" s="109"/>
       <c r="EV10" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW10" s="109"/>
       <c r="EX10" s="109" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="EY10" s="109"/>
       <c r="EZ10" s="109"/>
       <c r="FA10" s="109"/>
       <c r="FB10" s="109" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="FC10" s="109"/>
       <c r="FD10" s="109"/>
@@ -10570,7 +10570,7 @@
       <c r="CJ19" s="109"/>
       <c r="CK19" s="109"/>
       <c r="CL19" s="109">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="CM19" s="109"/>
       <c r="CN19" s="109"/>
@@ -10622,10 +10622,10 @@
       </c>
       <c r="DS19" s="109"/>
       <c r="DT19" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU19" s="109" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="DV19" s="109">
         <v>1</v>
@@ -10668,10 +10668,10 @@
       </c>
       <c r="EU19" s="109"/>
       <c r="EV19" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW19" s="109" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="EX19" s="109">
         <v>0.03</v>
@@ -10826,7 +10826,7 @@
       <c r="CJ20" s="109"/>
       <c r="CK20" s="109"/>
       <c r="CL20" s="109" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="CM20" s="109"/>
       <c r="CN20" s="109"/>
@@ -10850,13 +10850,13 @@
       <c r="CZ20" s="109"/>
       <c r="DA20" s="109"/>
       <c r="DB20" s="109" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="DC20" s="109"/>
       <c r="DD20" s="109"/>
       <c r="DE20" s="109"/>
       <c r="DF20" s="109" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="DG20" s="109"/>
       <c r="DH20" s="109"/>
@@ -10874,7 +10874,7 @@
       <c r="DP20" s="109"/>
       <c r="DQ20" s="109"/>
       <c r="DR20" s="109" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="DS20" s="109"/>
       <c r="DT20" s="109"/>
@@ -10916,7 +10916,7 @@
       <c r="ER20" s="109"/>
       <c r="ES20" s="109"/>
       <c r="ET20" s="109" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="EU20" s="109"/>
       <c r="EV20" s="109"/>
@@ -11074,7 +11074,7 @@
       <c r="CJ21" s="109"/>
       <c r="CK21" s="109"/>
       <c r="CL21" s="109" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="CM21" s="109"/>
       <c r="CN21" s="109"/>
@@ -11104,7 +11104,7 @@
       <c r="DD21" s="109"/>
       <c r="DE21" s="109"/>
       <c r="DF21" s="109" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="DG21" s="109"/>
       <c r="DH21" s="109"/>
@@ -11122,14 +11122,14 @@
       <c r="DP21" s="109"/>
       <c r="DQ21" s="109"/>
       <c r="DR21" s="109" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="DS21" s="109"/>
       <c r="DT21" s="109" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="DU21" s="109" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="DV21" s="109" t="s">
         <v>127</v>
@@ -11168,23 +11168,23 @@
       <c r="ER21" s="109"/>
       <c r="ES21" s="109"/>
       <c r="ET21" s="109" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="EU21" s="109"/>
       <c r="EV21" s="109" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="EW21" s="109" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="EX21" s="109" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="EY21" s="109"/>
       <c r="EZ21" s="109"/>
       <c r="FA21" s="109"/>
       <c r="FB21" s="109" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="FC21" s="109"/>
       <c r="FD21" s="109"/>
@@ -11336,13 +11336,13 @@
       <c r="CF22" s="109"/>
       <c r="CG22" s="109"/>
       <c r="CH22" s="109" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="CI22" s="109"/>
       <c r="CJ22" s="109"/>
       <c r="CK22" s="109"/>
       <c r="CL22" s="109" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="CM22" s="109"/>
       <c r="CN22" s="109"/>
@@ -11366,13 +11366,13 @@
       <c r="CZ22" s="109"/>
       <c r="DA22" s="109"/>
       <c r="DB22" s="109" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="DC22" s="109"/>
       <c r="DD22" s="109"/>
       <c r="DE22" s="109"/>
       <c r="DF22" s="109" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="DG22" s="109"/>
       <c r="DH22" s="109"/>
@@ -11384,22 +11384,22 @@
       <c r="DL22" s="109"/>
       <c r="DM22" s="109"/>
       <c r="DN22" s="109" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="DO22" s="109"/>
       <c r="DP22" s="109" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="DQ22" s="109"/>
       <c r="DR22" s="109" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="DS22" s="109"/>
       <c r="DT22" s="109" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="DU22" s="109" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="DV22" s="109" t="s">
         <v>200</v>
@@ -11438,14 +11438,14 @@
       <c r="ER22" s="109"/>
       <c r="ES22" s="109"/>
       <c r="ET22" s="109" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="EU22" s="109"/>
       <c r="EV22" s="109" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="EW22" s="109" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="EX22" s="109" t="s">
         <v>277</v>
@@ -11454,7 +11454,7 @@
       <c r="EZ22" s="109"/>
       <c r="FA22" s="109"/>
       <c r="FB22" s="109" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="FC22" s="109"/>
       <c r="FD22" s="109"/>
@@ -12139,14 +12139,14 @@
       <c r="DP24" s="109"/>
       <c r="DQ24" s="109"/>
       <c r="DR24" s="109" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="DS24" s="109"/>
       <c r="DT24" s="109" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="DU24" s="109" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="DV24" s="109" t="str">
         <f t="shared" si="0"/>
@@ -12226,23 +12226,23 @@
       <c r="ER24" s="109"/>
       <c r="ES24" s="109"/>
       <c r="ET24" s="109" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="EU24" s="109"/>
       <c r="EV24" s="109" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="EW24" s="109" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="EX24" s="109" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="EY24" s="109"/>
       <c r="EZ24" s="109"/>
       <c r="FA24" s="109"/>
       <c r="FB24" s="109" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="FC24" s="109"/>
       <c r="FD24" s="109"/>
@@ -14178,7 +14178,7 @@
       <c r="CJ31" s="109"/>
       <c r="CK31" s="109"/>
       <c r="CL31" s="109">
-        <v>8.3000000000000007</v>
+        <v>9</v>
       </c>
       <c r="CM31" s="109"/>
       <c r="CN31" s="109"/>
@@ -14204,7 +14204,7 @@
       <c r="DD31" s="109"/>
       <c r="DE31" s="109"/>
       <c r="DF31" s="109" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="DG31" s="109"/>
       <c r="DH31" s="109"/>
@@ -14220,7 +14220,7 @@
       </c>
       <c r="DO31" s="109"/>
       <c r="DP31" s="109" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="DQ31" s="109"/>
       <c r="DR31" s="109"/>
@@ -14448,7 +14448,7 @@
       </c>
       <c r="DO32" s="109"/>
       <c r="DP32" s="109" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="DQ32" s="109"/>
       <c r="DR32" s="109"/>
@@ -14494,7 +14494,7 @@
       <c r="EV32" s="109"/>
       <c r="EW32" s="109"/>
       <c r="EX32" s="109" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="EY32" s="109"/>
       <c r="EZ32" s="109"/>
@@ -14634,7 +14634,7 @@
       <c r="CJ33" s="109"/>
       <c r="CK33" s="109"/>
       <c r="CL33" s="109">
-        <v>0.87</v>
+        <v>0.89</v>
       </c>
       <c r="CM33" s="109"/>
       <c r="CN33" s="109"/>
@@ -14676,7 +14676,7 @@
       </c>
       <c r="DO33" s="109"/>
       <c r="DP33" s="109" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="DQ33" s="109"/>
       <c r="DR33" s="109"/>
@@ -14873,8 +14873,7 @@
       <c r="CJ34" s="109"/>
       <c r="CK34" s="109"/>
       <c r="CL34" s="109">
-        <f t="shared" si="3"/>
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="CM34" s="109">
         <f t="shared" si="3"/>
@@ -14972,7 +14971,7 @@
       </c>
       <c r="DO34" s="109"/>
       <c r="DP34" s="109" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="DQ34" s="109"/>
       <c r="DR34" s="109"/>
@@ -15198,7 +15197,7 @@
       <c r="CJ35" s="109"/>
       <c r="CK35" s="109"/>
       <c r="CL35" s="109" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="CM35" s="109"/>
       <c r="CN35" s="109"/>
@@ -15224,7 +15223,7 @@
       <c r="DD35" s="109"/>
       <c r="DE35" s="109"/>
       <c r="DF35" s="109" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="DG35" s="109"/>
       <c r="DH35" s="109"/>
@@ -15424,7 +15423,7 @@
       <c r="CJ36" s="109"/>
       <c r="CK36" s="109"/>
       <c r="CL36" s="109">
-        <v>2.9</v>
+        <v>4.05</v>
       </c>
       <c r="CM36" s="109"/>
       <c r="CN36" s="109"/>
@@ -15466,7 +15465,7 @@
       </c>
       <c r="DO36" s="109"/>
       <c r="DP36" s="109" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="DQ36" s="109"/>
       <c r="DR36" s="109"/>
@@ -15555,7 +15554,7 @@
     </row>
     <row r="37" spans="1:190" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="61" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B37" s="101"/>
       <c r="C37" s="101"/>
@@ -15781,7 +15780,7 @@
     </row>
     <row r="38" spans="1:190" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="61" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B38" s="101"/>
       <c r="C38" s="101"/>
@@ -17006,13 +17005,13 @@
       <c r="CF42" s="113"/>
       <c r="CG42" s="113"/>
       <c r="CH42" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="CI42" s="113"/>
       <c r="CJ42" s="113"/>
       <c r="CK42" s="113"/>
       <c r="CL42" s="113" t="s">
-        <v>669</v>
+        <v>762</v>
       </c>
       <c r="CM42" s="113"/>
       <c r="CN42" s="113"/>
@@ -17036,13 +17035,13 @@
       <c r="CZ42" s="113"/>
       <c r="DA42" s="113"/>
       <c r="DB42" s="113" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="DC42" s="113"/>
       <c r="DD42" s="113"/>
       <c r="DE42" s="113"/>
       <c r="DF42" s="113" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="DG42" s="113"/>
       <c r="DH42" s="113"/>
@@ -17054,22 +17053,22 @@
       <c r="DL42" s="113"/>
       <c r="DM42" s="113"/>
       <c r="DN42" s="113" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="DO42" s="113"/>
       <c r="DP42" s="113"/>
       <c r="DQ42" s="113" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="DR42" s="113" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="DS42" s="113"/>
       <c r="DT42" s="113" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="DU42" s="113" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="DV42" s="113" t="s">
         <v>314</v>
@@ -17112,13 +17111,13 @@
       <c r="EV42" s="113"/>
       <c r="EW42" s="113"/>
       <c r="EX42" s="113" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="EY42" s="113"/>
       <c r="EZ42" s="113"/>
       <c r="FA42" s="113"/>
       <c r="FB42" s="113" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="FC42" s="113"/>
       <c r="FD42" s="113"/>
@@ -17254,7 +17253,7 @@
       <c r="CJ43" s="113"/>
       <c r="CK43" s="113"/>
       <c r="CL43" s="113">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="CM43" s="113"/>
       <c r="CN43" s="113"/>
@@ -17490,7 +17489,7 @@
       <c r="CJ44" s="113"/>
       <c r="CK44" s="113"/>
       <c r="CL44" s="113">
-        <v>-0.05</v>
+        <v>-0.01</v>
       </c>
       <c r="CM44" s="113"/>
       <c r="CN44" s="113"/>
@@ -17627,7 +17626,7 @@
     </row>
     <row r="45" spans="1:190" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="63" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B45" s="112"/>
       <c r="C45" s="112"/>
@@ -18722,7 +18721,7 @@
       <c r="CJ49" s="113"/>
       <c r="CK49" s="113"/>
       <c r="CL49" s="113">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="CM49" s="113"/>
       <c r="CN49" s="113"/>
@@ -19962,7 +19961,7 @@
       <c r="CJ54" s="113"/>
       <c r="CK54" s="113"/>
       <c r="CL54" s="113">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="CM54" s="113"/>
       <c r="CN54" s="113"/>
@@ -20099,7 +20098,7 @@
     </row>
     <row r="55" spans="1:190" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="159" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B55" s="112"/>
       <c r="C55" s="112"/>
@@ -20138,7 +20137,7 @@
       <c r="AJ55" s="94"/>
       <c r="AK55" s="94"/>
       <c r="AL55" s="167" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="AM55" s="164"/>
       <c r="AN55" s="164"/>
@@ -20180,109 +20179,109 @@
       <c r="BX55" s="168"/>
       <c r="BY55" s="168"/>
       <c r="BZ55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="CA55" s="113"/>
       <c r="CB55" s="113"/>
       <c r="CC55" s="113"/>
       <c r="CD55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="CE55" s="113"/>
       <c r="CF55" s="113"/>
       <c r="CG55" s="113"/>
       <c r="CH55" s="113" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="CI55" s="113"/>
       <c r="CJ55" s="113"/>
       <c r="CK55" s="113"/>
       <c r="CL55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="CM55" s="113"/>
       <c r="CN55" s="113"/>
       <c r="CO55" s="113"/>
       <c r="CP55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="CQ55" s="113"/>
       <c r="CR55" s="113"/>
       <c r="CS55" s="113"/>
       <c r="CT55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="CU55" s="113"/>
       <c r="CV55" s="113"/>
       <c r="CW55" s="113"/>
       <c r="CX55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="CY55" s="113"/>
       <c r="CZ55" s="113"/>
       <c r="DA55" s="113"/>
       <c r="DB55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="DC55" s="113"/>
       <c r="DD55" s="113"/>
       <c r="DE55" s="113"/>
       <c r="DF55" s="113" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="DG55" s="113"/>
       <c r="DH55" s="113"/>
       <c r="DI55" s="113"/>
       <c r="DJ55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="DK55" s="113"/>
       <c r="DL55" s="113"/>
       <c r="DM55" s="113"/>
       <c r="DN55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="DO55" s="113"/>
       <c r="DP55" s="113"/>
       <c r="DQ55" s="113"/>
       <c r="DR55" s="113" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="DS55" s="113"/>
       <c r="DT55" s="113"/>
       <c r="DU55" s="113"/>
       <c r="DV55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="DW55" s="113"/>
       <c r="DX55" s="113"/>
       <c r="DY55" s="113"/>
       <c r="DZ55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="EA55" s="113"/>
       <c r="EB55" s="113"/>
       <c r="EC55" s="113"/>
       <c r="ED55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="EE55" s="113"/>
       <c r="EF55" s="113"/>
       <c r="EG55" s="113"/>
       <c r="EH55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="EI55" s="113"/>
       <c r="EJ55" s="113"/>
       <c r="EK55" s="113"/>
       <c r="EL55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="EM55" s="113"/>
       <c r="EN55" s="113"/>
       <c r="EO55" s="113"/>
       <c r="EP55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="EQ55" s="187"/>
       <c r="ER55" s="187"/>
@@ -20292,13 +20291,13 @@
       <c r="EV55" s="187"/>
       <c r="EW55" s="187"/>
       <c r="EX55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="EY55" s="187"/>
       <c r="EZ55" s="187"/>
       <c r="FA55" s="187"/>
       <c r="FB55" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="FC55" s="187"/>
       <c r="FD55" s="187"/>
@@ -20434,7 +20433,7 @@
       <c r="CJ56" s="113"/>
       <c r="CK56" s="113"/>
       <c r="CL56" s="113" t="s">
-        <v>663</v>
+        <v>763</v>
       </c>
       <c r="CM56" s="113"/>
       <c r="CN56" s="113"/>
@@ -20446,13 +20445,13 @@
       <c r="CR56" s="113"/>
       <c r="CS56" s="113"/>
       <c r="CT56" s="113" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="CU56" s="113"/>
       <c r="CV56" s="113"/>
       <c r="CW56" s="113"/>
       <c r="CX56" s="113" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="CY56" s="113"/>
       <c r="CZ56" s="113"/>
@@ -20500,13 +20499,13 @@
       <c r="EB56" s="113"/>
       <c r="EC56" s="113"/>
       <c r="ED56" s="113" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="EE56" s="113"/>
       <c r="EF56" s="113"/>
       <c r="EG56" s="113"/>
       <c r="EH56" s="113" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="EI56" s="113"/>
       <c r="EJ56" s="113"/>
@@ -20518,7 +20517,7 @@
       <c r="EN56" s="113"/>
       <c r="EO56" s="113"/>
       <c r="EP56" s="113" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="EQ56" s="187"/>
       <c r="ER56" s="187"/>
@@ -20528,7 +20527,7 @@
       <c r="EV56" s="187"/>
       <c r="EW56" s="187"/>
       <c r="EX56" s="212" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="EY56" s="187"/>
       <c r="EZ56" s="187"/>
@@ -21132,7 +21131,7 @@
       </c>
       <c r="DS58" s="111"/>
       <c r="DT58" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU58" s="111"/>
       <c r="DV58" s="70"/>
@@ -21166,7 +21165,7 @@
       </c>
       <c r="EU58" s="111"/>
       <c r="EV58" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW58" s="111"/>
       <c r="EX58" s="111"/>
@@ -21770,10 +21769,10 @@
       </c>
       <c r="DS60" s="111"/>
       <c r="DT60" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU60" s="111" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="DV60" s="70"/>
       <c r="DW60" s="111"/>
@@ -21806,10 +21805,10 @@
       </c>
       <c r="EU60" s="111"/>
       <c r="EV60" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW60" s="111" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="EX60" s="111"/>
       <c r="EY60" s="111"/>
@@ -22412,7 +22411,7 @@
       </c>
       <c r="DS62" s="111"/>
       <c r="DT62" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU62" s="111"/>
       <c r="DV62" s="70"/>
@@ -22446,7 +22445,7 @@
       </c>
       <c r="EU62" s="111"/>
       <c r="EV62" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW62" s="111"/>
       <c r="EX62" s="111"/>
@@ -23050,10 +23049,10 @@
       </c>
       <c r="DS64" s="111"/>
       <c r="DT64" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU64" s="111" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="DV64" s="70"/>
       <c r="DW64" s="111"/>
@@ -23086,10 +23085,10 @@
       </c>
       <c r="EU64" s="111"/>
       <c r="EV64" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW64" s="111" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="EX64" s="111"/>
       <c r="EY64" s="111"/>
@@ -23692,10 +23691,10 @@
       </c>
       <c r="DS66" s="111"/>
       <c r="DT66" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU66" s="111" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="DV66" s="70"/>
       <c r="DW66" s="111"/>
@@ -23728,10 +23727,10 @@
       </c>
       <c r="EU66" s="111"/>
       <c r="EV66" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW66" s="111" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="EX66" s="111"/>
       <c r="EY66" s="111"/>
@@ -24334,7 +24333,7 @@
       </c>
       <c r="DS68" s="111"/>
       <c r="DT68" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU68" s="111"/>
       <c r="DV68" s="70"/>
@@ -24368,10 +24367,10 @@
       </c>
       <c r="EU68" s="111"/>
       <c r="EV68" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW68" s="111" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="EX68" s="111"/>
       <c r="EY68" s="111"/>
@@ -24974,10 +24973,10 @@
       </c>
       <c r="DS70" s="111"/>
       <c r="DT70" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU70" s="111" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="DV70" s="70"/>
       <c r="DW70" s="111"/>
@@ -25010,10 +25009,10 @@
       </c>
       <c r="EU70" s="111"/>
       <c r="EV70" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW70" s="111" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="EX70" s="111"/>
       <c r="EY70" s="111"/>
@@ -25616,7 +25615,7 @@
       </c>
       <c r="DS72" s="111"/>
       <c r="DT72" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU72" s="111"/>
       <c r="DV72" s="70"/>
@@ -25650,7 +25649,7 @@
       </c>
       <c r="EU72" s="111"/>
       <c r="EV72" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW72" s="111"/>
       <c r="EX72" s="111"/>
@@ -26254,10 +26253,10 @@
       </c>
       <c r="DS74" s="111"/>
       <c r="DT74" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU74" s="111" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="DV74" s="70"/>
       <c r="DW74" s="111"/>
@@ -26290,10 +26289,10 @@
       </c>
       <c r="EU74" s="111"/>
       <c r="EV74" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW74" s="111" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="EX74" s="111"/>
       <c r="EY74" s="111"/>
@@ -26896,10 +26895,10 @@
       </c>
       <c r="DS76" s="111"/>
       <c r="DT76" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU76" s="111" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="DV76" s="70"/>
       <c r="DW76" s="111"/>
@@ -26932,10 +26931,10 @@
       </c>
       <c r="EU76" s="111"/>
       <c r="EV76" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW76" s="111" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="EX76" s="111"/>
       <c r="EY76" s="111"/>
@@ -27538,7 +27537,7 @@
       </c>
       <c r="DS78" s="111"/>
       <c r="DT78" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU78" s="111"/>
       <c r="DV78" s="70"/>
@@ -27572,10 +27571,10 @@
       </c>
       <c r="EU78" s="111"/>
       <c r="EV78" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW78" s="111" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="EX78" s="111"/>
       <c r="EY78" s="111"/>
@@ -28178,7 +28177,7 @@
       </c>
       <c r="DS80" s="111"/>
       <c r="DT80" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU80" s="111"/>
       <c r="DV80" s="70"/>
@@ -28212,7 +28211,7 @@
       </c>
       <c r="EU80" s="111"/>
       <c r="EV80" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW80" s="111"/>
       <c r="EX80" s="111"/>
@@ -28816,7 +28815,7 @@
       </c>
       <c r="DS82" s="111"/>
       <c r="DT82" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="DU82" s="111"/>
       <c r="DV82" s="70"/>
@@ -28850,10 +28849,10 @@
       </c>
       <c r="EU82" s="111"/>
       <c r="EV82" s="109" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="EW82" s="111" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="EX82" s="111"/>
       <c r="EY82" s="111"/>
@@ -28954,7 +28953,7 @@
         <v>633</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -28984,7 +28983,7 @@
         <v>130</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -29001,7 +29000,7 @@
         <v>634</v>
       </c>
       <c r="E6" s="74" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -29031,7 +29030,7 @@
         <v>480</v>
       </c>
       <c r="E8" s="74" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -29048,7 +29047,7 @@
         <v>635</v>
       </c>
       <c r="E9" s="74" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -29085,13 +29084,13 @@
       </c>
       <c r="B12" s="74"/>
       <c r="C12" s="192" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D12" s="74" t="s">
         <v>636</v>
       </c>
       <c r="E12" s="74" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -29207,7 +29206,7 @@
         <v>230</v>
       </c>
       <c r="D21" s="74" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E21" s="74"/>
     </row>
@@ -29246,7 +29245,7 @@
         <v>231</v>
       </c>
       <c r="D24" s="74" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E24" s="74"/>
     </row>
@@ -29350,7 +29349,7 @@
       </c>
       <c r="B33" s="74"/>
       <c r="C33" s="192" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D33" s="74"/>
       <c r="E33" s="74"/>
@@ -29385,7 +29384,7 @@
       </c>
       <c r="B36" s="74"/>
       <c r="C36" s="192" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D36" s="74"/>
       <c r="E36" s="74"/>

</xml_diff>

<commit_message>
fix:mmcdaniel-fentanyl: Correct fentanyl intrinsic clearance
Intrinsic hepatic clearance must be back calculated from reported total
hepatic clearance (unless source explicity state intrinsic clearance).  Tune fentanyl EC50 following PK changes
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\worktrees\FentanylValidation\build\runtime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\worktrees\FentanylValidation\share\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2238,15 +2238,9 @@
     <t>0.3335 g/dL</t>
   </si>
   <si>
-    <t>11.0 mL/min kg</t>
-  </si>
-  <si>
     <t>0.7 mL/min kg</t>
   </si>
   <si>
-    <t>11.7 mL/min kg</t>
-  </si>
-  <si>
     <t>2.0 1/min</t>
   </si>
   <si>
@@ -2322,10 +2316,16 @@
     <t>0.75 1/hr</t>
   </si>
   <si>
-    <t>0.007 ug/mL</t>
-  </si>
-  <si>
     <t>0.145 1/min</t>
+  </si>
+  <si>
+    <t>781.0 mL/min kg</t>
+  </si>
+  <si>
+    <t>15.5 mL/min kg</t>
+  </si>
+  <si>
+    <t>0.004 ug/mL</t>
   </si>
 </sst>
 </file>
@@ -5049,10 +5049,10 @@
   <dimension ref="A1:GH82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CD23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CD18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CL40" sqref="CL40:CL56"/>
+      <selection pane="bottomRight" activeCell="CL42" sqref="CL42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5956,16 +5956,16 @@
         <v>50</v>
       </c>
       <c r="CH2" s="98" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="CI2" s="98" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="CJ2" s="98" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="CK2" s="98" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="CL2" s="98" t="s">
         <v>51</v>
@@ -6028,16 +6028,16 @@
         <v>47</v>
       </c>
       <c r="DF2" s="98" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="DG2" s="98" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="DH2" s="98" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="DI2" s="98" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="DJ2" s="98" t="s">
         <v>48</v>
@@ -6160,16 +6160,16 @@
         <v>684</v>
       </c>
       <c r="EX2" s="98" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="EY2" s="98" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="EZ2" s="98" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="FA2" s="98" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="FB2" s="98" t="s">
         <v>668</v>
@@ -8170,7 +8170,7 @@
       <c r="CF10" s="109"/>
       <c r="CG10" s="109"/>
       <c r="CH10" s="109" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="CI10" s="109"/>
       <c r="CJ10" s="109"/>
@@ -8206,7 +8206,7 @@
       <c r="DD10" s="109"/>
       <c r="DE10" s="109"/>
       <c r="DF10" s="109" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="DG10" s="109"/>
       <c r="DH10" s="109"/>
@@ -8276,7 +8276,7 @@
       </c>
       <c r="EW10" s="109"/>
       <c r="EX10" s="109" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="EY10" s="109"/>
       <c r="EZ10" s="109"/>
@@ -10826,7 +10826,7 @@
       <c r="CJ20" s="109"/>
       <c r="CK20" s="109"/>
       <c r="CL20" s="109" t="s">
-        <v>734</v>
+        <v>761</v>
       </c>
       <c r="CM20" s="109"/>
       <c r="CN20" s="109"/>
@@ -10856,7 +10856,7 @@
       <c r="DD20" s="109"/>
       <c r="DE20" s="109"/>
       <c r="DF20" s="109" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="DG20" s="109"/>
       <c r="DH20" s="109"/>
@@ -11074,7 +11074,7 @@
       <c r="CJ21" s="109"/>
       <c r="CK21" s="109"/>
       <c r="CL21" s="109" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="CM21" s="109"/>
       <c r="CN21" s="109"/>
@@ -11104,7 +11104,7 @@
       <c r="DD21" s="109"/>
       <c r="DE21" s="109"/>
       <c r="DF21" s="109" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="DG21" s="109"/>
       <c r="DH21" s="109"/>
@@ -11178,7 +11178,7 @@
         <v>692</v>
       </c>
       <c r="EX21" s="109" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="EY21" s="109"/>
       <c r="EZ21" s="109"/>
@@ -11336,13 +11336,13 @@
       <c r="CF22" s="109"/>
       <c r="CG22" s="109"/>
       <c r="CH22" s="109" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="CI22" s="109"/>
       <c r="CJ22" s="109"/>
       <c r="CK22" s="109"/>
       <c r="CL22" s="109" t="s">
-        <v>736</v>
+        <v>762</v>
       </c>
       <c r="CM22" s="109"/>
       <c r="CN22" s="109"/>
@@ -11372,7 +11372,7 @@
       <c r="DD22" s="109"/>
       <c r="DE22" s="109"/>
       <c r="DF22" s="109" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="DG22" s="109"/>
       <c r="DH22" s="109"/>
@@ -12236,7 +12236,7 @@
         <v>692</v>
       </c>
       <c r="EX24" s="109" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="EY24" s="109"/>
       <c r="EZ24" s="109"/>
@@ -14204,7 +14204,7 @@
       <c r="DD31" s="109"/>
       <c r="DE31" s="109"/>
       <c r="DF31" s="109" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="DG31" s="109"/>
       <c r="DH31" s="109"/>
@@ -14494,7 +14494,7 @@
       <c r="EV32" s="109"/>
       <c r="EW32" s="109"/>
       <c r="EX32" s="109" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="EY32" s="109"/>
       <c r="EZ32" s="109"/>
@@ -14634,7 +14634,7 @@
       <c r="CJ33" s="109"/>
       <c r="CK33" s="109"/>
       <c r="CL33" s="109">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="CM33" s="109"/>
       <c r="CN33" s="109"/>
@@ -15223,7 +15223,7 @@
       <c r="DD35" s="109"/>
       <c r="DE35" s="109"/>
       <c r="DF35" s="109" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="DG35" s="109"/>
       <c r="DH35" s="109"/>
@@ -17005,13 +17005,13 @@
       <c r="CF42" s="113"/>
       <c r="CG42" s="113"/>
       <c r="CH42" s="113" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="CI42" s="113"/>
       <c r="CJ42" s="113"/>
       <c r="CK42" s="113"/>
       <c r="CL42" s="113" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="CM42" s="113"/>
       <c r="CN42" s="113"/>
@@ -17041,7 +17041,7 @@
       <c r="DD42" s="113"/>
       <c r="DE42" s="113"/>
       <c r="DF42" s="113" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="DG42" s="113"/>
       <c r="DH42" s="113"/>
@@ -17111,7 +17111,7 @@
       <c r="EV42" s="113"/>
       <c r="EW42" s="113"/>
       <c r="EX42" s="113" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="EY42" s="113"/>
       <c r="EZ42" s="113"/>
@@ -17626,7 +17626,7 @@
     </row>
     <row r="45" spans="1:190" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="63" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B45" s="112"/>
       <c r="C45" s="112"/>
@@ -20098,7 +20098,7 @@
     </row>
     <row r="55" spans="1:190" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="159" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B55" s="112"/>
       <c r="C55" s="112"/>
@@ -20137,7 +20137,7 @@
       <c r="AJ55" s="94"/>
       <c r="AK55" s="94"/>
       <c r="AL55" s="167" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="AM55" s="164"/>
       <c r="AN55" s="164"/>
@@ -20179,109 +20179,109 @@
       <c r="BX55" s="168"/>
       <c r="BY55" s="168"/>
       <c r="BZ55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="CA55" s="113"/>
       <c r="CB55" s="113"/>
       <c r="CC55" s="113"/>
       <c r="CD55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="CE55" s="113"/>
       <c r="CF55" s="113"/>
       <c r="CG55" s="113"/>
       <c r="CH55" s="113" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="CI55" s="113"/>
       <c r="CJ55" s="113"/>
       <c r="CK55" s="113"/>
       <c r="CL55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="CM55" s="113"/>
       <c r="CN55" s="113"/>
       <c r="CO55" s="113"/>
       <c r="CP55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="CQ55" s="113"/>
       <c r="CR55" s="113"/>
       <c r="CS55" s="113"/>
       <c r="CT55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="CU55" s="113"/>
       <c r="CV55" s="113"/>
       <c r="CW55" s="113"/>
       <c r="CX55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="CY55" s="113"/>
       <c r="CZ55" s="113"/>
       <c r="DA55" s="113"/>
       <c r="DB55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="DC55" s="113"/>
       <c r="DD55" s="113"/>
       <c r="DE55" s="113"/>
       <c r="DF55" s="113" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="DG55" s="113"/>
       <c r="DH55" s="113"/>
       <c r="DI55" s="113"/>
       <c r="DJ55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="DK55" s="113"/>
       <c r="DL55" s="113"/>
       <c r="DM55" s="113"/>
       <c r="DN55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="DO55" s="113"/>
       <c r="DP55" s="113"/>
       <c r="DQ55" s="113"/>
       <c r="DR55" s="113" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="DS55" s="113"/>
       <c r="DT55" s="113"/>
       <c r="DU55" s="113"/>
       <c r="DV55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="DW55" s="113"/>
       <c r="DX55" s="113"/>
       <c r="DY55" s="113"/>
       <c r="DZ55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="EA55" s="113"/>
       <c r="EB55" s="113"/>
       <c r="EC55" s="113"/>
       <c r="ED55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="EE55" s="113"/>
       <c r="EF55" s="113"/>
       <c r="EG55" s="113"/>
       <c r="EH55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="EI55" s="113"/>
       <c r="EJ55" s="113"/>
       <c r="EK55" s="113"/>
       <c r="EL55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="EM55" s="113"/>
       <c r="EN55" s="113"/>
       <c r="EO55" s="113"/>
       <c r="EP55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="EQ55" s="187"/>
       <c r="ER55" s="187"/>
@@ -20291,13 +20291,13 @@
       <c r="EV55" s="187"/>
       <c r="EW55" s="187"/>
       <c r="EX55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="EY55" s="187"/>
       <c r="EZ55" s="187"/>
       <c r="FA55" s="187"/>
       <c r="FB55" s="113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="FC55" s="187"/>
       <c r="FD55" s="187"/>
@@ -20433,7 +20433,7 @@
       <c r="CJ56" s="113"/>
       <c r="CK56" s="113"/>
       <c r="CL56" s="113" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="CM56" s="113"/>
       <c r="CN56" s="113"/>
@@ -20445,7 +20445,7 @@
       <c r="CR56" s="113"/>
       <c r="CS56" s="113"/>
       <c r="CT56" s="113" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="CU56" s="113"/>
       <c r="CV56" s="113"/>
@@ -20527,7 +20527,7 @@
       <c r="EV56" s="187"/>
       <c r="EW56" s="187"/>
       <c r="EX56" s="212" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="EY56" s="187"/>
       <c r="EZ56" s="187"/>
@@ -29206,7 +29206,7 @@
         <v>230</v>
       </c>
       <c r="D21" s="74" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E21" s="74"/>
     </row>
@@ -29245,7 +29245,7 @@
         <v>231</v>
       </c>
       <c r="D24" s="74" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E24" s="74"/>
     </row>

</xml_diff>

<commit_message>
f/mmcdaniel-tourniquet: Update TXA hemorrhage modifier
Past changes to PK model changed TXA plasma profile.  Update TXA
hemorrhage modifier to match previous baselines.  Note that TXA
multiplier in CalcDrugEffects was changed from 1e-5 to 1e-4, so this
change essentially doubled the modifier value.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\worktrees\FentanylValidation\build\runtime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\worktrees\Tourniquet\share\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5055,10 +5055,10 @@
   <dimension ref="A1:GH82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CH3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CH13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DR19" sqref="DR19"/>
+      <selection pane="bottomRight" activeCell="EX45" sqref="EX45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -17873,7 +17873,7 @@
       <c r="EV45" s="113"/>
       <c r="EW45" s="210"/>
       <c r="EX45" s="113">
-        <v>-0.59699999999999998</v>
+        <v>-0.1</v>
       </c>
       <c r="EY45" s="211"/>
       <c r="EZ45" s="211"/>

</xml_diff>

<commit_message>
f/ntatum-WholeBloodMinorUpdates: agglutinate serialization and cardio doc -Updated documentation to ensure updated markdown for txa, htr, and override functionality -Allowed serialization of htr variables in blood chem
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6025" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6025" uniqueCount="807">
   <si>
     <t>Name</t>
   </si>
@@ -2452,6 +2452,9 @@
   </si>
   <si>
     <t>1.08 g/mL</t>
+  </si>
+  <si>
+    <t>16.8 g/dL</t>
   </si>
 </sst>
 </file>
@@ -5342,7 +5345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HF86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="EX3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -33078,8 +33081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34855,7 +34858,7 @@
         <v>771</v>
       </c>
       <c r="J47" s="72" t="s">
-        <v>771</v>
+        <v>806</v>
       </c>
       <c r="K47" s="72" t="s">
         <v>771</v>

</xml_diff>

<commit_message>
r/ntatum-WholeBloodUpdates: not so minor anymore
- Added antigen concentration to compound files, now handled directly
- Updated antigen/rbc handling in HTR
- Re-tuned the system
- Updated substance and compound xlsx/csv
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6025" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6116" uniqueCount="810">
   <si>
     <t>Name</t>
   </si>
@@ -2454,7 +2454,16 @@
     <t>1.08 g/mL</t>
   </si>
   <si>
-    <t>16.8 g/dL</t>
+    <t>0.019 g/L</t>
+  </si>
+  <si>
+    <t>0.023 g/L</t>
+  </si>
+  <si>
+    <t>0.0115 g/L</t>
+  </si>
+  <si>
+    <t>0.0095 g/L</t>
   </si>
 </sst>
 </file>
@@ -5346,10 +5355,10 @@
   <dimension ref="A1:HF86"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="EX3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="FV3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="GX2" sqref="GX2"/>
+      <selection pane="bottomRight" activeCell="GL5" sqref="GL5:HB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -33079,10 +33088,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33582,28 +33591,28 @@
         <v>129</v>
       </c>
       <c r="F13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="G13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="H13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="I13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="J13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="K13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="L13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="M13" s="72" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="N13" s="72" t="s">
         <v>165</v>
@@ -33626,28 +33635,28 @@
         <v>693</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="G14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="J14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="K14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="L14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="M14" s="72" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="N14" s="72" t="s">
         <v>226</v>
@@ -33665,28 +33674,28 @@
       <c r="E15" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="76" t="s">
+      <c r="G15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="76" t="s">
+      <c r="H15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="76" t="s">
+      <c r="I15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J15" s="76" t="s">
+      <c r="J15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K15" s="76" t="s">
+      <c r="K15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="L15" s="76" t="s">
+      <c r="L15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="M15" s="76" t="s">
+      <c r="M15" s="21" t="s">
         <v>2</v>
       </c>
       <c r="N15" s="76" t="s">
@@ -33708,28 +33717,28 @@
       </c>
       <c r="E16" s="72"/>
       <c r="F16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="G16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="H16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="I16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="J16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="K16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="L16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="M16" s="72" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="N16" s="72" t="s">
         <v>168</v>
@@ -33750,28 +33759,28 @@
       </c>
       <c r="E17" s="72"/>
       <c r="F17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="G17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="H17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="I17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="J17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="K17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="L17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="M17" s="72" t="s">
-        <v>225</v>
+        <v>723</v>
       </c>
       <c r="N17" s="72" t="s">
         <v>227</v>
@@ -33782,8 +33791,12 @@
       <c r="B18" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E18" s="76" t="s">
         <v>2</v>
       </c>
@@ -33826,28 +33839,28 @@
       </c>
       <c r="E19" s="72"/>
       <c r="F19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="G19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="H19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="I19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="J19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="K19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="L19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="M19" s="72" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="N19" s="72" t="s">
         <v>600</v>
@@ -33864,28 +33877,28 @@
       </c>
       <c r="E20" s="72"/>
       <c r="F20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="G20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="H20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="I20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="J20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="K20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="L20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="M20" s="72" t="s">
-        <v>226</v>
+        <v>719</v>
       </c>
       <c r="N20" s="72" t="s">
         <v>228</v>
@@ -33896,8 +33909,12 @@
       <c r="B21" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="21"/>
+      <c r="C21" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E21" s="76" t="s">
         <v>2</v>
       </c>
@@ -33940,28 +33957,28 @@
       </c>
       <c r="E22" s="72"/>
       <c r="F22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="G22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="H22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="I22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="J22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="K22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="L22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="M22" s="72" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="N22" s="72" t="s">
         <v>173</v>
@@ -33978,28 +33995,28 @@
       </c>
       <c r="E23" s="72"/>
       <c r="F23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M23" s="72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N23" s="72" t="s">
         <v>229</v>
@@ -34010,8 +34027,12 @@
       <c r="B24" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="76"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E24" s="76" t="s">
         <v>2</v>
       </c>
@@ -34054,28 +34075,28 @@
       </c>
       <c r="E25" s="72"/>
       <c r="F25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="G25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="H25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="I25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="J25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="K25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="L25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="M25" s="72" t="s">
-        <v>600</v>
+        <v>165</v>
       </c>
       <c r="N25" s="72" t="s">
         <v>167</v>
@@ -34092,28 +34113,28 @@
       </c>
       <c r="E26" s="72"/>
       <c r="F26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M26" s="72" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N26" s="72" t="s">
         <v>230</v>
@@ -34124,8 +34145,12 @@
       <c r="B27" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="76"/>
-      <c r="D27" s="21"/>
+      <c r="C27" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E27" s="76" t="s">
         <v>2</v>
       </c>
@@ -34166,28 +34191,28 @@
       <c r="D28" s="72"/>
       <c r="E28" s="72"/>
       <c r="F28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="L28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="M28" s="72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="N28" s="72" t="s">
         <v>471</v>
@@ -34202,28 +34227,28 @@
       <c r="D29" s="72"/>
       <c r="E29" s="72"/>
       <c r="F29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M29" s="72" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N29" s="72" t="s">
         <v>717</v>
@@ -34234,8 +34259,12 @@
       <c r="B30" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="76"/>
-      <c r="D30" s="21"/>
+      <c r="C30" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E30" s="76" t="s">
         <v>2</v>
       </c>
@@ -34276,28 +34305,28 @@
       <c r="D31" s="72"/>
       <c r="E31" s="72"/>
       <c r="F31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="G31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="H31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="I31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="J31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="K31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="L31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="M31" s="72" t="s">
-        <v>167</v>
+        <v>600</v>
       </c>
       <c r="N31" s="72" t="s">
         <v>472</v>
@@ -34312,28 +34341,28 @@
       <c r="D32" s="72"/>
       <c r="E32" s="72"/>
       <c r="F32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M32" s="72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="N32" s="72" t="s">
         <v>718</v>
@@ -34344,8 +34373,12 @@
       <c r="B33" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="76"/>
-      <c r="D33" s="21"/>
+      <c r="C33" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E33" s="76" t="s">
         <v>2</v>
       </c>
@@ -34386,28 +34419,28 @@
       <c r="D34" s="72"/>
       <c r="E34" s="72"/>
       <c r="F34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="G34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="H34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="I34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="J34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="K34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="L34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="M34" s="72" t="s">
-        <v>471</v>
+        <v>173</v>
       </c>
       <c r="N34" s="72" t="s">
         <v>471</v>
@@ -34422,28 +34455,28 @@
       <c r="D35" s="72"/>
       <c r="E35" s="72"/>
       <c r="F35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="G35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="H35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="I35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="J35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="K35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="L35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="M35" s="72" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="N35" s="72" t="s">
         <v>717</v>
@@ -34454,8 +34487,12 @@
       <c r="B36" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E36" s="76" t="s">
         <v>2</v>
       </c>
@@ -34496,28 +34533,28 @@
       <c r="D37" s="72"/>
       <c r="E37" s="72"/>
       <c r="F37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="G37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="H37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="I37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="J37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="K37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="L37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="M37" s="72" t="s">
-        <v>472</v>
+        <v>167</v>
       </c>
       <c r="N37" s="72" t="s">
         <v>472</v>
@@ -34532,28 +34569,28 @@
       <c r="D38" s="72"/>
       <c r="E38" s="72"/>
       <c r="F38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="G38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="H38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="I38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="J38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="K38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="L38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="M38" s="72" t="s">
-        <v>718</v>
+        <v>230</v>
       </c>
       <c r="N38" s="72" t="s">
         <v>718</v>
@@ -34564,8 +34601,12 @@
       <c r="B39" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="76"/>
-      <c r="D39" s="21"/>
+      <c r="C39" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E39" s="76" t="s">
         <v>2</v>
       </c>
@@ -34593,7 +34634,9 @@
       <c r="M39" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N39" s="76"/>
+      <c r="N39" s="76" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="71" t="s">
@@ -34604,28 +34647,28 @@
       <c r="D40" s="72"/>
       <c r="E40" s="72"/>
       <c r="F40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="G40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="H40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="I40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="J40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="K40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="L40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="M40" s="72" t="s">
-        <v>768</v>
+        <v>471</v>
       </c>
       <c r="N40" s="72"/>
     </row>
@@ -34638,28 +34681,28 @@
       <c r="D41" s="72"/>
       <c r="E41" s="72"/>
       <c r="F41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="G41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="H41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="I41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="J41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="K41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="L41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="M41" s="72" t="s">
-        <v>769</v>
+        <v>717</v>
       </c>
       <c r="N41" s="72"/>
     </row>
@@ -34668,8 +34711,12 @@
       <c r="B42" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="76"/>
-      <c r="D42" s="21"/>
+      <c r="C42" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E42" s="76" t="s">
         <v>2</v>
       </c>
@@ -34697,7 +34744,9 @@
       <c r="M42" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N42" s="76"/>
+      <c r="N42" s="76" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="71" t="s">
@@ -34708,28 +34757,28 @@
       <c r="D43" s="72"/>
       <c r="E43" s="72"/>
       <c r="F43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="G43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="H43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="I43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="J43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="K43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="L43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="M43" s="72" t="s">
-        <v>770</v>
+        <v>472</v>
       </c>
       <c r="N43" s="72"/>
     </row>
@@ -34742,28 +34791,28 @@
       <c r="D44" s="72"/>
       <c r="E44" s="72"/>
       <c r="F44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="G44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="H44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="I44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="J44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="K44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="L44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="M44" s="72" t="s">
-        <v>771</v>
+        <v>718</v>
       </c>
       <c r="N44" s="72"/>
     </row>
@@ -34772,8 +34821,12 @@
       <c r="B45" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="76"/>
-      <c r="D45" s="21"/>
+      <c r="C45" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E45" s="76" t="s">
         <v>2</v>
       </c>
@@ -34801,7 +34854,9 @@
       <c r="M45" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N45" s="76"/>
+      <c r="N45" s="76" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="71" t="s">
@@ -34812,28 +34867,28 @@
       <c r="D46" s="72"/>
       <c r="E46" s="72"/>
       <c r="F46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="G46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="H46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="I46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="J46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="K46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="L46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="M46" s="72" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="N46" s="72"/>
     </row>
@@ -34846,28 +34901,28 @@
       <c r="D47" s="72"/>
       <c r="E47" s="72"/>
       <c r="F47" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G47" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="H47" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="I47" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="J47" s="72" t="s">
-        <v>806</v>
+        <v>769</v>
       </c>
       <c r="K47" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="L47" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="M47" s="72" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="N47" s="72"/>
     </row>
@@ -34876,8 +34931,12 @@
       <c r="B48" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="76"/>
-      <c r="D48" s="21"/>
+      <c r="C48" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E48" s="76" t="s">
         <v>2</v>
       </c>
@@ -34905,7 +34964,9 @@
       <c r="M48" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N48" s="76"/>
+      <c r="N48" s="76" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="71" t="s">
@@ -34916,28 +34977,28 @@
       <c r="D49" s="72"/>
       <c r="E49" s="72"/>
       <c r="F49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="G49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="H49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="I49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="J49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="K49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="L49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="M49" s="72" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="N49" s="72"/>
     </row>
@@ -34950,28 +35011,28 @@
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
       <c r="F50" s="72" t="s">
-        <v>774</v>
+        <v>808</v>
       </c>
       <c r="G50" s="72" t="s">
-        <v>774</v>
+        <v>808</v>
       </c>
       <c r="H50" s="72" t="s">
-        <v>774</v>
+        <v>807</v>
       </c>
       <c r="I50" s="72" t="s">
-        <v>774</v>
+        <v>807</v>
       </c>
       <c r="J50" s="72" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="K50" s="72" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="L50" s="72" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="M50" s="72" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="N50" s="72"/>
     </row>
@@ -34980,8 +35041,12 @@
       <c r="B51" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="76"/>
-      <c r="D51" s="21"/>
+      <c r="C51" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="76" t="s">
+        <v>2</v>
+      </c>
       <c r="E51" s="76" t="s">
         <v>2</v>
       </c>
@@ -35009,7 +35074,9 @@
       <c r="M51" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N51" s="76"/>
+      <c r="N51" s="76" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="71" t="s">
@@ -35020,28 +35087,28 @@
       <c r="D52" s="72"/>
       <c r="E52" s="72"/>
       <c r="F52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="G52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="H52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="I52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="J52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="K52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="L52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="M52" s="72" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="N52" s="72"/>
     </row>
@@ -35054,30 +35121,250 @@
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
       <c r="F53" s="72" t="s">
+        <v>809</v>
+      </c>
+      <c r="G53" s="72" t="s">
+        <v>809</v>
+      </c>
+      <c r="H53" s="72" t="s">
+        <v>771</v>
+      </c>
+      <c r="I53" s="72" t="s">
+        <v>771</v>
+      </c>
+      <c r="J53" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="K53" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="L53" s="72" t="s">
+        <v>771</v>
+      </c>
+      <c r="M53" s="72" t="s">
+        <v>771</v>
+      </c>
+      <c r="N53" s="72"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="74"/>
+      <c r="B54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="G54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="H54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="I54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="J54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="K54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="L54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="M54" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="N54" s="76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="72"/>
+      <c r="C55" s="72"/>
+      <c r="D55" s="72"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="G55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="H55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="I55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="J55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="K55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="L55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="M55" s="72" t="s">
+        <v>773</v>
+      </c>
+      <c r="N55" s="72"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="72"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="72"/>
+      <c r="F56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="G56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="H56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="I56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="J56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="K56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="L56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="M56" s="72" t="s">
+        <v>774</v>
+      </c>
+      <c r="N56" s="72"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="74"/>
+      <c r="B57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="G57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="H57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="I57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="K57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="L57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="M57" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="N57" s="76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="72"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72"/>
+      <c r="E58" s="72"/>
+      <c r="F58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="G58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="H58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="I58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="J58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="K58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="L58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="M58" s="72" t="s">
+        <v>775</v>
+      </c>
+      <c r="N58" s="72"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="72"/>
+      <c r="C59" s="72"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="72"/>
+      <c r="F59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="G53" s="72" t="s">
+      <c r="G59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="H53" s="72" t="s">
+      <c r="H59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="I53" s="72" t="s">
+      <c r="I59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="J53" s="72" t="s">
+      <c r="J59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="K53" s="72" t="s">
+      <c r="K59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="L53" s="72" t="s">
+      <c r="L59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="M53" s="72" t="s">
+      <c r="M59" s="72" t="s">
         <v>776</v>
       </c>
-      <c r="N53" s="72"/>
+      <c r="N59" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
f/abaird-renal-validation: matt comments addressed here and some final potassium levels tuning in blood chemistr
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntatum\BioGearsCMake\core\share\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BioGears\biogears\core\share\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -5354,11 +5354,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HF86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="FV3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="GL5" sqref="GL5:HB5"/>
+      <selection pane="bottomRight" activeCell="AD33" sqref="AD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -14656,7 +14656,7 @@
       <c r="T29" s="88"/>
       <c r="U29" s="88"/>
       <c r="V29" s="88">
-        <v>1.8</v>
+        <v>0.8</v>
       </c>
       <c r="W29" s="81">
         <v>0.99</v>
@@ -14668,7 +14668,7 @@
         <v>291</v>
       </c>
       <c r="Z29" s="84">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="AA29" s="88"/>
       <c r="AB29" s="88"/>
@@ -33090,7 +33090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F48" sqref="F48:M53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
mmcdaniel-doc : Add WholeBlood classification to Plasma
Plasma not "whole blood" technically but the whole blood
classification seems to be better understood as "Blood Product" in terms
of how we use it.  Adding this classification will filter Plasma into
transfusion products bin when setting up visualizer actions.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BioGears\biogears\core\share\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\worktrees\Documentation\share\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="15090" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6116" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6117" uniqueCount="810">
   <si>
     <t>Name</t>
   </si>
@@ -5354,8 +5354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HF86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="DZ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AD33" sqref="AD33"/>
@@ -33090,8 +33090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48:M53"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33242,7 +33242,9 @@
       <c r="M4" s="216" t="s">
         <v>767</v>
       </c>
-      <c r="N4" s="216"/>
+      <c r="N4" s="216" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="215" t="s">

</xml_diff>

<commit_message>
fix/substanceState: Add "WholeBlood" to cmd_bio subGenerator
GenData did not have a case for Classification = WholeBlood, so subs
with this classification were not correctly parsed.
Change "State" of antigens to "Molecular" because previous value of
"Cellular" did not exist on schema.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6161" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6161" uniqueCount="816">
   <si>
     <t>Name</t>
   </si>
@@ -2389,9 +2389,6 @@
   </si>
   <si>
     <t>Plasma</t>
-  </si>
-  <si>
-    <t>Cellular</t>
   </si>
   <si>
     <t>Antigen</t>
@@ -5435,10 +5432,10 @@
   <dimension ref="A1:HG88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="EE43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="GI3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="EE57" sqref="EE57"/>
+      <selection pane="bottomRight" activeCell="GU4" sqref="GU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6403,7 +6400,7 @@
         <v>165</v>
       </c>
       <c r="BZ2" s="96" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="CA2" s="257" t="s">
         <v>190</v>
@@ -7603,32 +7600,32 @@
       <c r="GJ4" s="178"/>
       <c r="GK4" s="178"/>
       <c r="GL4" s="178"/>
-      <c r="GM4" s="245" t="s">
-        <v>785</v>
+      <c r="GM4" s="249" t="s">
+        <v>23</v>
       </c>
       <c r="GN4" s="246"/>
       <c r="GO4" s="246"/>
       <c r="GP4" s="246"/>
-      <c r="GQ4" s="245" t="s">
-        <v>785</v>
+      <c r="GQ4" s="249" t="s">
+        <v>23</v>
       </c>
       <c r="GR4" s="246"/>
       <c r="GS4" s="246"/>
       <c r="GT4" s="246"/>
-      <c r="GU4" s="245" t="s">
-        <v>785</v>
+      <c r="GU4" s="249" t="s">
+        <v>23</v>
       </c>
       <c r="GV4" s="246"/>
       <c r="GW4" s="246"/>
       <c r="GX4" s="246"/>
-      <c r="GY4" s="245" t="s">
-        <v>785</v>
+      <c r="GY4" s="249" t="s">
+        <v>23</v>
       </c>
       <c r="GZ4" s="246"/>
       <c r="HA4" s="246"/>
       <c r="HB4" s="246"/>
-      <c r="HC4" s="245" t="s">
-        <v>785</v>
+      <c r="HC4" s="249" t="s">
+        <v>23</v>
       </c>
       <c r="HD4" s="221"/>
       <c r="HE4" s="221"/>
@@ -7991,7 +7988,7 @@
       <c r="BX6" s="167"/>
       <c r="BY6" s="252"/>
       <c r="BZ6" s="107" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="CA6" s="258" t="s">
         <v>124</v>
@@ -8124,19 +8121,19 @@
       <c r="GS6" s="246"/>
       <c r="GT6" s="246"/>
       <c r="GU6" s="249" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="GV6" s="246"/>
       <c r="GW6" s="246"/>
       <c r="GX6" s="246"/>
       <c r="GY6" s="249" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="GZ6" s="246"/>
       <c r="HA6" s="246"/>
       <c r="HB6" s="246"/>
       <c r="HC6" s="249" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="HD6" s="221"/>
       <c r="HE6" s="221"/>
@@ -8935,7 +8932,7 @@
       <c r="BX10" s="167"/>
       <c r="BY10" s="252"/>
       <c r="BZ10" s="107" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="CA10" s="258" t="s">
         <v>320</v>
@@ -9112,31 +9109,31 @@
       <c r="GK10" s="178"/>
       <c r="GL10" s="178"/>
       <c r="GM10" s="245" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="GN10" s="246"/>
       <c r="GO10" s="246"/>
       <c r="GP10" s="246"/>
       <c r="GQ10" s="245" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="GR10" s="246"/>
       <c r="GS10" s="246"/>
       <c r="GT10" s="246"/>
       <c r="GU10" s="245" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="GV10" s="246"/>
       <c r="GW10" s="246"/>
       <c r="GX10" s="246"/>
       <c r="GY10" s="245" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="GZ10" s="246"/>
       <c r="HA10" s="246"/>
       <c r="HB10" s="246"/>
       <c r="HC10" s="245" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="HD10" s="221"/>
       <c r="HE10" s="221"/>
@@ -9610,7 +9607,7 @@
     </row>
     <row r="13" spans="1:214" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="60" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B13" s="99"/>
       <c r="C13" s="99"/>
@@ -9806,13 +9803,13 @@
       <c r="GK13" s="177"/>
       <c r="GL13" s="177"/>
       <c r="GM13" s="245" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="GN13" s="245"/>
       <c r="GO13" s="245"/>
       <c r="GP13" s="245"/>
       <c r="GQ13" s="245" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="GR13" s="245"/>
       <c r="GS13" s="245"/>
@@ -12409,7 +12406,7 @@
       <c r="BX22" s="167"/>
       <c r="BY22" s="252"/>
       <c r="BZ22" s="107" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="CA22" s="258" t="s">
         <v>537</v>
@@ -13469,7 +13466,7 @@
       <c r="BX25" s="167"/>
       <c r="BY25" s="252"/>
       <c r="BZ25" s="107" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="CA25" s="258" t="str">
         <f>CA22</f>
@@ -15298,7 +15295,7 @@
     </row>
     <row r="31" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="79" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B31" s="222"/>
       <c r="C31" s="223" t="s">
@@ -15788,7 +15785,7 @@
     </row>
     <row r="32" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="80" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B32" s="99"/>
       <c r="C32" s="99"/>
@@ -15984,31 +15981,31 @@
       <c r="GK32" s="177"/>
       <c r="GL32" s="177"/>
       <c r="GM32" s="245" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="GN32" s="245"/>
       <c r="GO32" s="245"/>
       <c r="GP32" s="245"/>
       <c r="GQ32" s="245" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="GR32" s="245"/>
       <c r="GS32" s="245"/>
       <c r="GT32" s="245"/>
       <c r="GU32" s="245" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="GV32" s="245"/>
       <c r="GW32" s="245"/>
       <c r="GX32" s="245"/>
       <c r="GY32" s="245" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="GZ32" s="245"/>
       <c r="HA32" s="245"/>
       <c r="HB32" s="245"/>
       <c r="HC32" s="245" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="HD32" s="220"/>
       <c r="HE32" s="220"/>
@@ -16016,7 +16013,7 @@
     </row>
     <row r="33" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="80" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B33" s="99"/>
       <c r="C33" s="99"/>
@@ -16212,31 +16209,31 @@
       <c r="GK33" s="177"/>
       <c r="GL33" s="177"/>
       <c r="GM33" s="245" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="GN33" s="245"/>
       <c r="GO33" s="245"/>
       <c r="GP33" s="245"/>
       <c r="GQ33" s="245" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="GR33" s="245"/>
       <c r="GS33" s="245"/>
       <c r="GT33" s="245"/>
       <c r="GU33" s="245" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="GV33" s="245"/>
       <c r="GW33" s="245"/>
       <c r="GX33" s="245"/>
       <c r="GY33" s="245" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="GZ33" s="245"/>
       <c r="HA33" s="245"/>
       <c r="HB33" s="245"/>
       <c r="HC33" s="245" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="HD33" s="220"/>
       <c r="HE33" s="220"/>
@@ -20014,7 +20011,7 @@
       <c r="BX46" s="167"/>
       <c r="BY46" s="252"/>
       <c r="BZ46" s="111" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="CA46" s="208" t="s">
         <v>321</v>
@@ -20463,7 +20460,7 @@
     </row>
     <row r="48" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="62" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B48" s="110"/>
       <c r="C48" s="110"/>
@@ -23719,7 +23716,7 @@
     </row>
     <row r="60" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="62" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B60" s="110"/>
       <c r="C60" s="110"/>
@@ -33995,7 +33992,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="214" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D3" s="189" t="s">
         <v>623</v>
@@ -34074,28 +34071,28 @@
       <c r="D5" s="216"/>
       <c r="E5" s="216"/>
       <c r="F5" s="248" t="s">
+        <v>800</v>
+      </c>
+      <c r="G5" s="248" t="s">
         <v>801</v>
       </c>
-      <c r="G5" s="248" t="s">
-        <v>802</v>
-      </c>
       <c r="H5" s="248" t="s">
+        <v>800</v>
+      </c>
+      <c r="I5" s="248" t="s">
         <v>801</v>
       </c>
-      <c r="I5" s="248" t="s">
-        <v>802</v>
-      </c>
       <c r="J5" s="248" t="s">
+        <v>800</v>
+      </c>
+      <c r="K5" s="248" t="s">
         <v>801</v>
       </c>
-      <c r="K5" s="248" t="s">
-        <v>802</v>
-      </c>
       <c r="L5" s="248" t="s">
+        <v>800</v>
+      </c>
+      <c r="M5" s="248" t="s">
         <v>801</v>
-      </c>
-      <c r="M5" s="248" t="s">
-        <v>802</v>
       </c>
       <c r="N5" s="216"/>
     </row>
@@ -35832,16 +35829,16 @@
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
       <c r="F50" s="72" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G50" s="72" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="H50" s="72" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I50" s="72" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="J50" s="72" t="s">
         <v>771</v>
@@ -35942,10 +35939,10 @@
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
       <c r="F53" s="72" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G53" s="72" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="H53" s="72" t="s">
         <v>771</v>
@@ -35954,10 +35951,10 @@
         <v>771</v>
       </c>
       <c r="J53" s="72" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="K53" s="72" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="L53" s="72" t="s">
         <v>771</v>

</xml_diff>

<commit_message>
fix/substanceState: Fix legacy calcium and acetaminophen data errors
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5432,10 +5432,10 @@
   <dimension ref="A1:HG88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="GI3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="GU4" sqref="GU4"/>
+      <selection pane="bottomRight" activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -14782,7 +14782,7 @@
       <c r="T29" s="88"/>
       <c r="U29" s="88"/>
       <c r="V29" s="88">
-        <v>1.8</v>
+        <v>0.8</v>
       </c>
       <c r="W29" s="81">
         <v>0.99</v>

</xml_diff>

<commit_message>
fix/substanceState: Valid PD def for epinephrine and chloride ratio
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5435,7 +5435,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z29" sqref="Z29"/>
+      <selection pane="bottomRight" activeCell="Z30" sqref="Z30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -14794,7 +14794,7 @@
         <v>291</v>
       </c>
       <c r="Z29" s="84">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="AA29" s="88"/>
       <c r="AB29" s="88"/>

</xml_diff>

<commit_message>
f/mmcdaniel-RASS: Update bolus action and tune sedation drugs
Give the option to specify the length of time over which a bolus will be
administered.  Default time of 2 s was unrealistically fast and was
causing peak plasma concentrations for most bolus drugs to be too high.

Increase default admin time to 10 s and overwrite with user provided
admin time if provided.

Introduce scenarios for propofol, midazolam, and ketamine sedation and
anesthesia induction.
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6462" uniqueCount="862">
   <si>
     <t>Name</t>
   </si>
@@ -2115,9 +2115,6 @@
     <t>0.7 mL/min kg</t>
   </si>
   <si>
-    <t>2.0 1/min</t>
-  </si>
-  <si>
     <t>0.0314 g/L</t>
   </si>
   <si>
@@ -2202,18 +2199,12 @@
     <t>37.0 mL/min kg</t>
   </si>
   <si>
-    <t>195 mL/min kg</t>
-  </si>
-  <si>
     <t>420 mL/min kg</t>
   </si>
   <si>
     <t>27.5 mL/min kg</t>
   </si>
   <si>
-    <t>16 mL/min kg</t>
-  </si>
-  <si>
     <t>4.0 mL/min kg</t>
   </si>
   <si>
@@ -2226,12 +2217,6 @@
     <t>0.1 mL/min kg</t>
   </si>
   <si>
-    <t>13000 mL/min kg</t>
-  </si>
-  <si>
-    <t>40.0 mL/min kg</t>
-  </si>
-  <si>
     <t>Blood_ABNegative</t>
   </si>
   <si>
@@ -2394,9 +2379,6 @@
     <t>[0; 0.0 ug/L]</t>
   </si>
   <si>
-    <t>[1; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.8; 0.5 ug/mL]</t>
   </si>
   <si>
@@ -2409,9 +2391,6 @@
     <t>[-0.05; 4 ug/L]</t>
   </si>
   <si>
-    <t>[-0.25; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.15; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2445,12 +2424,6 @@
     <t>[-0.01; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0.2; 0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.3; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.06; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2487,9 +2460,6 @@
     <t>https://www.ncbi.nlm.nih.gov/pubmed/2875674; http://anesthesiology.pubs.asahq.org/article.aspx?articleid=1936490</t>
   </si>
   <si>
-    <t>[-0.5; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.5; 0.0588 ug/mL]</t>
   </si>
   <si>
@@ -2514,9 +2484,6 @@
     <t>[-0.33; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[0; 0.0588 ug/mL]</t>
   </si>
   <si>
@@ -2529,18 +2496,12 @@
     <t>[-0.95; 4 ug/L]</t>
   </si>
   <si>
-    <t>[-1; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-1; 0.075 ug/mL]</t>
   </si>
   <si>
     <t>[-0.5; 0.5 ug/mL]</t>
   </si>
   <si>
-    <t>[1; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[0.5; 0.9 ug/L]</t>
   </si>
   <si>
@@ -2550,12 +2511,6 @@
     <t>[-0.1; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0.25; 0.4319 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.5; 0.0558 ug/mL]</t>
-  </si>
-  <si>
     <t>[-0.1; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2571,9 +2526,6 @@
     <t>[1.0; 4 ug/L]</t>
   </si>
   <si>
-    <t>[0.75; 0.4319 ug/mL]</t>
-  </si>
-  <si>
     <t>[0.85; 0.075 ug/mL]</t>
   </si>
   <si>
@@ -2589,25 +2541,85 @@
     <t>[0.5; 0.4 ug/L]</t>
   </si>
   <si>
-    <t>[-0.25; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.15; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.5; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-1; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[-0.55; 1.99 ug/mL]</t>
-  </si>
-  <si>
-    <t>[0.7; 1.99 ug/mL]</t>
-  </si>
-  <si>
     <t>[0; 1.5 ug/L]</t>
+  </si>
+  <si>
+    <t>3350 mL/min kg</t>
+  </si>
+  <si>
+    <t>28.0 mL/min kg</t>
+  </si>
+  <si>
+    <t>[1.0; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-1; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.75; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1.0; 1.2 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.25; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.15; 2.0 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.5; 2.0 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.5; 1.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.75; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.25; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.6; 0.5 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.4; 0.3 ug/mL]</t>
+  </si>
+  <si>
+    <t>[1; 0.25 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.5; 0.4 ug/mL]</t>
+  </si>
+  <si>
+    <t>[-0.6; 0.3 ug/mL]</t>
+  </si>
+  <si>
+    <t>277 mL/min kg</t>
+  </si>
+  <si>
+    <t>20 mL/min kg</t>
+  </si>
+  <si>
+    <t>3.0 1/min</t>
+  </si>
+  <si>
+    <t>[1; 0.4 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.1; 0.75 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.25; 0.75 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.6; 0.2 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0; 0.4 ug/mL]</t>
+  </si>
+  <si>
+    <t>[0.4; 0.75 ug/mL]</t>
   </si>
 </sst>
 </file>
@@ -5558,10 +5570,10 @@
   <dimension ref="A1:HG86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CQ32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="BV36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DK47" sqref="DK47"/>
+      <selection pane="bottomRight" activeCell="CU4" sqref="CU4:CU60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6528,7 +6540,7 @@
         <v>165</v>
       </c>
       <c r="BZ2" s="96" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="CA2" s="257" t="s">
         <v>190</v>
@@ -6555,16 +6567,16 @@
         <v>50</v>
       </c>
       <c r="CI2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CJ2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CK2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CL2" s="96" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="CM2" s="96" t="s">
         <v>51</v>
@@ -6627,16 +6639,16 @@
         <v>47</v>
       </c>
       <c r="DG2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DH2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DI2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DJ2" s="96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="DK2" s="96" t="s">
         <v>48</v>
@@ -6759,16 +6771,16 @@
         <v>648</v>
       </c>
       <c r="EY2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="EZ2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="FA2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="FB2" s="96" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="FC2" s="96" t="s">
         <v>637</v>
@@ -6879,64 +6891,64 @@
         <v>563</v>
       </c>
       <c r="GM2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GN2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GO2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GP2" s="101" t="s">
+        <v>732</v>
+      </c>
+      <c r="GQ2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GR2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GS2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GT2" s="101" t="s">
+        <v>734</v>
+      </c>
+      <c r="GU2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GN2" s="101" t="s">
+      <c r="GV2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GO2" s="101" t="s">
+      <c r="GW2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GP2" s="101" t="s">
+      <c r="GX2" s="101" t="s">
         <v>737</v>
       </c>
-      <c r="GQ2" s="101" t="s">
-        <v>739</v>
-      </c>
-      <c r="GR2" s="101" t="s">
-        <v>739</v>
-      </c>
-      <c r="GS2" s="101" t="s">
-        <v>739</v>
-      </c>
-      <c r="GT2" s="101" t="s">
-        <v>739</v>
-      </c>
-      <c r="GU2" s="101" t="s">
-        <v>742</v>
-      </c>
-      <c r="GV2" s="101" t="s">
-        <v>742</v>
-      </c>
-      <c r="GW2" s="101" t="s">
-        <v>742</v>
-      </c>
-      <c r="GX2" s="101" t="s">
-        <v>742</v>
-      </c>
       <c r="GY2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="GZ2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="HA2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="HB2" s="101" t="s">
+        <v>730</v>
+      </c>
+      <c r="HC2" s="101" t="s">
         <v>735</v>
       </c>
-      <c r="GZ2" s="101" t="s">
+      <c r="HD2" s="101" t="s">
         <v>735</v>
       </c>
-      <c r="HA2" s="101" t="s">
+      <c r="HE2" s="101" t="s">
         <v>735</v>
       </c>
-      <c r="HB2" s="101" t="s">
+      <c r="HF2" s="101" t="s">
         <v>735</v>
-      </c>
-      <c r="HC2" s="101" t="s">
-        <v>740</v>
-      </c>
-      <c r="HD2" s="101" t="s">
-        <v>740</v>
-      </c>
-      <c r="HE2" s="101" t="s">
-        <v>740</v>
-      </c>
-      <c r="HF2" s="101" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="3" spans="1:214" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -7993,31 +8005,31 @@
       <c r="GK5" s="178"/>
       <c r="GL5" s="178"/>
       <c r="GM5" s="245" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="GN5" s="246"/>
       <c r="GO5" s="246"/>
       <c r="GP5" s="246"/>
       <c r="GQ5" s="245" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="GR5" s="246"/>
       <c r="GS5" s="246"/>
       <c r="GT5" s="246"/>
       <c r="GU5" s="245" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="GV5" s="246"/>
       <c r="GW5" s="246"/>
       <c r="GX5" s="246"/>
       <c r="GY5" s="245" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="GZ5" s="246"/>
       <c r="HA5" s="246"/>
       <c r="HB5" s="246"/>
       <c r="HC5" s="245" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="HD5" s="221"/>
       <c r="HE5" s="221"/>
@@ -8116,7 +8128,7 @@
       <c r="BX6" s="167"/>
       <c r="BY6" s="252"/>
       <c r="BZ6" s="107" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="CA6" s="258" t="s">
         <v>124</v>
@@ -8249,19 +8261,19 @@
       <c r="GS6" s="246"/>
       <c r="GT6" s="246"/>
       <c r="GU6" s="249" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="GV6" s="246"/>
       <c r="GW6" s="246"/>
       <c r="GX6" s="246"/>
       <c r="GY6" s="249" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="GZ6" s="246"/>
       <c r="HA6" s="246"/>
       <c r="HB6" s="246"/>
       <c r="HC6" s="249" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="HD6" s="221"/>
       <c r="HE6" s="221"/>
@@ -9060,7 +9072,7 @@
       <c r="BX10" s="167"/>
       <c r="BY10" s="252"/>
       <c r="BZ10" s="107" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="CA10" s="258" t="s">
         <v>312</v>
@@ -9075,7 +9087,7 @@
       <c r="CG10" s="107"/>
       <c r="CH10" s="107"/>
       <c r="CI10" s="107" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="CJ10" s="107"/>
       <c r="CK10" s="107"/>
@@ -9111,7 +9123,7 @@
       <c r="DE10" s="107"/>
       <c r="DF10" s="107"/>
       <c r="DG10" s="107" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="DH10" s="107"/>
       <c r="DI10" s="107"/>
@@ -9181,7 +9193,7 @@
       </c>
       <c r="EX10" s="107"/>
       <c r="EY10" s="107" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="EZ10" s="107"/>
       <c r="FA10" s="107"/>
@@ -9237,31 +9249,31 @@
       <c r="GK10" s="178"/>
       <c r="GL10" s="178"/>
       <c r="GM10" s="245" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="GN10" s="246"/>
       <c r="GO10" s="246"/>
       <c r="GP10" s="246"/>
       <c r="GQ10" s="245" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="GR10" s="246"/>
       <c r="GS10" s="246"/>
       <c r="GT10" s="246"/>
       <c r="GU10" s="245" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="GV10" s="246"/>
       <c r="GW10" s="246"/>
       <c r="GX10" s="246"/>
       <c r="GY10" s="245" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="GZ10" s="246"/>
       <c r="HA10" s="246"/>
       <c r="HB10" s="246"/>
       <c r="HC10" s="245" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="HD10" s="221"/>
       <c r="HE10" s="221"/>
@@ -11789,7 +11801,7 @@
       <c r="CS19" s="107"/>
       <c r="CT19" s="107"/>
       <c r="CU19" s="107">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="CV19" s="107"/>
       <c r="CW19" s="107"/>
@@ -12059,7 +12071,7 @@
       <c r="CK20" s="107"/>
       <c r="CL20" s="107"/>
       <c r="CM20" s="107" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="CN20" s="107"/>
       <c r="CO20" s="107"/>
@@ -12071,13 +12083,13 @@
       <c r="CS20" s="107"/>
       <c r="CT20" s="107"/>
       <c r="CU20" s="107" t="s">
-        <v>722</v>
+        <v>853</v>
       </c>
       <c r="CV20" s="107"/>
       <c r="CW20" s="107"/>
       <c r="CX20" s="107"/>
       <c r="CY20" s="107" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="CZ20" s="107"/>
       <c r="DA20" s="107"/>
@@ -12089,13 +12101,13 @@
       <c r="DE20" s="107"/>
       <c r="DF20" s="107"/>
       <c r="DG20" s="107" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="DH20" s="107"/>
       <c r="DI20" s="107"/>
       <c r="DJ20" s="107"/>
       <c r="DK20" s="107" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="DL20" s="107"/>
       <c r="DM20" s="107"/>
@@ -12125,13 +12137,13 @@
       <c r="EC20" s="107"/>
       <c r="ED20" s="107"/>
       <c r="EE20" s="107" t="s">
-        <v>730</v>
+        <v>836</v>
       </c>
       <c r="EF20" s="107"/>
       <c r="EG20" s="107"/>
       <c r="EH20" s="107"/>
       <c r="EI20" s="107" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="EJ20" s="107"/>
       <c r="EK20" s="107"/>
@@ -12149,7 +12161,7 @@
       <c r="ES20" s="107"/>
       <c r="ET20" s="107"/>
       <c r="EU20" s="107" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="EV20" s="107"/>
       <c r="EW20" s="107"/>
@@ -12161,7 +12173,7 @@
       <c r="FA20" s="107"/>
       <c r="FB20" s="107"/>
       <c r="FC20" s="107" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="FD20" s="107"/>
       <c r="FE20" s="107"/>
@@ -12312,7 +12324,7 @@
       <c r="BX21" s="167"/>
       <c r="BY21" s="252"/>
       <c r="BZ21" s="107" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="CA21" s="258" t="s">
         <v>528</v>
@@ -12351,7 +12363,7 @@
       <c r="CW21" s="107"/>
       <c r="CX21" s="107"/>
       <c r="CY21" s="107" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="CZ21" s="107"/>
       <c r="DA21" s="107"/>
@@ -12363,7 +12375,7 @@
       <c r="DE21" s="107"/>
       <c r="DF21" s="107"/>
       <c r="DG21" s="107" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="DH21" s="107"/>
       <c r="DI21" s="107"/>
@@ -12437,7 +12449,7 @@
         <v>656</v>
       </c>
       <c r="EY21" s="107" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EZ21" s="107"/>
       <c r="FA21" s="107"/>
@@ -12572,7 +12584,7 @@
         <v>591</v>
       </c>
       <c r="AV22" s="162" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="AW22" s="162"/>
       <c r="AX22" s="167"/>
@@ -12621,13 +12633,13 @@
       <c r="CG22" s="107"/>
       <c r="CH22" s="107"/>
       <c r="CI22" s="107" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="CJ22" s="107"/>
       <c r="CK22" s="107"/>
       <c r="CL22" s="107"/>
       <c r="CM22" s="107" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="CN22" s="107"/>
       <c r="CO22" s="107"/>
@@ -12639,7 +12651,7 @@
       <c r="CS22" s="107"/>
       <c r="CT22" s="107"/>
       <c r="CU22" s="107" t="s">
-        <v>725</v>
+        <v>854</v>
       </c>
       <c r="CV22" s="107"/>
       <c r="CW22" s="107"/>
@@ -12657,19 +12669,19 @@
       <c r="DE22" s="107"/>
       <c r="DF22" s="107"/>
       <c r="DG22" s="107" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="DH22" s="107"/>
       <c r="DI22" s="107"/>
       <c r="DJ22" s="107"/>
       <c r="DK22" s="107" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="DL22" s="107"/>
       <c r="DM22" s="107"/>
       <c r="DN22" s="107"/>
       <c r="DO22" s="107" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="DP22" s="107"/>
       <c r="DQ22" s="107" t="s">
@@ -12699,13 +12711,13 @@
       <c r="EC22" s="107"/>
       <c r="ED22" s="107"/>
       <c r="EE22" s="107" t="s">
-        <v>731</v>
+        <v>837</v>
       </c>
       <c r="EF22" s="107"/>
       <c r="EG22" s="107"/>
       <c r="EH22" s="107"/>
       <c r="EI22" s="107" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="EJ22" s="107"/>
       <c r="EK22" s="107"/>
@@ -12717,7 +12729,7 @@
       <c r="EO22" s="107"/>
       <c r="EP22" s="107"/>
       <c r="EQ22" s="107" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="ER22" s="107"/>
       <c r="ES22" s="107"/>
@@ -12733,13 +12745,13 @@
         <v>656</v>
       </c>
       <c r="EY22" s="107" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EZ22" s="107"/>
       <c r="FA22" s="107"/>
       <c r="FB22" s="107"/>
       <c r="FC22" s="107" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="FD22" s="107"/>
       <c r="FE22" s="107"/>
@@ -13372,7 +13384,7 @@
       <c r="BX24" s="167"/>
       <c r="BY24" s="252"/>
       <c r="BZ24" s="107" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="CA24" s="258" t="str">
         <f>CA21</f>
@@ -13607,7 +13619,7 @@
         <v>656</v>
       </c>
       <c r="EY24" s="107" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EZ24" s="107"/>
       <c r="FA24" s="107"/>
@@ -15201,7 +15213,7 @@
     </row>
     <row r="30" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="79" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="B30" s="222"/>
       <c r="C30" s="223" t="s">
@@ -15691,7 +15703,7 @@
     </row>
     <row r="31" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="80" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="B31" s="99"/>
       <c r="C31" s="99"/>
@@ -15887,31 +15899,31 @@
       <c r="GK31" s="177"/>
       <c r="GL31" s="177"/>
       <c r="GM31" s="245" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="GN31" s="245"/>
       <c r="GO31" s="245"/>
       <c r="GP31" s="245"/>
       <c r="GQ31" s="245" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="GR31" s="245"/>
       <c r="GS31" s="245"/>
       <c r="GT31" s="245"/>
       <c r="GU31" s="245" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="GV31" s="245"/>
       <c r="GW31" s="245"/>
       <c r="GX31" s="245"/>
       <c r="GY31" s="245" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="GZ31" s="245"/>
       <c r="HA31" s="245"/>
       <c r="HB31" s="245"/>
       <c r="HC31" s="245" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="HD31" s="220"/>
       <c r="HE31" s="220"/>
@@ -15919,7 +15931,7 @@
     </row>
     <row r="32" spans="1:214" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="80" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="B32" s="99"/>
       <c r="C32" s="99"/>
@@ -16115,31 +16127,31 @@
       <c r="GK32" s="177"/>
       <c r="GL32" s="177"/>
       <c r="GM32" s="245" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="GN32" s="245"/>
       <c r="GO32" s="245"/>
       <c r="GP32" s="245"/>
       <c r="GQ32" s="245" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="GR32" s="245"/>
       <c r="GS32" s="245"/>
       <c r="GT32" s="245"/>
       <c r="GU32" s="245" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="GV32" s="245"/>
       <c r="GW32" s="245"/>
       <c r="GX32" s="245"/>
       <c r="GY32" s="245" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="GZ32" s="245"/>
       <c r="HA32" s="245"/>
       <c r="HB32" s="245"/>
       <c r="HC32" s="245" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="HD32" s="220"/>
       <c r="HE32" s="220"/>
@@ -16765,7 +16777,7 @@
       <c r="DE34" s="107"/>
       <c r="DF34" s="107"/>
       <c r="DG34" s="107" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="DH34" s="107"/>
       <c r="DI34" s="107"/>
@@ -17091,7 +17103,7 @@
       <c r="EW35" s="107"/>
       <c r="EX35" s="107"/>
       <c r="EY35" s="107" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="EZ35" s="107"/>
       <c r="FA35" s="107"/>
@@ -17559,7 +17571,7 @@
         <v>0</v>
       </c>
       <c r="CU37" s="107">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="CV37" s="107">
         <f t="shared" si="3"/>
@@ -17912,7 +17924,7 @@
       <c r="DE38" s="107"/>
       <c r="DF38" s="107"/>
       <c r="DG38" s="107" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="DH38" s="107"/>
       <c r="DI38" s="107"/>
@@ -19410,7 +19422,7 @@
       <c r="CK43" s="111"/>
       <c r="CL43" s="111"/>
       <c r="CM43" s="111" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="CN43" s="111"/>
       <c r="CO43" s="111"/>
@@ -19422,7 +19434,7 @@
       <c r="CS43" s="111"/>
       <c r="CT43" s="111"/>
       <c r="CU43" s="111" t="s">
-        <v>693</v>
+        <v>855</v>
       </c>
       <c r="CV43" s="111"/>
       <c r="CW43" s="111"/>
@@ -19504,7 +19516,7 @@
       <c r="EW43" s="185"/>
       <c r="EX43" s="185"/>
       <c r="EY43" s="209" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="EZ43" s="185"/>
       <c r="FA43" s="185"/>
@@ -19738,7 +19750,7 @@
       <c r="EC44" s="111"/>
       <c r="ED44" s="111"/>
       <c r="EE44" s="111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="EF44" s="111"/>
       <c r="EG44" s="111"/>
@@ -19832,7 +19844,7 @@
     </row>
     <row r="45" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="157" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B45" s="110"/>
       <c r="C45" s="110"/>
@@ -19871,7 +19883,7 @@
       <c r="AJ45" s="92"/>
       <c r="AK45" s="92"/>
       <c r="AL45" s="165" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="AM45" s="162"/>
       <c r="AN45" s="162"/>
@@ -19913,112 +19925,112 @@
       <c r="BX45" s="166"/>
       <c r="BY45" s="250"/>
       <c r="BZ45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CA45" s="208" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CB45" s="111"/>
       <c r="CC45" s="111"/>
       <c r="CD45" s="111"/>
       <c r="CE45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CF45" s="111"/>
       <c r="CG45" s="111"/>
       <c r="CH45" s="111"/>
       <c r="CI45" s="111" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="CJ45" s="111"/>
       <c r="CK45" s="111"/>
       <c r="CL45" s="111"/>
       <c r="CM45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CN45" s="111"/>
       <c r="CO45" s="111"/>
       <c r="CP45" s="111"/>
       <c r="CQ45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CR45" s="111"/>
       <c r="CS45" s="111"/>
       <c r="CT45" s="111"/>
       <c r="CU45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CV45" s="111"/>
       <c r="CW45" s="111"/>
       <c r="CX45" s="111"/>
       <c r="CY45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="CZ45" s="111"/>
       <c r="DA45" s="111"/>
       <c r="DB45" s="111"/>
       <c r="DC45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DD45" s="111"/>
       <c r="DE45" s="111"/>
       <c r="DF45" s="111"/>
       <c r="DG45" s="111" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="DH45" s="111"/>
       <c r="DI45" s="111"/>
       <c r="DJ45" s="111"/>
       <c r="DK45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DL45" s="111"/>
       <c r="DM45" s="111"/>
       <c r="DN45" s="111"/>
       <c r="DO45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DP45" s="111"/>
       <c r="DQ45" s="111"/>
       <c r="DR45" s="111"/>
       <c r="DS45" s="111" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="DT45" s="111"/>
       <c r="DU45" s="111"/>
       <c r="DV45" s="111"/>
       <c r="DW45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="DX45" s="111"/>
       <c r="DY45" s="111"/>
       <c r="DZ45" s="111"/>
       <c r="EA45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EB45" s="111"/>
       <c r="EC45" s="111"/>
       <c r="ED45" s="111"/>
       <c r="EE45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EF45" s="111"/>
       <c r="EG45" s="111"/>
       <c r="EH45" s="111"/>
       <c r="EI45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EJ45" s="111"/>
       <c r="EK45" s="111"/>
       <c r="EL45" s="111"/>
       <c r="EM45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EN45" s="111"/>
       <c r="EO45" s="111"/>
       <c r="EP45" s="111"/>
       <c r="EQ45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="ER45" s="185"/>
       <c r="ES45" s="185"/>
@@ -20028,13 +20040,13 @@
       <c r="EW45" s="185"/>
       <c r="EX45" s="185"/>
       <c r="EY45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EZ45" s="185"/>
       <c r="FA45" s="185"/>
       <c r="FB45" s="185"/>
       <c r="FC45" s="111" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="FD45" s="185"/>
       <c r="FE45" s="185"/>
@@ -20133,14 +20145,14 @@
       <c r="AJ46" s="89"/>
       <c r="AK46" s="89"/>
       <c r="AL46" s="165" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="AM46" s="162"/>
       <c r="AN46" s="162" t="s">
         <v>285</v>
       </c>
       <c r="AO46" s="162" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="AP46" s="162"/>
       <c r="AQ46" s="162"/>
@@ -20179,112 +20191,112 @@
       <c r="BX46" s="167"/>
       <c r="BY46" s="252"/>
       <c r="BZ46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA46" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB46" s="111"/>
       <c r="CC46" s="111"/>
       <c r="CD46" s="111"/>
       <c r="CE46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF46" s="111"/>
       <c r="CG46" s="111"/>
       <c r="CH46" s="111"/>
       <c r="CI46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ46" s="111"/>
       <c r="CK46" s="111"/>
       <c r="CL46" s="111"/>
       <c r="CM46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CN46" s="111"/>
       <c r="CO46" s="111"/>
       <c r="CP46" s="111"/>
       <c r="CQ46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR46" s="111"/>
       <c r="CS46" s="111"/>
       <c r="CT46" s="111"/>
       <c r="CU46" s="111" t="s">
-        <v>786</v>
+        <v>856</v>
       </c>
       <c r="CV46" s="111"/>
       <c r="CW46" s="111"/>
       <c r="CX46" s="111"/>
       <c r="CY46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CZ46" s="111"/>
       <c r="DA46" s="111"/>
       <c r="DB46" s="111"/>
       <c r="DC46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DD46" s="111"/>
       <c r="DE46" s="111"/>
       <c r="DF46" s="111"/>
       <c r="DG46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH46" s="111"/>
       <c r="DI46" s="111"/>
       <c r="DJ46" s="111"/>
       <c r="DK46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL46" s="111"/>
       <c r="DM46" s="111"/>
       <c r="DN46" s="111"/>
       <c r="DO46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP46" s="111"/>
       <c r="DQ46" s="111"/>
       <c r="DR46" s="111"/>
       <c r="DS46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT46" s="111"/>
       <c r="DU46" s="111"/>
       <c r="DV46" s="111"/>
       <c r="DW46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX46" s="111"/>
       <c r="DY46" s="111"/>
       <c r="DZ46" s="111"/>
       <c r="EA46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB46" s="111"/>
       <c r="EC46" s="111"/>
       <c r="ED46" s="111"/>
       <c r="EE46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EF46" s="111"/>
       <c r="EG46" s="111"/>
       <c r="EH46" s="111"/>
       <c r="EI46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ46" s="111"/>
       <c r="EK46" s="111"/>
       <c r="EL46" s="111"/>
       <c r="EM46" s="111" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="EN46" s="111"/>
       <c r="EO46" s="111"/>
       <c r="EP46" s="111"/>
       <c r="EQ46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER46" s="111"/>
       <c r="ES46" s="111"/>
@@ -20294,13 +20306,13 @@
       <c r="EW46" s="111"/>
       <c r="EX46" s="111"/>
       <c r="EY46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ46" s="111"/>
       <c r="FA46" s="111"/>
       <c r="FB46" s="111"/>
       <c r="FC46" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD46" s="111"/>
       <c r="FE46" s="111"/>
@@ -20411,7 +20423,7 @@
         <v>283</v>
       </c>
       <c r="AL47" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM47" s="162"/>
       <c r="AN47" s="162"/>
@@ -20501,112 +20513,112 @@
         <v>283</v>
       </c>
       <c r="BZ47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA47" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB47" s="111"/>
       <c r="CC47" s="111"/>
       <c r="CD47" s="111"/>
       <c r="CE47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF47" s="111"/>
       <c r="CG47" s="111"/>
       <c r="CH47" s="111"/>
       <c r="CI47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ47" s="111"/>
       <c r="CK47" s="111"/>
       <c r="CL47" s="111"/>
       <c r="CM47" s="111" t="s">
-        <v>844</v>
+        <v>829</v>
       </c>
       <c r="CN47" s="111"/>
       <c r="CO47" s="111"/>
       <c r="CP47" s="111"/>
       <c r="CQ47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR47" s="111"/>
       <c r="CS47" s="111"/>
       <c r="CT47" s="111"/>
       <c r="CU47" s="111" t="s">
-        <v>845</v>
+        <v>779</v>
       </c>
       <c r="CV47" s="111"/>
       <c r="CW47" s="111"/>
       <c r="CX47" s="111"/>
       <c r="CY47" s="111" t="s">
-        <v>784</v>
+        <v>846</v>
       </c>
       <c r="CZ47" s="111"/>
       <c r="DA47" s="111"/>
       <c r="DB47" s="111"/>
       <c r="DC47" s="111" t="s">
-        <v>846</v>
+        <v>830</v>
       </c>
       <c r="DD47" s="111"/>
       <c r="DE47" s="111"/>
       <c r="DF47" s="111"/>
       <c r="DG47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH47" s="111"/>
       <c r="DI47" s="111"/>
       <c r="DJ47" s="111"/>
       <c r="DK47" s="111" t="s">
-        <v>857</v>
+        <v>835</v>
       </c>
       <c r="DL47" s="111"/>
       <c r="DM47" s="111"/>
       <c r="DN47" s="111"/>
       <c r="DO47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP47" s="111"/>
       <c r="DQ47" s="111"/>
       <c r="DR47" s="111"/>
       <c r="DS47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT47" s="111"/>
       <c r="DU47" s="111"/>
       <c r="DV47" s="111"/>
       <c r="DW47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX47" s="111"/>
       <c r="DY47" s="111"/>
       <c r="DZ47" s="111"/>
       <c r="EA47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB47" s="111"/>
       <c r="EC47" s="111"/>
       <c r="ED47" s="111"/>
       <c r="EE47" s="111" t="s">
-        <v>784</v>
+        <v>838</v>
       </c>
       <c r="EF47" s="111"/>
       <c r="EG47" s="111"/>
       <c r="EH47" s="111"/>
       <c r="EI47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ47" s="111"/>
       <c r="EK47" s="111"/>
       <c r="EL47" s="111"/>
       <c r="EM47" s="111" t="s">
-        <v>847</v>
+        <v>831</v>
       </c>
       <c r="EN47" s="111"/>
       <c r="EO47" s="111"/>
       <c r="EP47" s="111"/>
       <c r="EQ47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER47" s="111"/>
       <c r="ES47" s="111"/>
@@ -20616,13 +20628,13 @@
       <c r="EW47" s="111"/>
       <c r="EX47" s="207"/>
       <c r="EY47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ47" s="208"/>
       <c r="FA47" s="208"/>
       <c r="FB47" s="208"/>
       <c r="FC47" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD47" s="111"/>
       <c r="FE47" s="111"/>
@@ -20721,7 +20733,7 @@
       <c r="AJ48" s="89"/>
       <c r="AK48" s="89"/>
       <c r="AL48" s="165" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="AM48" s="162"/>
       <c r="AN48" s="162"/>
@@ -20763,112 +20775,112 @@
       <c r="BX48" s="167"/>
       <c r="BY48" s="252"/>
       <c r="BZ48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA48" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB48" s="111"/>
       <c r="CC48" s="111"/>
       <c r="CD48" s="111"/>
       <c r="CE48" s="111" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="CF48" s="111"/>
       <c r="CG48" s="111"/>
       <c r="CH48" s="111"/>
       <c r="CI48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ48" s="111"/>
       <c r="CK48" s="111"/>
       <c r="CL48" s="111"/>
       <c r="CM48" s="111" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="CN48" s="111"/>
       <c r="CO48" s="111"/>
       <c r="CP48" s="111"/>
       <c r="CQ48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR48" s="111"/>
       <c r="CS48" s="111"/>
       <c r="CT48" s="111"/>
       <c r="CU48" s="111" t="s">
-        <v>784</v>
+        <v>857</v>
       </c>
       <c r="CV48" s="111"/>
       <c r="CW48" s="111"/>
       <c r="CX48" s="111"/>
       <c r="CY48" s="111" t="s">
-        <v>791</v>
+        <v>847</v>
       </c>
       <c r="CZ48" s="111"/>
       <c r="DA48" s="111"/>
       <c r="DB48" s="111"/>
       <c r="DC48" s="111" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
       <c r="DD48" s="111"/>
       <c r="DE48" s="111"/>
       <c r="DF48" s="111"/>
       <c r="DG48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH48" s="111"/>
       <c r="DI48" s="111"/>
       <c r="DJ48" s="111"/>
       <c r="DK48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL48" s="111"/>
       <c r="DM48" s="111"/>
       <c r="DN48" s="111"/>
       <c r="DO48" s="111" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="DP48" s="111"/>
       <c r="DQ48" s="111"/>
       <c r="DR48" s="111"/>
       <c r="DS48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT48" s="111"/>
       <c r="DU48" s="111"/>
       <c r="DV48" s="111"/>
       <c r="DW48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX48" s="111"/>
       <c r="DY48" s="111"/>
       <c r="DZ48" s="111"/>
       <c r="EA48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB48" s="111"/>
       <c r="EC48" s="111"/>
       <c r="ED48" s="111"/>
       <c r="EE48" s="111" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
       <c r="EF48" s="111"/>
       <c r="EG48" s="111"/>
       <c r="EH48" s="111"/>
       <c r="EI48" s="111" t="s">
-        <v>794</v>
+        <v>787</v>
       </c>
       <c r="EJ48" s="111"/>
       <c r="EK48" s="111"/>
       <c r="EL48" s="111"/>
       <c r="EM48" s="111" t="s">
-        <v>795</v>
+        <v>788</v>
       </c>
       <c r="EN48" s="111"/>
       <c r="EO48" s="111"/>
       <c r="EP48" s="111"/>
       <c r="EQ48" s="111" t="s">
-        <v>796</v>
+        <v>789</v>
       </c>
       <c r="ER48" s="111"/>
       <c r="ES48" s="111"/>
@@ -20878,13 +20890,13 @@
       <c r="EW48" s="111"/>
       <c r="EX48" s="111"/>
       <c r="EY48" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ48" s="111"/>
       <c r="FA48" s="111"/>
       <c r="FB48" s="111"/>
       <c r="FC48" s="111" t="s">
-        <v>797</v>
+        <v>790</v>
       </c>
       <c r="FD48" s="111"/>
       <c r="FE48" s="111"/>
@@ -20944,7 +20956,7 @@
     </row>
     <row r="49" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="62" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="B49" s="110"/>
       <c r="C49" s="110"/>
@@ -20983,7 +20995,7 @@
       <c r="AJ49" s="89"/>
       <c r="AK49" s="89"/>
       <c r="AL49" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM49" s="162"/>
       <c r="AN49" s="162"/>
@@ -21025,112 +21037,112 @@
       <c r="BX49" s="167"/>
       <c r="BY49" s="252"/>
       <c r="BZ49" s="111" t="s">
-        <v>798</v>
+        <v>791</v>
       </c>
       <c r="CA49" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB49" s="111"/>
       <c r="CC49" s="111"/>
       <c r="CD49" s="111"/>
       <c r="CE49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF49" s="111"/>
       <c r="CG49" s="111"/>
       <c r="CH49" s="111"/>
       <c r="CI49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ49" s="111"/>
       <c r="CK49" s="111"/>
       <c r="CL49" s="111"/>
       <c r="CM49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CN49" s="111"/>
       <c r="CO49" s="111"/>
       <c r="CP49" s="111"/>
       <c r="CQ49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR49" s="111"/>
       <c r="CS49" s="111"/>
       <c r="CT49" s="111"/>
       <c r="CU49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CV49" s="111"/>
       <c r="CW49" s="111"/>
       <c r="CX49" s="111"/>
       <c r="CY49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CZ49" s="111"/>
       <c r="DA49" s="111"/>
       <c r="DB49" s="111"/>
       <c r="DC49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DD49" s="111"/>
       <c r="DE49" s="111"/>
       <c r="DF49" s="111"/>
       <c r="DG49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH49" s="111"/>
       <c r="DI49" s="111"/>
       <c r="DJ49" s="111"/>
       <c r="DK49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL49" s="111"/>
       <c r="DM49" s="111"/>
       <c r="DN49" s="111"/>
       <c r="DO49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP49" s="111"/>
       <c r="DQ49" s="111"/>
       <c r="DR49" s="111"/>
       <c r="DS49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT49" s="111"/>
       <c r="DU49" s="111"/>
       <c r="DV49" s="111"/>
       <c r="DW49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX49" s="111"/>
       <c r="DY49" s="111"/>
       <c r="DZ49" s="111"/>
       <c r="EA49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB49" s="111"/>
       <c r="EC49" s="111"/>
       <c r="ED49" s="111"/>
       <c r="EE49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EF49" s="111"/>
       <c r="EG49" s="111"/>
       <c r="EH49" s="111"/>
       <c r="EI49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ49" s="111"/>
       <c r="EK49" s="111"/>
       <c r="EL49" s="111"/>
       <c r="EM49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EN49" s="111"/>
       <c r="EO49" s="111"/>
       <c r="EP49" s="111"/>
       <c r="EQ49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER49" s="111"/>
       <c r="ES49" s="111"/>
@@ -21140,13 +21152,13 @@
       <c r="EW49" s="111"/>
       <c r="EX49" s="207"/>
       <c r="EY49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ49" s="208"/>
       <c r="FA49" s="208"/>
       <c r="FB49" s="208"/>
       <c r="FC49" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD49" s="111"/>
       <c r="FE49" s="111"/>
@@ -21245,7 +21257,7 @@
       <c r="AJ50" s="89"/>
       <c r="AK50" s="89"/>
       <c r="AL50" s="165" t="s">
-        <v>799</v>
+        <v>792</v>
       </c>
       <c r="AM50" s="162"/>
       <c r="AN50" s="162"/>
@@ -21287,112 +21299,112 @@
       <c r="BX50" s="167"/>
       <c r="BY50" s="252"/>
       <c r="BZ50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA50" s="208" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="CB50" s="111"/>
       <c r="CC50" s="111"/>
       <c r="CD50" s="111"/>
       <c r="CE50" s="111" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="CF50" s="111"/>
       <c r="CG50" s="111"/>
       <c r="CH50" s="111"/>
       <c r="CI50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ50" s="111"/>
       <c r="CK50" s="111"/>
       <c r="CL50" s="111"/>
       <c r="CM50" s="111" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="CN50" s="111"/>
       <c r="CO50" s="111"/>
       <c r="CP50" s="111"/>
       <c r="CQ50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR50" s="111"/>
       <c r="CS50" s="111"/>
       <c r="CT50" s="111"/>
       <c r="CU50" s="111" t="s">
-        <v>803</v>
+        <v>858</v>
       </c>
       <c r="CV50" s="111"/>
       <c r="CW50" s="111"/>
       <c r="CX50" s="111"/>
       <c r="CY50" s="111" t="s">
-        <v>804</v>
+        <v>848</v>
       </c>
       <c r="CZ50" s="111"/>
       <c r="DA50" s="111"/>
       <c r="DB50" s="111"/>
       <c r="DC50" s="111" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="DD50" s="111"/>
       <c r="DE50" s="111"/>
       <c r="DF50" s="111"/>
       <c r="DG50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH50" s="111"/>
       <c r="DI50" s="111"/>
       <c r="DJ50" s="111"/>
       <c r="DK50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL50" s="111"/>
       <c r="DM50" s="111"/>
       <c r="DN50" s="111"/>
       <c r="DO50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP50" s="111"/>
       <c r="DQ50" s="111"/>
       <c r="DR50" s="111"/>
       <c r="DS50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT50" s="111"/>
       <c r="DU50" s="111"/>
       <c r="DV50" s="111"/>
       <c r="DW50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX50" s="111"/>
       <c r="DY50" s="111"/>
       <c r="DZ50" s="111"/>
       <c r="EA50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB50" s="111"/>
       <c r="EC50" s="111"/>
       <c r="ED50" s="111"/>
       <c r="EE50" s="111" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="EF50" s="111"/>
       <c r="EG50" s="111"/>
       <c r="EH50" s="111"/>
       <c r="EI50" s="111" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="EJ50" s="111"/>
       <c r="EK50" s="111"/>
       <c r="EL50" s="111"/>
       <c r="EM50" s="111" t="s">
-        <v>795</v>
+        <v>788</v>
       </c>
       <c r="EN50" s="111"/>
       <c r="EO50" s="111"/>
       <c r="EP50" s="111"/>
       <c r="EQ50" s="111" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="ER50" s="111"/>
       <c r="ES50" s="111"/>
@@ -21402,13 +21414,13 @@
       <c r="EW50" s="111"/>
       <c r="EX50" s="207"/>
       <c r="EY50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ50" s="208"/>
       <c r="FA50" s="208"/>
       <c r="FB50" s="208"/>
       <c r="FC50" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD50" s="111"/>
       <c r="FE50" s="111"/>
@@ -21468,7 +21480,7 @@
     </row>
     <row r="51" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="62" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B51" s="110"/>
       <c r="C51" s="110"/>
@@ -21507,7 +21519,7 @@
       <c r="AJ51" s="89"/>
       <c r="AK51" s="89"/>
       <c r="AL51" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM51" s="162"/>
       <c r="AN51" s="162"/>
@@ -21549,112 +21561,112 @@
       <c r="BX51" s="167"/>
       <c r="BY51" s="252"/>
       <c r="BZ51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA51" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB51" s="111"/>
       <c r="CC51" s="111"/>
       <c r="CD51" s="111"/>
       <c r="CE51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF51" s="111"/>
       <c r="CG51" s="111"/>
       <c r="CH51" s="111"/>
       <c r="CI51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ51" s="111"/>
       <c r="CK51" s="111"/>
       <c r="CL51" s="111"/>
       <c r="CM51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CN51" s="111"/>
       <c r="CO51" s="111"/>
       <c r="CP51" s="111"/>
       <c r="CQ51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR51" s="111"/>
       <c r="CS51" s="111"/>
       <c r="CT51" s="111"/>
       <c r="CU51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CV51" s="111"/>
       <c r="CW51" s="111"/>
       <c r="CX51" s="111"/>
       <c r="CY51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CZ51" s="111"/>
       <c r="DA51" s="111"/>
       <c r="DB51" s="111"/>
       <c r="DC51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DD51" s="111"/>
       <c r="DE51" s="111"/>
       <c r="DF51" s="111"/>
       <c r="DG51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH51" s="111"/>
       <c r="DI51" s="111"/>
       <c r="DJ51" s="111"/>
       <c r="DK51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL51" s="111"/>
       <c r="DM51" s="111"/>
       <c r="DN51" s="111"/>
       <c r="DO51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP51" s="111"/>
       <c r="DQ51" s="111"/>
       <c r="DR51" s="111"/>
       <c r="DS51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT51" s="111"/>
       <c r="DU51" s="111"/>
       <c r="DV51" s="111"/>
       <c r="DW51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX51" s="111"/>
       <c r="DY51" s="111"/>
       <c r="DZ51" s="111"/>
       <c r="EA51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB51" s="111"/>
       <c r="EC51" s="111"/>
       <c r="ED51" s="111"/>
       <c r="EE51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EF51" s="111"/>
       <c r="EG51" s="111"/>
       <c r="EH51" s="111"/>
       <c r="EI51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ51" s="111"/>
       <c r="EK51" s="111"/>
       <c r="EL51" s="111"/>
       <c r="EM51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EN51" s="111"/>
       <c r="EO51" s="111"/>
       <c r="EP51" s="111"/>
       <c r="EQ51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER51" s="111"/>
       <c r="ES51" s="111"/>
@@ -21664,13 +21676,13 @@
       <c r="EW51" s="111"/>
       <c r="EX51" s="207"/>
       <c r="EY51" s="111" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
       <c r="EZ51" s="208"/>
       <c r="FA51" s="208"/>
       <c r="FB51" s="208"/>
       <c r="FC51" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD51" s="111"/>
       <c r="FE51" s="111"/>
@@ -21769,7 +21781,7 @@
       <c r="AJ52" s="89"/>
       <c r="AK52" s="89"/>
       <c r="AL52" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM52" s="162"/>
       <c r="AN52" s="162"/>
@@ -21811,112 +21823,112 @@
       <c r="BX52" s="167"/>
       <c r="BY52" s="252"/>
       <c r="BZ52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA52" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB52" s="111"/>
       <c r="CC52" s="111"/>
       <c r="CD52" s="111"/>
       <c r="CE52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF52" s="111"/>
       <c r="CG52" s="111"/>
       <c r="CH52" s="111"/>
       <c r="CI52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ52" s="111"/>
       <c r="CK52" s="111"/>
       <c r="CL52" s="111"/>
       <c r="CM52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CN52" s="111"/>
       <c r="CO52" s="111"/>
       <c r="CP52" s="111"/>
       <c r="CQ52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR52" s="111"/>
       <c r="CS52" s="111"/>
       <c r="CT52" s="111"/>
       <c r="CU52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CV52" s="111"/>
       <c r="CW52" s="111"/>
       <c r="CX52" s="111"/>
       <c r="CY52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CZ52" s="111"/>
       <c r="DA52" s="111"/>
       <c r="DB52" s="111"/>
       <c r="DC52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DD52" s="111"/>
       <c r="DE52" s="111"/>
       <c r="DF52" s="111"/>
       <c r="DG52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH52" s="111"/>
       <c r="DI52" s="111"/>
       <c r="DJ52" s="111"/>
       <c r="DK52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL52" s="111"/>
       <c r="DM52" s="111"/>
       <c r="DN52" s="111"/>
       <c r="DO52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP52" s="111"/>
       <c r="DQ52" s="111"/>
       <c r="DR52" s="111"/>
       <c r="DS52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT52" s="111"/>
       <c r="DU52" s="111"/>
       <c r="DV52" s="111"/>
       <c r="DW52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX52" s="111"/>
       <c r="DY52" s="111"/>
       <c r="DZ52" s="111"/>
       <c r="EA52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB52" s="111"/>
       <c r="EC52" s="111"/>
       <c r="ED52" s="111"/>
       <c r="EE52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EF52" s="111"/>
       <c r="EG52" s="111"/>
       <c r="EH52" s="111"/>
       <c r="EI52" s="111" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="EJ52" s="111"/>
       <c r="EK52" s="111"/>
       <c r="EL52" s="111"/>
       <c r="EM52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EN52" s="111"/>
       <c r="EO52" s="111"/>
       <c r="EP52" s="111"/>
       <c r="EQ52" s="111" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="ER52" s="111"/>
       <c r="ES52" s="111"/>
@@ -21926,13 +21938,13 @@
       <c r="EW52" s="111"/>
       <c r="EX52" s="207"/>
       <c r="EY52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ52" s="208"/>
       <c r="FA52" s="208"/>
       <c r="FB52" s="208"/>
       <c r="FC52" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD52" s="111"/>
       <c r="FE52" s="111"/>
@@ -21992,7 +22004,7 @@
     </row>
     <row r="53" spans="1:214" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="62" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="B53" s="110"/>
       <c r="C53" s="110"/>
@@ -22043,7 +22055,7 @@
         <v>283</v>
       </c>
       <c r="AL53" s="165" t="s">
-        <v>848</v>
+        <v>832</v>
       </c>
       <c r="AM53" s="162"/>
       <c r="AN53" s="162"/>
@@ -22133,112 +22145,112 @@
         <v>283</v>
       </c>
       <c r="BZ53" s="111" t="s">
-        <v>849</v>
+        <v>833</v>
       </c>
       <c r="CA53" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB53" s="111"/>
       <c r="CC53" s="111"/>
       <c r="CD53" s="111"/>
       <c r="CE53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF53" s="111"/>
       <c r="CG53" s="111"/>
       <c r="CH53" s="111"/>
       <c r="CI53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ53" s="111"/>
       <c r="CK53" s="111"/>
       <c r="CL53" s="111"/>
       <c r="CM53" s="111" t="s">
-        <v>850</v>
+        <v>834</v>
       </c>
       <c r="CN53" s="111"/>
       <c r="CO53" s="111"/>
       <c r="CP53" s="111"/>
       <c r="CQ53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR53" s="111"/>
       <c r="CS53" s="111"/>
       <c r="CT53" s="111"/>
       <c r="CU53" s="111" t="s">
-        <v>845</v>
+        <v>859</v>
       </c>
       <c r="CV53" s="111"/>
       <c r="CW53" s="111"/>
       <c r="CX53" s="111"/>
       <c r="CY53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CZ53" s="111"/>
       <c r="DA53" s="111"/>
       <c r="DB53" s="111"/>
       <c r="DC53" s="111" t="s">
-        <v>846</v>
+        <v>830</v>
       </c>
       <c r="DD53" s="111"/>
       <c r="DE53" s="111"/>
       <c r="DF53" s="111"/>
       <c r="DG53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH53" s="111"/>
       <c r="DI53" s="111"/>
       <c r="DJ53" s="111"/>
       <c r="DK53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL53" s="111"/>
       <c r="DM53" s="111"/>
       <c r="DN53" s="111"/>
       <c r="DO53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP53" s="111"/>
       <c r="DQ53" s="111"/>
       <c r="DR53" s="111"/>
       <c r="DS53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT53" s="111"/>
       <c r="DU53" s="111"/>
       <c r="DV53" s="111"/>
       <c r="DW53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX53" s="111"/>
       <c r="DY53" s="111"/>
       <c r="DZ53" s="111"/>
       <c r="EA53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB53" s="111"/>
       <c r="EC53" s="111"/>
       <c r="ED53" s="111"/>
       <c r="EE53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EF53" s="111"/>
       <c r="EG53" s="111"/>
       <c r="EH53" s="111"/>
       <c r="EI53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ53" s="111"/>
       <c r="EK53" s="111"/>
       <c r="EL53" s="111"/>
       <c r="EM53" s="111" t="s">
-        <v>847</v>
+        <v>831</v>
       </c>
       <c r="EN53" s="111"/>
       <c r="EO53" s="111"/>
       <c r="EP53" s="111"/>
       <c r="EQ53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER53" s="111"/>
       <c r="ES53" s="111"/>
@@ -22248,13 +22260,13 @@
       <c r="EW53" s="111"/>
       <c r="EX53" s="207"/>
       <c r="EY53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ53" s="208"/>
       <c r="FA53" s="208"/>
       <c r="FB53" s="208"/>
       <c r="FC53" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD53" s="111"/>
       <c r="FE53" s="111"/>
@@ -22323,7 +22335,7 @@
       <c r="F54" s="110"/>
       <c r="G54" s="110"/>
       <c r="H54" s="110" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="I54" s="110" t="s">
         <v>545</v>
@@ -22357,7 +22369,7 @@
       <c r="AJ54" s="89"/>
       <c r="AK54" s="89"/>
       <c r="AL54" s="165" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="AM54" s="162"/>
       <c r="AN54" s="162"/>
@@ -22399,46 +22411,46 @@
       <c r="BX54" s="167"/>
       <c r="BY54" s="252"/>
       <c r="BZ54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA54" s="208" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="CB54" s="111"/>
       <c r="CC54" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD54" s="111" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="CE54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF54" s="111"/>
       <c r="CG54" s="111"/>
       <c r="CH54" s="111"/>
       <c r="CI54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ54" s="111"/>
       <c r="CK54" s="111"/>
       <c r="CL54" s="111"/>
       <c r="CM54" s="111" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="CN54" s="111"/>
       <c r="CO54" s="111" t="s">
-        <v>816</v>
+        <v>807</v>
       </c>
       <c r="CP54" s="111"/>
       <c r="CQ54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR54" s="111"/>
       <c r="CS54" s="111"/>
       <c r="CT54" s="111"/>
       <c r="CU54" s="111" t="s">
-        <v>817</v>
+        <v>851</v>
       </c>
       <c r="CV54" s="111"/>
       <c r="CW54" s="111" t="s">
@@ -22446,7 +22458,7 @@
       </c>
       <c r="CX54" s="111"/>
       <c r="CY54" s="111" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="CZ54" s="111" t="s">
         <v>547</v>
@@ -22456,7 +22468,7 @@
       </c>
       <c r="DB54" s="111"/>
       <c r="DC54" s="111" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="DD54" s="111" t="s">
         <v>546</v>
@@ -22464,47 +22476,47 @@
       <c r="DE54" s="111"/>
       <c r="DF54" s="111"/>
       <c r="DG54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH54" s="111"/>
       <c r="DI54" s="111"/>
       <c r="DJ54" s="111"/>
       <c r="DK54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL54" s="111"/>
       <c r="DM54" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN54" s="111" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="DO54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP54" s="111"/>
       <c r="DQ54" s="111"/>
       <c r="DR54" s="111"/>
       <c r="DS54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT54" s="111"/>
       <c r="DU54" s="111"/>
       <c r="DV54" s="111"/>
       <c r="DW54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX54" s="111"/>
       <c r="DY54" s="111"/>
       <c r="DZ54" s="111"/>
       <c r="EA54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB54" s="111"/>
       <c r="EC54" s="111"/>
       <c r="ED54" s="111"/>
       <c r="EE54" s="111" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
       <c r="EF54" s="111"/>
       <c r="EG54" s="111" t="s">
@@ -22512,7 +22524,7 @@
       </c>
       <c r="EH54" s="111"/>
       <c r="EI54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ54" s="111"/>
       <c r="EK54" s="111" t="s">
@@ -22520,13 +22532,13 @@
       </c>
       <c r="EL54" s="111"/>
       <c r="EM54" s="111" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="EN54" s="111"/>
       <c r="EO54" s="111"/>
       <c r="EP54" s="111"/>
       <c r="EQ54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER54" s="111"/>
       <c r="ES54" s="111" t="s">
@@ -22538,13 +22550,13 @@
       <c r="EW54" s="111"/>
       <c r="EX54" s="207"/>
       <c r="EY54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ54" s="208"/>
       <c r="FA54" s="208"/>
       <c r="FB54" s="208"/>
       <c r="FC54" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD54" s="111"/>
       <c r="FE54" s="111"/>
@@ -22613,7 +22625,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="110"/>
       <c r="H55" s="110" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="I55" s="110" t="s">
         <v>545</v>
@@ -22647,11 +22659,11 @@
       <c r="AJ55" s="89"/>
       <c r="AK55" s="89"/>
       <c r="AL55" s="165" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="AM55" s="162"/>
       <c r="AN55" s="162" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="AO55" s="162"/>
       <c r="AP55" s="162"/>
@@ -22691,46 +22703,46 @@
       <c r="BX55" s="167"/>
       <c r="BY55" s="252"/>
       <c r="BZ55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA55" s="208" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="CB55" s="111"/>
       <c r="CC55" s="111" t="s">
         <v>552</v>
       </c>
       <c r="CD55" s="111" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="CE55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF55" s="111"/>
       <c r="CG55" s="111"/>
       <c r="CH55" s="111"/>
       <c r="CI55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ55" s="111"/>
       <c r="CK55" s="111"/>
       <c r="CL55" s="111"/>
       <c r="CM55" s="111" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="CN55" s="111"/>
       <c r="CO55" s="111" t="s">
-        <v>816</v>
+        <v>807</v>
       </c>
       <c r="CP55" s="111"/>
       <c r="CQ55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR55" s="111"/>
       <c r="CS55" s="111"/>
       <c r="CT55" s="111"/>
       <c r="CU55" s="111" t="s">
-        <v>826</v>
+        <v>860</v>
       </c>
       <c r="CV55" s="111"/>
       <c r="CW55" s="111" t="s">
@@ -22738,13 +22750,13 @@
       </c>
       <c r="CX55" s="111"/>
       <c r="CY55" s="111" t="s">
-        <v>827</v>
+        <v>816</v>
       </c>
       <c r="CZ55" s="111"/>
       <c r="DA55" s="111"/>
       <c r="DB55" s="111"/>
       <c r="DC55" s="111" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="DD55" s="111" t="s">
         <v>546</v>
@@ -22752,65 +22764,65 @@
       <c r="DE55" s="111"/>
       <c r="DF55" s="111"/>
       <c r="DG55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH55" s="111"/>
       <c r="DI55" s="111"/>
       <c r="DJ55" s="111"/>
       <c r="DK55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL55" s="111"/>
       <c r="DM55" s="111" t="s">
         <v>549</v>
       </c>
       <c r="DN55" s="111" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="DO55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP55" s="111"/>
       <c r="DQ55" s="111"/>
       <c r="DR55" s="111"/>
       <c r="DS55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT55" s="111"/>
       <c r="DU55" s="111"/>
       <c r="DV55" s="111"/>
       <c r="DW55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX55" s="111"/>
       <c r="DY55" s="111"/>
       <c r="DZ55" s="111"/>
       <c r="EA55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB55" s="111"/>
       <c r="EC55" s="111"/>
       <c r="ED55" s="111"/>
       <c r="EE55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EF55" s="111"/>
       <c r="EG55" s="111"/>
       <c r="EH55" s="111"/>
       <c r="EI55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ55" s="111"/>
       <c r="EK55" s="111"/>
       <c r="EL55" s="111"/>
       <c r="EM55" s="111" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="EN55" s="111"/>
       <c r="EO55" s="111"/>
       <c r="EP55" s="111"/>
       <c r="EQ55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER55" s="111"/>
       <c r="ES55" s="111"/>
@@ -22820,13 +22832,13 @@
       <c r="EW55" s="111"/>
       <c r="EX55" s="207"/>
       <c r="EY55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ55" s="208"/>
       <c r="FA55" s="208"/>
       <c r="FB55" s="208"/>
       <c r="FC55" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD55" s="111"/>
       <c r="FE55" s="111"/>
@@ -22925,7 +22937,7 @@
       <c r="AJ56" s="89"/>
       <c r="AK56" s="89"/>
       <c r="AL56" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM56" s="162"/>
       <c r="AN56" s="162"/>
@@ -22967,112 +22979,112 @@
       <c r="BX56" s="167"/>
       <c r="BY56" s="252"/>
       <c r="BZ56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA56" s="208" t="s">
-        <v>828</v>
+        <v>817</v>
       </c>
       <c r="CB56" s="111"/>
       <c r="CC56" s="111"/>
       <c r="CD56" s="111"/>
       <c r="CE56" s="111" t="s">
-        <v>829</v>
+        <v>818</v>
       </c>
       <c r="CF56" s="111"/>
       <c r="CG56" s="111"/>
       <c r="CH56" s="111"/>
       <c r="CI56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ56" s="111"/>
       <c r="CK56" s="111"/>
       <c r="CL56" s="111"/>
       <c r="CM56" s="111" t="s">
-        <v>830</v>
+        <v>819</v>
       </c>
       <c r="CN56" s="111"/>
       <c r="CO56" s="111"/>
       <c r="CP56" s="111"/>
       <c r="CQ56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR56" s="111"/>
       <c r="CS56" s="111"/>
       <c r="CT56" s="111"/>
       <c r="CU56" s="111" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
       <c r="CV56" s="111"/>
       <c r="CW56" s="111"/>
       <c r="CX56" s="111"/>
       <c r="CY56" s="111" t="s">
-        <v>831</v>
+        <v>849</v>
       </c>
       <c r="CZ56" s="111"/>
       <c r="DA56" s="111"/>
       <c r="DB56" s="111"/>
       <c r="DC56" s="111" t="s">
-        <v>832</v>
+        <v>820</v>
       </c>
       <c r="DD56" s="111"/>
       <c r="DE56" s="111"/>
       <c r="DF56" s="111"/>
       <c r="DG56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH56" s="111"/>
       <c r="DI56" s="111"/>
       <c r="DJ56" s="111"/>
       <c r="DK56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL56" s="111"/>
       <c r="DM56" s="111"/>
       <c r="DN56" s="111"/>
       <c r="DO56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP56" s="111"/>
       <c r="DQ56" s="111"/>
       <c r="DR56" s="111"/>
       <c r="DS56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT56" s="111"/>
       <c r="DU56" s="111"/>
       <c r="DV56" s="111"/>
       <c r="DW56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX56" s="111"/>
       <c r="DY56" s="111"/>
       <c r="DZ56" s="111"/>
       <c r="EA56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB56" s="111"/>
       <c r="EC56" s="111"/>
       <c r="ED56" s="111"/>
       <c r="EE56" s="111" t="s">
-        <v>854</v>
+        <v>839</v>
       </c>
       <c r="EF56" s="111"/>
       <c r="EG56" s="111"/>
       <c r="EH56" s="111"/>
       <c r="EI56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ56" s="111"/>
       <c r="EK56" s="111"/>
       <c r="EL56" s="111"/>
       <c r="EM56" s="111" t="s">
-        <v>833</v>
+        <v>821</v>
       </c>
       <c r="EN56" s="111"/>
       <c r="EO56" s="111"/>
       <c r="EP56" s="111"/>
       <c r="EQ56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER56" s="111"/>
       <c r="ES56" s="111"/>
@@ -23082,13 +23094,13 @@
       <c r="EW56" s="111"/>
       <c r="EX56" s="207"/>
       <c r="EY56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ56" s="208"/>
       <c r="FA56" s="208"/>
       <c r="FB56" s="208"/>
       <c r="FC56" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD56" s="111"/>
       <c r="FE56" s="111"/>
@@ -23187,7 +23199,7 @@
       <c r="AJ57" s="89"/>
       <c r="AK57" s="89"/>
       <c r="AL57" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM57" s="162"/>
       <c r="AN57" s="162"/>
@@ -23229,112 +23241,112 @@
       <c r="BX57" s="167"/>
       <c r="BY57" s="252"/>
       <c r="BZ57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA57" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB57" s="111"/>
       <c r="CC57" s="111"/>
       <c r="CD57" s="111"/>
       <c r="CE57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF57" s="111"/>
       <c r="CG57" s="111"/>
       <c r="CH57" s="111"/>
       <c r="CI57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ57" s="111"/>
       <c r="CK57" s="111"/>
       <c r="CL57" s="111"/>
       <c r="CM57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CN57" s="111"/>
       <c r="CO57" s="111"/>
       <c r="CP57" s="111"/>
       <c r="CQ57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR57" s="111"/>
       <c r="CS57" s="111"/>
       <c r="CT57" s="111"/>
       <c r="CU57" s="111" t="s">
-        <v>786</v>
+        <v>856</v>
       </c>
       <c r="CV57" s="111"/>
       <c r="CW57" s="111"/>
       <c r="CX57" s="111"/>
       <c r="CY57" s="111" t="s">
-        <v>834</v>
+        <v>850</v>
       </c>
       <c r="CZ57" s="111"/>
       <c r="DA57" s="111"/>
       <c r="DB57" s="111"/>
       <c r="DC57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DD57" s="111"/>
       <c r="DE57" s="111"/>
       <c r="DF57" s="111"/>
       <c r="DG57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH57" s="111"/>
       <c r="DI57" s="111"/>
       <c r="DJ57" s="111"/>
       <c r="DK57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL57" s="111"/>
       <c r="DM57" s="111"/>
       <c r="DN57" s="111"/>
       <c r="DO57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP57" s="111"/>
       <c r="DQ57" s="111"/>
       <c r="DR57" s="111"/>
       <c r="DS57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT57" s="111"/>
       <c r="DU57" s="111"/>
       <c r="DV57" s="111"/>
       <c r="DW57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX57" s="111"/>
       <c r="DY57" s="111"/>
       <c r="DZ57" s="111"/>
       <c r="EA57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB57" s="111"/>
       <c r="EC57" s="111"/>
       <c r="ED57" s="111"/>
       <c r="EE57" s="111" t="s">
-        <v>856</v>
+        <v>841</v>
       </c>
       <c r="EF57" s="111"/>
       <c r="EG57" s="111"/>
       <c r="EH57" s="111"/>
       <c r="EI57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ57" s="111"/>
       <c r="EK57" s="111"/>
       <c r="EL57" s="111"/>
       <c r="EM57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EN57" s="111"/>
       <c r="EO57" s="111"/>
       <c r="EP57" s="111"/>
       <c r="EQ57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER57" s="111"/>
       <c r="ES57" s="111"/>
@@ -23344,13 +23356,13 @@
       <c r="EW57" s="111"/>
       <c r="EX57" s="207"/>
       <c r="EY57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ57" s="208"/>
       <c r="FA57" s="208"/>
       <c r="FB57" s="208"/>
       <c r="FC57" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD57" s="111"/>
       <c r="FE57" s="111"/>
@@ -23449,7 +23461,7 @@
       <c r="AJ58" s="90"/>
       <c r="AK58" s="88"/>
       <c r="AL58" s="165" t="s">
-        <v>835</v>
+        <v>822</v>
       </c>
       <c r="AM58" s="162"/>
       <c r="AN58" s="162"/>
@@ -23491,112 +23503,112 @@
       <c r="BX58" s="167"/>
       <c r="BY58" s="252"/>
       <c r="BZ58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA58" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB58" s="111"/>
       <c r="CC58" s="111"/>
       <c r="CD58" s="111"/>
       <c r="CE58" s="111" t="s">
-        <v>836</v>
+        <v>823</v>
       </c>
       <c r="CF58" s="111"/>
       <c r="CG58" s="111"/>
       <c r="CH58" s="111"/>
       <c r="CI58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ58" s="111"/>
       <c r="CK58" s="111"/>
       <c r="CL58" s="111"/>
       <c r="CM58" s="111" t="s">
-        <v>837</v>
+        <v>824</v>
       </c>
       <c r="CN58" s="111"/>
       <c r="CO58" s="111"/>
       <c r="CP58" s="111"/>
       <c r="CQ58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR58" s="111"/>
       <c r="CS58" s="111"/>
       <c r="CT58" s="111"/>
       <c r="CU58" s="111" t="s">
-        <v>838</v>
+        <v>861</v>
       </c>
       <c r="CV58" s="111"/>
       <c r="CW58" s="111"/>
       <c r="CX58" s="111"/>
       <c r="CY58" s="111" t="s">
-        <v>839</v>
+        <v>851</v>
       </c>
       <c r="CZ58" s="111"/>
       <c r="DA58" s="111"/>
       <c r="DB58" s="111"/>
       <c r="DC58" s="111" t="s">
-        <v>840</v>
+        <v>825</v>
       </c>
       <c r="DD58" s="111"/>
       <c r="DE58" s="111"/>
       <c r="DF58" s="111"/>
       <c r="DG58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH58" s="111"/>
       <c r="DI58" s="111"/>
       <c r="DJ58" s="111"/>
       <c r="DK58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL58" s="111"/>
       <c r="DM58" s="111"/>
       <c r="DN58" s="111"/>
       <c r="DO58" s="111" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="DP58" s="111"/>
       <c r="DQ58" s="111"/>
       <c r="DR58" s="111"/>
       <c r="DS58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT58" s="111"/>
       <c r="DU58" s="111"/>
       <c r="DV58" s="111"/>
       <c r="DW58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX58" s="111"/>
       <c r="DY58" s="111"/>
       <c r="DZ58" s="111"/>
       <c r="EA58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB58" s="111"/>
       <c r="EC58" s="111"/>
       <c r="ED58" s="111"/>
       <c r="EE58" s="111" t="s">
-        <v>855</v>
+        <v>845</v>
       </c>
       <c r="EF58" s="111"/>
       <c r="EG58" s="111"/>
       <c r="EH58" s="111"/>
       <c r="EI58" s="111" t="s">
-        <v>794</v>
+        <v>787</v>
       </c>
       <c r="EJ58" s="111"/>
       <c r="EK58" s="111"/>
       <c r="EL58" s="111"/>
       <c r="EM58" s="111" t="s">
-        <v>795</v>
+        <v>788</v>
       </c>
       <c r="EN58" s="111"/>
       <c r="EO58" s="111"/>
       <c r="EP58" s="111"/>
       <c r="EQ58" s="111" t="s">
-        <v>796</v>
+        <v>789</v>
       </c>
       <c r="ER58" s="111"/>
       <c r="ES58" s="111"/>
@@ -23606,13 +23618,13 @@
       <c r="EW58" s="111"/>
       <c r="EX58" s="207"/>
       <c r="EY58" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ58" s="208"/>
       <c r="FA58" s="208"/>
       <c r="FB58" s="208"/>
       <c r="FC58" s="208" t="s">
-        <v>797</v>
+        <v>790</v>
       </c>
       <c r="FD58" s="111"/>
       <c r="FE58" s="111"/>
@@ -23711,7 +23723,7 @@
       <c r="AJ59" s="90"/>
       <c r="AK59" s="90"/>
       <c r="AL59" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM59" s="162"/>
       <c r="AN59" s="162"/>
@@ -23753,112 +23765,112 @@
       <c r="BX59" s="167"/>
       <c r="BY59" s="252"/>
       <c r="BZ59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA59" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB59" s="111"/>
       <c r="CC59" s="111"/>
       <c r="CD59" s="111"/>
       <c r="CE59" s="111" t="s">
-        <v>841</v>
+        <v>826</v>
       </c>
       <c r="CF59" s="111"/>
       <c r="CG59" s="111"/>
       <c r="CH59" s="111"/>
       <c r="CI59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ59" s="111"/>
       <c r="CK59" s="111"/>
       <c r="CL59" s="111"/>
       <c r="CM59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CN59" s="111"/>
       <c r="CO59" s="111"/>
       <c r="CP59" s="111"/>
       <c r="CQ59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CR59" s="111"/>
       <c r="CS59" s="111"/>
       <c r="CT59" s="111"/>
       <c r="CU59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CV59" s="111"/>
       <c r="CW59" s="111"/>
       <c r="CX59" s="111"/>
       <c r="CY59" s="111" t="s">
-        <v>831</v>
+        <v>852</v>
       </c>
       <c r="CZ59" s="111"/>
       <c r="DA59" s="111"/>
       <c r="DB59" s="111"/>
       <c r="DC59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DD59" s="111"/>
       <c r="DE59" s="111"/>
       <c r="DF59" s="111"/>
       <c r="DG59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH59" s="111"/>
       <c r="DI59" s="111"/>
       <c r="DJ59" s="111"/>
       <c r="DK59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL59" s="111"/>
       <c r="DM59" s="111"/>
       <c r="DN59" s="111"/>
       <c r="DO59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP59" s="111"/>
       <c r="DQ59" s="111"/>
       <c r="DR59" s="111"/>
       <c r="DS59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT59" s="111"/>
       <c r="DU59" s="111"/>
       <c r="DV59" s="111"/>
       <c r="DW59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX59" s="111"/>
       <c r="DY59" s="111"/>
       <c r="DZ59" s="111"/>
       <c r="EA59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB59" s="111"/>
       <c r="EC59" s="111"/>
       <c r="ED59" s="111"/>
       <c r="EE59" s="111" t="s">
-        <v>851</v>
+        <v>840</v>
       </c>
       <c r="EF59" s="111"/>
       <c r="EG59" s="111"/>
       <c r="EH59" s="111"/>
       <c r="EI59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ59" s="111"/>
       <c r="EK59" s="111"/>
       <c r="EL59" s="111"/>
       <c r="EM59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EN59" s="111"/>
       <c r="EO59" s="111"/>
       <c r="EP59" s="111"/>
       <c r="EQ59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER59" s="111"/>
       <c r="ES59" s="111"/>
@@ -23868,13 +23880,13 @@
       <c r="EW59" s="111"/>
       <c r="EX59" s="207"/>
       <c r="EY59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ59" s="208"/>
       <c r="FA59" s="208"/>
       <c r="FB59" s="208"/>
       <c r="FC59" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="FD59" s="111"/>
       <c r="FE59" s="111"/>
@@ -23973,7 +23985,7 @@
       <c r="AJ60" s="90"/>
       <c r="AK60" s="90"/>
       <c r="AL60" s="165" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AM60" s="162"/>
       <c r="AN60" s="162"/>
@@ -24015,112 +24027,112 @@
       <c r="BX60" s="167"/>
       <c r="BY60" s="252"/>
       <c r="BZ60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CA60" s="111" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="CB60" s="111"/>
       <c r="CC60" s="111"/>
       <c r="CD60" s="111"/>
       <c r="CE60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CF60" s="111"/>
       <c r="CG60" s="111"/>
       <c r="CH60" s="111"/>
       <c r="CI60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CJ60" s="111"/>
       <c r="CK60" s="111"/>
       <c r="CL60" s="111"/>
       <c r="CM60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CN60" s="111"/>
       <c r="CO60" s="111"/>
       <c r="CP60" s="111"/>
       <c r="CQ60" s="111" t="s">
-        <v>842</v>
+        <v>827</v>
       </c>
       <c r="CR60" s="111"/>
       <c r="CS60" s="111"/>
       <c r="CT60" s="111"/>
       <c r="CU60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CV60" s="111"/>
       <c r="CW60" s="111"/>
       <c r="CX60" s="111"/>
       <c r="CY60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="CZ60" s="111"/>
       <c r="DA60" s="111"/>
       <c r="DB60" s="111"/>
       <c r="DC60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DD60" s="111"/>
       <c r="DE60" s="111"/>
       <c r="DF60" s="111"/>
       <c r="DG60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DH60" s="111"/>
       <c r="DI60" s="111"/>
       <c r="DJ60" s="111"/>
       <c r="DK60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DL60" s="111"/>
       <c r="DM60" s="111"/>
       <c r="DN60" s="111"/>
       <c r="DO60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DP60" s="111"/>
       <c r="DQ60" s="111"/>
       <c r="DR60" s="111"/>
       <c r="DS60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DT60" s="111"/>
       <c r="DU60" s="111"/>
       <c r="DV60" s="111"/>
       <c r="DW60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="DX60" s="111"/>
       <c r="DY60" s="111"/>
       <c r="DZ60" s="111"/>
       <c r="EA60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EB60" s="111"/>
       <c r="EC60" s="111"/>
       <c r="ED60" s="111"/>
       <c r="EE60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EF60" s="111"/>
       <c r="EG60" s="111"/>
       <c r="EH60" s="111"/>
       <c r="EI60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EJ60" s="111"/>
       <c r="EK60" s="111"/>
       <c r="EL60" s="111"/>
       <c r="EM60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EN60" s="111"/>
       <c r="EO60" s="111"/>
       <c r="EP60" s="111"/>
       <c r="EQ60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="ER60" s="111"/>
       <c r="ES60" s="111"/>
@@ -24130,13 +24142,13 @@
       <c r="EW60" s="111"/>
       <c r="EX60" s="207"/>
       <c r="EY60" s="111" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="EZ60" s="208"/>
       <c r="FA60" s="208"/>
       <c r="FB60" s="208"/>
       <c r="FC60" s="208" t="s">
-        <v>843</v>
+        <v>828</v>
       </c>
       <c r="FD60" s="111"/>
       <c r="FE60" s="111"/>
@@ -33626,7 +33638,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="214" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="D3" s="189" t="s">
         <v>603</v>
@@ -33635,31 +33647,31 @@
         <v>663</v>
       </c>
       <c r="F3" s="214" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="G3" s="214" t="s">
+        <v>739</v>
+      </c>
+      <c r="H3" s="214" t="s">
+        <v>740</v>
+      </c>
+      <c r="I3" s="214" t="s">
+        <v>741</v>
+      </c>
+      <c r="J3" s="214" t="s">
+        <v>742</v>
+      </c>
+      <c r="K3" s="214" t="s">
+        <v>743</v>
+      </c>
+      <c r="L3" s="214" t="s">
         <v>744</v>
       </c>
-      <c r="H3" s="214" t="s">
+      <c r="M3" s="214" t="s">
         <v>745</v>
       </c>
-      <c r="I3" s="214" t="s">
+      <c r="N3" s="214" t="s">
         <v>746</v>
-      </c>
-      <c r="J3" s="214" t="s">
-        <v>747</v>
-      </c>
-      <c r="K3" s="214" t="s">
-        <v>748</v>
-      </c>
-      <c r="L3" s="214" t="s">
-        <v>749</v>
-      </c>
-      <c r="M3" s="214" t="s">
-        <v>750</v>
-      </c>
-      <c r="N3" s="214" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
@@ -33671,62 +33683,62 @@
       <c r="D4" s="216"/>
       <c r="E4" s="216"/>
       <c r="F4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="G4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="H4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="I4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="J4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="K4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="L4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="M4" s="216" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="N4" s="216"/>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="215" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="B5" s="216"/>
       <c r="C5" s="216"/>
       <c r="D5" s="216"/>
       <c r="E5" s="216"/>
       <c r="F5" s="248" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="G5" s="248" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="H5" s="248" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="I5" s="248" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="J5" s="248" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="K5" s="248" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="L5" s="248" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="M5" s="248" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="N5" s="216"/>
     </row>
@@ -34075,10 +34087,10 @@
         <v>53</v>
       </c>
       <c r="B14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D14" s="72" t="s">
         <v>606</v>
@@ -34087,28 +34099,28 @@
         <v>666</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="J14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="L14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="M14" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N14" s="72" t="s">
         <v>226</v>
@@ -34201,38 +34213,38 @@
         <v>53</v>
       </c>
       <c r="B17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D17" s="72" t="s">
         <v>607</v>
       </c>
       <c r="E17" s="72"/>
       <c r="F17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="K17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="L17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="M17" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N17" s="72" t="s">
         <v>227</v>
@@ -34443,7 +34455,7 @@
       <c r="B23" s="72"/>
       <c r="C23" s="72"/>
       <c r="D23" s="72" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E23" s="72"/>
       <c r="F23" s="72" t="s">
@@ -34561,7 +34573,7 @@
       <c r="B26" s="72"/>
       <c r="C26" s="72"/>
       <c r="D26" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E26" s="72"/>
       <c r="F26" s="72" t="s">
@@ -35319,28 +35331,28 @@
       <c r="D46" s="72"/>
       <c r="E46" s="72"/>
       <c r="F46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="G46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="H46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="I46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="J46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="K46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="L46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="M46" s="72" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="N46" s="72"/>
     </row>
@@ -35353,28 +35365,28 @@
       <c r="D47" s="72"/>
       <c r="E47" s="72"/>
       <c r="F47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="G47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="H47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="I47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="J47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="K47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="L47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="M47" s="72" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="N47" s="72"/>
     </row>
@@ -35429,28 +35441,28 @@
       <c r="D49" s="72"/>
       <c r="E49" s="72"/>
       <c r="F49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="G49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="H49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="I49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="J49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="K49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="L49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="M49" s="72" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="N49" s="72"/>
     </row>
@@ -35463,28 +35475,28 @@
       <c r="D50" s="72"/>
       <c r="E50" s="72"/>
       <c r="F50" s="72" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="G50" s="72" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="H50" s="72" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="I50" s="72" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="J50" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="K50" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="L50" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="M50" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="N50" s="72"/>
     </row>
@@ -35539,28 +35551,28 @@
       <c r="D52" s="72"/>
       <c r="E52" s="72"/>
       <c r="F52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="G52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="H52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="I52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="J52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="K52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="L52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="M52" s="72" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="N52" s="72"/>
     </row>
@@ -35573,28 +35585,28 @@
       <c r="D53" s="72"/>
       <c r="E53" s="72"/>
       <c r="F53" s="72" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="G53" s="72" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="H53" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="I53" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="J53" s="72" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="K53" s="72" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="L53" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="M53" s="72" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="N53" s="72"/>
     </row>
@@ -35649,28 +35661,28 @@
       <c r="D55" s="72"/>
       <c r="E55" s="72"/>
       <c r="F55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="G55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="H55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="I55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="J55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="K55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="L55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="M55" s="72" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="N55" s="72"/>
     </row>
@@ -35683,28 +35695,28 @@
       <c r="D56" s="72"/>
       <c r="E56" s="72"/>
       <c r="F56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="G56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="H56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="I56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="J56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="K56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="L56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="M56" s="72" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="N56" s="72"/>
     </row>
@@ -35759,28 +35771,28 @@
       <c r="D58" s="72"/>
       <c r="E58" s="72"/>
       <c r="F58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="G58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="H58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="I58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="J58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="K58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="L58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="M58" s="72" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="N58" s="72"/>
     </row>
@@ -35793,28 +35805,28 @@
       <c r="D59" s="72"/>
       <c r="E59" s="72"/>
       <c r="F59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="G59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="H59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="I59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="J59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="K59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="L59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="M59" s="72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="N59" s="72"/>
     </row>

</xml_diff>